<commit_message>
Added missing pictures, new resultsANSYS.xlsx
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18240" windowHeight="8508"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18240" windowHeight="8508" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HSR Cluster" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
   <si>
     <t>pipe02</t>
   </si>
@@ -97,12 +97,21 @@
   <si>
     <t>Case</t>
   </si>
+  <si>
+    <t>Size per node</t>
+  </si>
+  <si>
+    <t>std dev</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +124,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -154,12 +176,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -167,24 +195,130 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -281,8 +415,384 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HSR Cluster'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pipe01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$C$21:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$F$5:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>894.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>486.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>274.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>219.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HSR Cluster'!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pipe02</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$C$21:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$M$5:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1864.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>743.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>524.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>376.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>336.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>264.22500000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HSR Cluster'!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pipe06</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$C$21:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$F$13:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2365.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1223.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>835.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>657.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>597.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HSR Cluster'!$I$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pipe04</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$C$21:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$M$13:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4072.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1404.86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1096.6099999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>915.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>'HSR Cluster'!$B$20</c:f>
@@ -320,368 +830,54 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'HSR Cluster'!$C$21:$C$25</c:f>
+              <c:f>'HSR Cluster'!$C$21:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'HSR Cluster'!$F$21:$F$25</c:f>
+              <c:f>'HSR Cluster'!$F$21:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5985.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4403.74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2937.19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2239.5700000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1778.97</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2239.5700000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2937.19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2008.19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5985.82</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'HSR Cluster'!$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pipe06</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'HSR Cluster'!$F$13:$F$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>597.59</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>657.32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>835.63</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1223.82</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2365.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'HSR Cluster'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pipe01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'HSR Cluster'!$F$5:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>171.94</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>188.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>219.74</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>274.64999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>486.45</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'HSR Cluster'!$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pipe02</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'HSR Cluster'!$M$5:$M$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>264.22500000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>336.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>376.78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>524.37</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>743.86</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'HSR Cluster'!$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pipe02</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'HSR Cluster'!$M$5:$M$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>264.22500000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>336.3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>376.78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>524.37</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>743.86</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'HSR Cluster'!$I$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pipe04</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'HSR Cluster'!$M$13:$M$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>915.85</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1096.6099999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1404.86</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2008.19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4072.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,6 +1116,426 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
+              <a:t>Weak</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> scaling</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-CH"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$B$31:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$C$31:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>894.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>743.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1223.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1096.6099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$B$31:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$D$31:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1864.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2365.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2239.5700000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="235151488"/>
+        <c:axId val="235152664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="235151488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235152664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="235152664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235151488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
               <a:t>Weak scaling</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
@@ -1323,7 +1939,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1793,7 +2409,6 @@
       <c:valAx>
         <c:axId val="159887216"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1924,7 +2539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2066,6 +2681,59 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1616.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>HSR</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'HSR Cluster'!$M$21:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5351.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4472.3100000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4587.58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3487.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2397,6 +3065,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4409,20 +5117,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4436,6 +5647,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4884,20 +6125,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:X25"/>
+  <dimension ref="B3:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -4911,7 +6158,7 @@
       <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
@@ -4926,335 +6173,261 @@
       <c r="M4" t="s">
         <v>4</v>
       </c>
-      <c r="Q4">
+      <c r="X4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <f>$C$41/C5</f>
+        <v>32517</v>
+      </c>
+      <c r="C5">
         <v>6</v>
       </c>
-      <c r="R4">
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>54.62</v>
+      </c>
+      <c r="F5" s="13">
+        <f>D5*60+E5</f>
+        <v>894.62</v>
+      </c>
+      <c r="I5" s="1">
+        <f>$C$42/J5</f>
+        <v>72153.166666666672</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>31</v>
+      </c>
+      <c r="L5">
+        <v>4.79</v>
+      </c>
+      <c r="M5" s="31">
+        <f>K5*60+L5</f>
+        <v>1864.79</v>
+      </c>
+      <c r="X5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>195102</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:B10" si="0">$C$41/C6</f>
+        <v>16258.5</v>
+      </c>
+      <c r="C6">
         <v>12</v>
       </c>
-      <c r="S4">
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>6.45</v>
+      </c>
+      <c r="F6">
+        <f>D6*60+E6</f>
+        <v>486.45</v>
+      </c>
+      <c r="I6" s="1">
+        <f>$C$42/J6</f>
+        <v>36076.583333333336</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>23.86</v>
+      </c>
+      <c r="M6" s="30">
+        <f>K6*60+L6</f>
+        <v>743.86</v>
+      </c>
+      <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>432919</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>8129.25</v>
+      </c>
+      <c r="C7">
         <v>24</v>
       </c>
-      <c r="T4">
-        <v>48</v>
-      </c>
-      <c r="U4">
-        <v>60</v>
-      </c>
-      <c r="W4" t="s">
-        <v>24</v>
-      </c>
-      <c r="X4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>60</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>51.94</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F6" si="0">D5*60+E5</f>
-        <v>171.94</v>
-      </c>
-      <c r="J5">
-        <v>60</v>
-      </c>
-      <c r="K5">
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="L5">
-        <v>24.225000000000001</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5:M6" si="1">K5*60+L5</f>
-        <v>264.22500000000002</v>
-      </c>
-      <c r="O5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P5" s="3">
-        <f>X5</f>
-        <v>195102</v>
-      </c>
-      <c r="Q5" s="1">
-        <f>$P$5/Q$4</f>
-        <v>32517</v>
-      </c>
-      <c r="R5" s="1">
-        <f>$P$5/R$4</f>
-        <v>16258.5</v>
-      </c>
-      <c r="S5" s="1">
-        <f t="shared" ref="S5:U5" si="2">$P$5/S$4</f>
-        <v>8129.25</v>
-      </c>
-      <c r="T5" s="1">
-        <f t="shared" si="2"/>
-        <v>4064.625</v>
-      </c>
-      <c r="U5" s="1">
-        <f t="shared" si="2"/>
-        <v>3251.7</v>
-      </c>
-      <c r="W5" t="s">
-        <v>5</v>
-      </c>
-      <c r="X5" s="1">
-        <v>195102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>48</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>188.05</v>
-      </c>
-      <c r="J6">
-        <v>48</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
-        <v>336.3</v>
-      </c>
-      <c r="O6" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <f>X6</f>
-        <v>432919</v>
-      </c>
-      <c r="Q6" s="1">
-        <f>$P$6/Q$4</f>
-        <v>72153.166666666672</v>
-      </c>
-      <c r="R6" s="1">
-        <f t="shared" ref="R6:U6" si="3">$P$6/R$4</f>
-        <v>36076.583333333336</v>
-      </c>
-      <c r="S6" s="1">
-        <f t="shared" si="3"/>
-        <v>18038.291666666668</v>
-      </c>
-      <c r="T6" s="1">
-        <f t="shared" si="3"/>
-        <v>9019.1458333333339</v>
-      </c>
-      <c r="U6" s="1">
-        <f t="shared" si="3"/>
-        <v>7215.3166666666666</v>
-      </c>
-      <c r="W6" t="s">
-        <v>0</v>
-      </c>
-      <c r="X6" s="1">
-        <v>432919</v>
-      </c>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>36</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
       <c r="E7">
-        <v>39.74</v>
+        <v>34.65</v>
       </c>
       <c r="F7">
         <f>D7*60+E7</f>
-        <v>219.74</v>
+        <v>274.64999999999998</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:I10" si="1">$C$42/J7</f>
+        <v>18038.291666666668</v>
       </c>
       <c r="J7">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L7">
-        <v>16.78</v>
+        <v>44.37</v>
       </c>
       <c r="M7">
         <f>K7*60+L7</f>
-        <v>376.78</v>
-      </c>
-      <c r="O7" t="s">
+        <v>524.37</v>
+      </c>
+      <c r="X7" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="3">
-        <f>X7</f>
+      <c r="Y7" s="1">
         <v>1017573</v>
       </c>
-      <c r="Q7" s="1">
-        <f>$P$7/Q$4</f>
-        <v>169595.5</v>
-      </c>
-      <c r="R7" s="1">
-        <f t="shared" ref="R7:U7" si="4">$P$7/R$4</f>
-        <v>84797.75</v>
-      </c>
-      <c r="S7" s="1">
-        <f t="shared" si="4"/>
-        <v>42398.875</v>
-      </c>
-      <c r="T7" s="1">
-        <f t="shared" si="4"/>
-        <v>21199.4375</v>
-      </c>
-      <c r="U7" s="1">
-        <f t="shared" si="4"/>
-        <v>16959.55</v>
-      </c>
-      <c r="W7" t="s">
-        <v>21</v>
-      </c>
-      <c r="X7" s="1">
-        <v>1017573</v>
-      </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>5419.5</v>
+      </c>
       <c r="C8">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>34.65</v>
+        <v>39.74</v>
       </c>
       <c r="F8">
         <f>D8*60+E8</f>
-        <v>274.64999999999998</v>
+        <v>219.74</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>12025.527777777777</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="K8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L8">
-        <v>44.37</v>
+        <v>16.78</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M9" si="5">K8*60+L8</f>
-        <v>524.37</v>
-      </c>
-      <c r="O8" t="s">
+        <f>K8*60+L8</f>
+        <v>376.78</v>
+      </c>
+      <c r="X8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="3">
-        <f>X8</f>
+      <c r="Y8" s="1">
         <v>2037710</v>
       </c>
-      <c r="Q8" s="1">
-        <f>$P$8/Q$4</f>
-        <v>339618.33333333331</v>
-      </c>
-      <c r="R8" s="1">
-        <f t="shared" ref="R8:U8" si="6">$P$8/R$4</f>
-        <v>169809.16666666666</v>
-      </c>
-      <c r="S8" s="1">
-        <f t="shared" si="6"/>
-        <v>84904.583333333328</v>
-      </c>
-      <c r="T8" s="1">
-        <f t="shared" si="6"/>
-        <v>42452.291666666664</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" si="6"/>
-        <v>33961.833333333336</v>
-      </c>
-      <c r="W8" t="s">
-        <v>7</v>
-      </c>
-      <c r="X8" s="1">
-        <v>2037710</v>
-      </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>4064.625</v>
+      </c>
       <c r="C9">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>6.45</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F9">
         <f>D9*60+E9</f>
-        <v>486.45</v>
+        <v>188.05</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>9019.1458333333339</v>
       </c>
       <c r="J9">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="K9">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L9">
-        <v>23.86</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
-        <v>743.86</v>
-      </c>
-      <c r="O9" t="s">
+        <f>K9*60+L9</f>
+        <v>336.3</v>
+      </c>
+      <c r="X9" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="3">
-        <f>X9</f>
+      <c r="Y9" s="1">
         <v>4010210</v>
       </c>
-      <c r="Q9" s="1">
-        <f>$P$9/Q$4</f>
-        <v>668368.33333333337</v>
-      </c>
-      <c r="R9" s="1">
-        <f t="shared" ref="R9:U9" si="7">$P$9/R$4</f>
-        <v>334184.16666666669</v>
-      </c>
-      <c r="S9" s="1">
-        <f t="shared" si="7"/>
-        <v>167092.08333333334</v>
-      </c>
-      <c r="T9" s="1">
-        <f t="shared" si="7"/>
-        <v>83546.041666666672</v>
-      </c>
-      <c r="U9" s="1">
-        <f t="shared" si="7"/>
-        <v>66836.833333333328</v>
-      </c>
-      <c r="W9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X9" s="1">
-        <v>4010210</v>
-      </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>3251.7</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>51.94</v>
+      </c>
+      <c r="F10">
+        <f>D10*60+E10</f>
+        <v>171.94</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>7215.3166666666666</v>
+      </c>
+      <c r="J10">
+        <v>60</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>24.225000000000001</v>
+      </c>
+      <c r="M10">
+        <f>K10*60+L10</f>
+        <v>264.22500000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
@@ -5269,7 +6442,7 @@
       <c r="F12" t="s">
         <v>4</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="12" t="s">
         <v>7</v>
       </c>
       <c r="J12" t="s">
@@ -5285,148 +6458,210 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>60</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>57.59</v>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <f>$C$43/C13</f>
+        <v>169595.5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>6</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F17" si="8">D13*60+E13</f>
-        <v>597.59</v>
-      </c>
-      <c r="J13">
-        <v>60</v>
-      </c>
-      <c r="K13">
-        <v>15</v>
-      </c>
-      <c r="L13">
-        <v>15.85</v>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f>$C$44/J13</f>
+        <v>339618.33333333331</v>
+      </c>
+      <c r="J13" s="4">
+        <v>6</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13:M17" si="9">K13*60+L13</f>
-        <v>915.85</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <f>$C$43/C14</f>
+        <v>84797.75</v>
+      </c>
       <c r="C14">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E14">
-        <v>57.32</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="8"/>
-        <v>657.32</v>
+        <v>25.75</v>
+      </c>
+      <c r="F14" s="31">
+        <f>D14*60+E14</f>
+        <v>2365.75</v>
+      </c>
+      <c r="I14" s="1">
+        <f>$C$44/J14</f>
+        <v>169809.16666666666</v>
       </c>
       <c r="J14">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="K14">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="L14">
-        <v>16.61</v>
+        <v>52.02</v>
       </c>
       <c r="M14">
-        <f t="shared" si="9"/>
-        <v>1096.6099999999999</v>
+        <f>K14*60+L14</f>
+        <v>4072.02</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <f t="shared" ref="B15:B18" si="2">$C$43/C15</f>
+        <v>42398.875</v>
+      </c>
       <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>23.82</v>
+      </c>
+      <c r="F15" s="13">
+        <f>D15*60+E15</f>
+        <v>1223.82</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15:I18" si="3">$C$44/J15</f>
+        <v>84904.583333333328</v>
+      </c>
+      <c r="J15">
+        <v>24</v>
+      </c>
+      <c r="K15">
+        <v>33</v>
+      </c>
+      <c r="L15">
+        <v>28.19</v>
+      </c>
+      <c r="M15" s="31">
+        <f>K15*60+L15</f>
+        <v>2008.19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <f t="shared" si="2"/>
+        <v>28265.916666666668</v>
+      </c>
+      <c r="C16">
         <v>36</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>13</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>55.63</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="8"/>
+      <c r="F16">
+        <f>D16*60+E16</f>
         <v>835.63</v>
       </c>
-      <c r="J15">
+      <c r="I16" s="1">
+        <f t="shared" si="3"/>
+        <v>56603.055555555555</v>
+      </c>
+      <c r="J16">
         <v>36</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>23</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>24.86</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="9"/>
+      <c r="M16">
+        <f>K16*60+L16</f>
         <v>1404.86</v>
-      </c>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>24</v>
-      </c>
-      <c r="D16">
-        <v>20</v>
-      </c>
-      <c r="E16">
-        <v>23.82</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="8"/>
-        <v>1223.82</v>
-      </c>
-      <c r="J16">
-        <v>24</v>
-      </c>
-      <c r="K16">
-        <v>33</v>
-      </c>
-      <c r="L16">
-        <v>28.19</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="9"/>
-        <v>2008.19</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <f t="shared" si="2"/>
+        <v>21199.4375</v>
+      </c>
       <c r="C17">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D17">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>25.75</v>
+        <v>57.32</v>
       </c>
       <c r="F17">
-        <f t="shared" si="8"/>
-        <v>2365.75</v>
+        <f>D17*60+E17</f>
+        <v>657.32</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="3"/>
+        <v>42452.291666666664</v>
       </c>
       <c r="J17">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="K17">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="L17">
-        <v>52.02</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="9"/>
-        <v>4072.02</v>
+        <v>16.61</v>
+      </c>
+      <c r="M17" s="13">
+        <f>K17*60+L17</f>
+        <v>1096.6099999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <f t="shared" si="2"/>
+        <v>16959.55</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>57.59</v>
+      </c>
+      <c r="F18">
+        <f>D18*60+E18</f>
+        <v>597.59</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="3"/>
+        <v>33961.833333333336</v>
+      </c>
+      <c r="J18">
+        <v>60</v>
+      </c>
+      <c r="K18">
+        <v>15</v>
+      </c>
+      <c r="L18">
+        <v>15.85</v>
+      </c>
+      <c r="M18">
+        <f>K18*60+L18</f>
+        <v>915.85</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
@@ -5458,145 +6693,455 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>60</v>
-      </c>
-      <c r="D21">
-        <v>29</v>
-      </c>
-      <c r="E21">
-        <v>38.97</v>
+      <c r="B21" s="1">
+        <f>$C$45/C21</f>
+        <v>668368.33333333337</v>
+      </c>
+      <c r="C21" s="4">
+        <v>6</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F25" si="10">D21*60+E21</f>
-        <v>1778.97</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="K21">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="L21">
-        <v>34.700000000000003</v>
+        <v>11.41</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M25" si="11">K21*60+L21</f>
-        <v>3154.7</v>
+        <f>K21*60+L21</f>
+        <v>5351.41</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <f>$C$45/C22</f>
+        <v>334184.16666666669</v>
+      </c>
       <c r="C22">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D22">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="E22">
-        <v>19.57</v>
+        <v>45.82</v>
       </c>
       <c r="F22">
-        <f t="shared" si="10"/>
-        <v>2239.5700000000002</v>
+        <f>D22*60+E22</f>
+        <v>5985.82</v>
       </c>
       <c r="J22">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="K22">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="L22">
-        <v>7.35</v>
+        <v>32.31</v>
       </c>
       <c r="M22">
-        <f t="shared" si="11"/>
-        <v>3487.35</v>
+        <f>K22*60+L22</f>
+        <v>4472.3100000000004</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <f t="shared" ref="B23:B26" si="4">$C$45/C23</f>
+        <v>167092.08333333334</v>
+      </c>
       <c r="C23">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>73</v>
+      </c>
+      <c r="E23">
+        <v>23.74</v>
+      </c>
+      <c r="F23">
+        <f>D23*60+E23</f>
+        <v>4403.74</v>
+      </c>
+      <c r="J23">
         <v>36</v>
       </c>
-      <c r="D23">
-        <v>48</v>
-      </c>
-      <c r="E23">
-        <v>57.19</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="10"/>
-        <v>2937.19</v>
-      </c>
-      <c r="J23" s="4">
-        <v>36</v>
-      </c>
       <c r="K23">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="L23">
+        <v>27.58</v>
       </c>
       <c r="M23">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>K23*60+L23</f>
+        <v>4587.58</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <f t="shared" si="4"/>
+        <v>111394.72222222222</v>
+      </c>
       <c r="C24">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D24">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E24">
-        <v>28.19</v>
+        <v>57.19</v>
       </c>
       <c r="F24">
-        <f t="shared" si="10"/>
-        <v>2008.19</v>
+        <f>D24*60+E24</f>
+        <v>2937.19</v>
       </c>
       <c r="J24">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="K24">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="L24">
-        <v>32.31</v>
+        <v>7.35</v>
       </c>
       <c r="M24">
-        <f t="shared" si="11"/>
-        <v>4472.3100000000004</v>
+        <f>K24*60+L24</f>
+        <v>3487.35</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <f t="shared" si="4"/>
+        <v>83546.041666666672</v>
+      </c>
       <c r="C25">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <v>19.57</v>
+      </c>
+      <c r="F25" s="31">
+        <f>D25*60+E25</f>
+        <v>2239.5700000000002</v>
+      </c>
+      <c r="J25">
+        <v>60</v>
+      </c>
+      <c r="K25">
+        <v>52</v>
+      </c>
+      <c r="L25">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="M25">
+        <f>K25*60+L25</f>
+        <v>3154.7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <f t="shared" si="4"/>
+        <v>66836.833333333328</v>
+      </c>
+      <c r="C26">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>38.97</v>
+      </c>
+      <c r="F26">
+        <f>D26*60+E26</f>
+        <v>1778.97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="D25">
-        <v>99</v>
-      </c>
-      <c r="E25">
-        <v>45.82</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="10"/>
-        <v>5985.82</v>
-      </c>
-      <c r="J25">
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <f>C36</f>
+        <v>38361.1875</v>
+      </c>
+      <c r="D30" s="1">
+        <f>D36</f>
+        <v>81350.385416666672</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <f>F5</f>
+        <v>894.62</v>
+      </c>
+      <c r="D31">
+        <f>M5</f>
+        <v>1864.79</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32">
         <v>12</v>
       </c>
-      <c r="K25">
-        <v>89</v>
-      </c>
-      <c r="L25">
-        <v>11.41</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="11"/>
-        <v>5351.41</v>
+      <c r="C32">
+        <f>M6</f>
+        <v>743.86</v>
+      </c>
+      <c r="D32">
+        <f>F14</f>
+        <v>2365.75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <f>F15</f>
+        <v>1223.82</v>
+      </c>
+      <c r="D33">
+        <f>M15</f>
+        <v>2008.19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>48</v>
+      </c>
+      <c r="C34">
+        <f>M17</f>
+        <v>1096.6099999999999</v>
+      </c>
+      <c r="D34">
+        <f>F25</f>
+        <v>2239.5700000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1">
+        <f>AVERAGE(D41,E42,F43,G44)</f>
+        <v>38361.1875</v>
+      </c>
+      <c r="D36" s="1">
+        <f>AVERAGE(D42,E43,F44,G45)</f>
+        <v>81350.385416666672</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="1">
+        <f>STDEV(G44,F43,E42,D41)</f>
+        <v>4913.0437742700242</v>
+      </c>
+      <c r="D37">
+        <f>STDEV(D42,E43,F44,G45)</f>
+        <v>6162.4233465083689</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="2">
+        <f>C37/C36</f>
+        <v>0.12807329737302903</v>
+      </c>
+      <c r="D38" s="2">
+        <f>D37/D36</f>
+        <v>7.5751618322951936E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17">
+        <v>6</v>
+      </c>
+      <c r="E40" s="17">
+        <v>12</v>
+      </c>
+      <c r="F40" s="17">
+        <v>24</v>
+      </c>
+      <c r="G40" s="18">
+        <v>48</v>
+      </c>
+      <c r="H40" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="20">
+        <f>Y5</f>
+        <v>195102</v>
+      </c>
+      <c r="D41" s="21">
+        <f>$C$41/D$40</f>
+        <v>32517</v>
+      </c>
+      <c r="E41" s="22">
+        <f>$C$41/E$40</f>
+        <v>16258.5</v>
+      </c>
+      <c r="F41" s="22">
+        <f>$C$41/F$40</f>
+        <v>8129.25</v>
+      </c>
+      <c r="G41" s="23">
+        <f>$C$41/G$40</f>
+        <v>4064.625</v>
+      </c>
+      <c r="H41" s="10">
+        <f>$C$41/H$40</f>
+        <v>3251.7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="20">
+        <f>Y6</f>
+        <v>432919</v>
+      </c>
+      <c r="D42" s="24">
+        <f>$C$42/D$40</f>
+        <v>72153.166666666672</v>
+      </c>
+      <c r="E42" s="21">
+        <f>$C$42/E$40</f>
+        <v>36076.583333333336</v>
+      </c>
+      <c r="F42" s="22">
+        <f>$C$42/F$40</f>
+        <v>18038.291666666668</v>
+      </c>
+      <c r="G42" s="23">
+        <f>$C$42/G$40</f>
+        <v>9019.1458333333339</v>
+      </c>
+      <c r="H42" s="10">
+        <f>$C$42/H$40</f>
+        <v>7215.3166666666666</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="20">
+        <f>Y7</f>
+        <v>1017573</v>
+      </c>
+      <c r="D43" s="22">
+        <f>$C$43/D$40</f>
+        <v>169595.5</v>
+      </c>
+      <c r="E43" s="24">
+        <f>$C$43/E$40</f>
+        <v>84797.75</v>
+      </c>
+      <c r="F43" s="21">
+        <f>$C$43/F$40</f>
+        <v>42398.875</v>
+      </c>
+      <c r="G43" s="23">
+        <f>$C$43/G$40</f>
+        <v>21199.4375</v>
+      </c>
+      <c r="H43" s="10">
+        <f>$C$43/H$40</f>
+        <v>16959.55</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="20">
+        <f>Y8</f>
+        <v>2037710</v>
+      </c>
+      <c r="D44" s="22">
+        <f>$C$44/D$40</f>
+        <v>339618.33333333331</v>
+      </c>
+      <c r="E44" s="22">
+        <f>$C$44/E$40</f>
+        <v>169809.16666666666</v>
+      </c>
+      <c r="F44" s="24">
+        <f>$C$44/F$40</f>
+        <v>84904.583333333328</v>
+      </c>
+      <c r="G44" s="25">
+        <f>$C$44/G$40</f>
+        <v>42452.291666666664</v>
+      </c>
+      <c r="H44" s="10">
+        <f>$C$44/H$40</f>
+        <v>33961.833333333336</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="27">
+        <f>Y9</f>
+        <v>4010210</v>
+      </c>
+      <c r="D45" s="28">
+        <f>$C$45/D$40</f>
+        <v>668368.33333333337</v>
+      </c>
+      <c r="E45" s="28">
+        <f>$C$45/E$40</f>
+        <v>334184.16666666669</v>
+      </c>
+      <c r="F45" s="28">
+        <f>$C$45/F$40</f>
+        <v>167092.08333333334</v>
+      </c>
+      <c r="G45" s="29">
+        <f>$C$45/G$40</f>
+        <v>83546.041666666672</v>
+      </c>
+      <c r="H45" s="10">
+        <f>$C$45/H$40</f>
+        <v>66836.833333333328</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5604,8 +7149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:W44"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6417,6 +7962,9 @@
     </row>
     <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="L33">
         <v>8</v>
@@ -6444,10 +7992,7 @@
       <c r="C34" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="1">
-        <f>J42</f>
-        <v>14385.4453125</v>
-      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="1">
         <f>J43</f>
         <v>30506.39453125</v>
@@ -6544,10 +8089,6 @@
       <c r="C36">
         <v>16</v>
       </c>
-      <c r="D36">
-        <f>H7</f>
-        <v>10.47</v>
-      </c>
       <c r="E36">
         <f>O7</f>
         <v>518.11900000000003</v>
@@ -6596,10 +8137,6 @@
       <c r="C37">
         <v>32</v>
       </c>
-      <c r="D37">
-        <f>O8</f>
-        <v>307.14999999999998</v>
-      </c>
       <c r="E37">
         <f>H19</f>
         <v>677.45</v>
@@ -6647,10 +8184,6 @@
     <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>64</v>
-      </c>
-      <c r="D38">
-        <f>W20</f>
-        <v>598.66999999999996</v>
       </c>
       <c r="E38" s="3">
         <f>O20</f>

</xml_diff>

<commit_message>
Serial run for pipe04 added. Added definition of eff for weak scaling
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HSR Cluster" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="68">
   <si>
     <t>pipe01</t>
   </si>
@@ -198,12 +198,6 @@
     <t>mean # cores</t>
   </si>
   <si>
-    <t>different file has been computed</t>
-  </si>
-  <si>
-    <t>job download error</t>
-  </si>
-  <si>
     <t>sizeup</t>
   </si>
   <si>
@@ -212,13 +206,34 @@
   <si>
     <t>Strong scaling</t>
   </si>
+  <si>
+    <t>Strong Scaling</t>
+  </si>
+  <si>
+    <t>Sizeup</t>
+  </si>
+  <si>
+    <t>Weak Scaling</t>
+  </si>
+  <si>
+    <t>check the iterative solvers</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>SizeUp</t>
+  </si>
+  <si>
+    <t>not enough memory on siet0003</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -351,12 +366,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -376,6 +385,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,7 +477,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -497,42 +512,45 @@
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="3"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -652,7 +670,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1186,11 +1203,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209767856"/>
-        <c:axId val="209482024"/>
+        <c:axId val="209669840"/>
+        <c:axId val="130707296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209767856"/>
+        <c:axId val="209669840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,7 +1225,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209482024"/>
+        <c:crossAx val="130707296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1216,7 +1233,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209482024"/>
+        <c:axId val="130707296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1258,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209767856"/>
+        <c:crossAx val="209669840"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1254,7 +1271,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1596,11 +1612,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209344688"/>
-        <c:axId val="209345072"/>
+        <c:axId val="209783576"/>
+        <c:axId val="209346000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209344688"/>
+        <c:axId val="209783576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1634,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209345072"/>
+        <c:crossAx val="209346000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1626,7 +1642,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209345072"/>
+        <c:axId val="209346000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,7 +1667,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209344688"/>
+        <c:crossAx val="209783576"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1664,7 +1680,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1724,7 +1739,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1812,15 +1826,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SimplyHPC A8'!$E$42:$E$46</c:f>
+              <c:f>'SimplyHPC A8'!$E$42:$E$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>518.11900000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>677.45</c:v>
@@ -1830,6 +1844,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>781.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1108.038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1915,12 +1932,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SimplyHPC A8'!$F$42:$F$45</c:f>
+              <c:f>'SimplyHPC A8'!$F$42:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>986.61</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1264.05</c:v>
@@ -1930,6 +1947,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1216.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1246.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1546.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1999,7 +2022,7 @@
                   <c:v>2237.1799999999998</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2078.0300000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,23 +2075,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SimplyHPC A8'!$D$43:$D$47</c:f>
+              <c:f>'SimplyHPC A8'!$D$42:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
                   <c:v>10.47</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>307.14999999999998</c:v>
-                </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>441</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>499.97</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>681.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2086,11 +2109,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209339088"/>
-        <c:axId val="210031592"/>
+        <c:axId val="210078168"/>
+        <c:axId val="210045104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209339088"/>
+        <c:axId val="210078168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2108,7 +2131,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210031592"/>
+        <c:crossAx val="210045104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2116,7 +2139,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210031592"/>
+        <c:axId val="210045104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2164,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209339088"/>
+        <c:crossAx val="210078168"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2154,7 +2177,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2214,7 +2236,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2336,7 +2357,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SimplyHPC A8'!$L$14</c:f>
+              <c:f>'SimplyHPC A8'!$O$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2412,7 +2433,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SimplyHPC A8'!$Q$18:$Q$23</c:f>
+              <c:f>'SimplyHPC A8'!$T$18:$T$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2524,7 +2545,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00E+00">
+                <c:pt idx="0">
                   <c:v>2478.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -2540,7 +2561,7 @@
                   <c:v>383.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>410.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,7 +2573,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SimplyHPC A8'!$L$3</c:f>
+              <c:f>'SimplyHPC A8'!$R$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2632,24 +2653,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>986.61</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>518.11900000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>307.14999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>252.13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>216.96</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>296.72000000000003</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2773,11 +2776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209705968"/>
-        <c:axId val="208556784"/>
+        <c:axId val="210583448"/>
+        <c:axId val="210583840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209705968"/>
+        <c:axId val="210583448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,7 +2798,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="208556784"/>
+        <c:crossAx val="210583840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2803,7 +2806,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208556784"/>
+        <c:axId val="210583840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2828,7 +2831,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209705968"/>
+        <c:crossAx val="210583448"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2841,7 +2844,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2901,7 +2903,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3083,11 +3084,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="208558744"/>
-        <c:axId val="208559136"/>
+        <c:axId val="210586584"/>
+        <c:axId val="210586976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208558744"/>
+        <c:axId val="210586584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3105,7 +3106,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="208559136"/>
+        <c:crossAx val="210586976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3113,7 +3114,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208559136"/>
+        <c:axId val="210586976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3138,7 +3139,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="208558744"/>
+        <c:crossAx val="210586584"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3597,8 +3598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3618,10 +3619,10 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="50" t="s">
+      <c r="R3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="50"/>
+      <c r="S3" s="57"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -3667,10 +3668,10 @@
         <v>48</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="X4" t="s">
         <v>7</v>
@@ -3698,7 +3699,7 @@
       <c r="H5" s="6"/>
       <c r="J5" s="26"/>
       <c r="K5" s="2">
-        <f>$C$45/L5</f>
+        <f t="shared" ref="K5:K11" si="1">$C$45/L5</f>
         <v>432919</v>
       </c>
       <c r="L5" s="6">
@@ -3711,7 +3712,7 @@
         <v>25.87</v>
       </c>
       <c r="O5" s="26">
-        <f t="shared" ref="O5" si="1">M5*60+N5</f>
+        <f t="shared" ref="O5" si="2">M5*60+N5</f>
         <v>5965.87</v>
       </c>
       <c r="P5" s="6"/>
@@ -3727,7 +3728,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <f>$C$44/C6</f>
+        <f t="shared" ref="B6:B11" si="3">$C$44/C6</f>
         <v>32517</v>
       </c>
       <c r="C6">
@@ -3740,7 +3741,7 @@
         <v>54.62</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ref="F6:F11" si="2">D6*60+E6</f>
+        <f t="shared" ref="F6:F11" si="4">D6*60+E6</f>
         <v>894.62</v>
       </c>
       <c r="G6" s="27">
@@ -3752,7 +3753,7 @@
         <v>0.4267765457214609</v>
       </c>
       <c r="K6" s="2">
-        <f>$C$45/L6</f>
+        <f t="shared" si="1"/>
         <v>72153.166666666672</v>
       </c>
       <c r="L6">
@@ -3765,7 +3766,7 @@
         <v>4.79</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" ref="O6:O11" si="3">M6*60+N6</f>
+        <f t="shared" ref="O6:O11" si="5">M6*60+N6</f>
         <v>1864.79</v>
       </c>
       <c r="P6" s="27">
@@ -3780,7 +3781,7 @@
         <f>K6/$K$5*$O$5/O6</f>
         <v>0.53320302375423867</v>
       </c>
-      <c r="S6" s="39">
+      <c r="S6" s="38">
         <f>R6/L6</f>
         <v>8.886717062570644E-2</v>
       </c>
@@ -3793,7 +3794,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <f>$C$44/C7</f>
+        <f t="shared" si="3"/>
         <v>16258.5</v>
       </c>
       <c r="C7">
@@ -3806,19 +3807,19 @@
         <v>6.45</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>486.45</v>
       </c>
       <c r="G7" s="27">
-        <f t="shared" ref="G7:G11" si="4">$F$5/F7</f>
+        <f t="shared" ref="G7:G11" si="6">$F$5/F7</f>
         <v>4.7092548052215024</v>
       </c>
       <c r="H7" s="27">
-        <f t="shared" ref="H7:H11" si="5">G7/C7</f>
+        <f t="shared" ref="H7:H11" si="7">G7/C7</f>
         <v>0.39243790043512522</v>
       </c>
       <c r="K7" s="2">
-        <f>$C$45/L7</f>
+        <f t="shared" si="1"/>
         <v>36076.583333333336</v>
       </c>
       <c r="L7">
@@ -3831,23 +3832,23 @@
         <v>23.86</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>743.86</v>
       </c>
       <c r="P7" s="27">
-        <f t="shared" ref="P7:P11" si="6">$O$5/O7</f>
+        <f t="shared" ref="P7:P11" si="8">$O$5/O7</f>
         <v>8.0201516414379039</v>
       </c>
       <c r="Q7" s="27">
-        <f t="shared" ref="Q7:Q11" si="7">P7/L7</f>
+        <f t="shared" ref="Q7:Q11" si="9">P7/L7</f>
         <v>0.66834597011982533</v>
       </c>
       <c r="R7" s="27">
-        <f t="shared" ref="R7:R11" si="8">K7/$K$5*$O$5/O7</f>
+        <f t="shared" ref="R7:R11" si="10">K7/$K$5*$O$5/O7</f>
         <v>0.66834597011982544</v>
       </c>
-      <c r="S7" s="39">
-        <f t="shared" ref="S7:S11" si="9">R7/L7</f>
+      <c r="S7" s="38">
+        <f t="shared" ref="S7:S11" si="11">R7/L7</f>
         <v>5.5695497509985453E-2</v>
       </c>
       <c r="X7" t="s">
@@ -3859,7 +3860,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <f>$C$44/C8</f>
+        <f t="shared" si="3"/>
         <v>8129.25</v>
       </c>
       <c r="C8">
@@ -3872,19 +3873,19 @@
         <v>34.65</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>274.64999999999998</v>
       </c>
       <c r="G8" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.3408592754414723</v>
       </c>
       <c r="H8" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.34753580314339466</v>
       </c>
       <c r="K8" s="2">
-        <f>$C$45/L8</f>
+        <f t="shared" si="1"/>
         <v>18038.291666666668</v>
       </c>
       <c r="L8">
@@ -3897,23 +3898,23 @@
         <v>44.37</v>
       </c>
       <c r="O8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>524.37</v>
       </c>
       <c r="P8" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>11.377214562236588</v>
       </c>
       <c r="Q8" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.47405060675985783</v>
       </c>
       <c r="R8" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.47405060675985788</v>
       </c>
-      <c r="S8" s="39">
-        <f t="shared" si="9"/>
+      <c r="S8" s="38">
+        <f t="shared" si="11"/>
         <v>1.9752108614994077E-2</v>
       </c>
       <c r="X8" t="s">
@@ -3925,7 +3926,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <f>$C$44/C9</f>
+        <f t="shared" si="3"/>
         <v>5419.5</v>
       </c>
       <c r="C9">
@@ -3938,19 +3939,19 @@
         <v>39.74</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>219.74</v>
       </c>
       <c r="G9" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.425125147902065</v>
       </c>
       <c r="H9" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.28958680966394623</v>
       </c>
       <c r="K9" s="2">
-        <f>$C$45/L9</f>
+        <f t="shared" si="1"/>
         <v>12025.527777777777</v>
       </c>
       <c r="L9">
@@ -3963,23 +3964,23 @@
         <v>16.78</v>
       </c>
       <c r="O9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>376.78</v>
       </c>
       <c r="P9" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>15.833828759488297</v>
       </c>
       <c r="Q9" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.43982857665245267</v>
       </c>
       <c r="R9" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.43982857665245267</v>
       </c>
-      <c r="S9" s="39">
-        <f t="shared" si="9"/>
+      <c r="S9" s="38">
+        <f t="shared" si="11"/>
         <v>1.2217460462568129E-2</v>
       </c>
       <c r="X9" t="s">
@@ -3991,7 +3992,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <f>$C$44/C10</f>
+        <f t="shared" si="3"/>
         <v>4064.625</v>
       </c>
       <c r="C10">
@@ -4004,19 +4005,19 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>188.05</v>
       </c>
       <c r="G10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12.181956926349374</v>
       </c>
       <c r="H10" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.25379076929894528</v>
       </c>
       <c r="K10" s="2">
-        <f>$C$45/L10</f>
+        <f t="shared" si="1"/>
         <v>9019.1458333333339</v>
       </c>
       <c r="L10">
@@ -4029,29 +4030,29 @@
         <v>36.299999999999997</v>
       </c>
       <c r="O10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>336.3</v>
       </c>
       <c r="P10" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17.739726434730894</v>
       </c>
       <c r="Q10" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.36957763405689364</v>
       </c>
       <c r="R10" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.36957763405689364</v>
       </c>
-      <c r="S10" s="39">
-        <f t="shared" si="9"/>
+      <c r="S10" s="38">
+        <f t="shared" si="11"/>
         <v>7.6995340428519512E-3</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <f>$C$44/C11</f>
+        <f t="shared" si="3"/>
         <v>3251.7</v>
       </c>
       <c r="C11">
@@ -4064,19 +4065,19 @@
         <v>51.94</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>171.94</v>
       </c>
       <c r="G11" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13.323351169012446</v>
       </c>
       <c r="H11" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.22205585281687409</v>
       </c>
       <c r="K11" s="2">
-        <f>$C$45/L11</f>
+        <f t="shared" si="1"/>
         <v>7215.3166666666666</v>
       </c>
       <c r="L11">
@@ -4089,34 +4090,34 @@
         <v>24.225000000000001</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>264.22500000000002</v>
       </c>
       <c r="P11" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>22.578749172107102</v>
       </c>
       <c r="Q11" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.37631248620178503</v>
       </c>
       <c r="R11" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.37631248620178509</v>
       </c>
-      <c r="S11" s="39">
-        <f t="shared" si="9"/>
+      <c r="S11" s="38">
+        <f t="shared" si="11"/>
         <v>6.2718747700297511E-3</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
-        <v>62</v>
-      </c>
-      <c r="R12" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="S12" s="50"/>
+      <c r="S12" s="57"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -4162,7 +4163,7 @@
         <v>48</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S13" s="6" t="s">
         <v>48</v>
@@ -4180,12 +4181,12 @@
         <v>7.12</v>
       </c>
       <c r="F14" s="26">
-        <f t="shared" ref="F14" si="10">D14*60+E14</f>
+        <f t="shared" ref="F14" si="12">D14*60+E14</f>
         <v>13687.12</v>
       </c>
       <c r="J14" s="26"/>
       <c r="K14" s="2">
-        <f>$C$47/L14</f>
+        <f t="shared" ref="K14:K20" si="13">$C$47/L14</f>
         <v>2037710</v>
       </c>
       <c r="L14">
@@ -4198,7 +4199,7 @@
         <v>56.62</v>
       </c>
       <c r="O14" s="26">
-        <f t="shared" ref="O14:O15" si="11">M14*60+N14</f>
+        <f t="shared" ref="O14:O15" si="14">M14*60+N14</f>
         <v>17036.62</v>
       </c>
       <c r="P14" s="6"/>
@@ -4208,7 +4209,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <f>$C$46/C15</f>
+        <f t="shared" ref="B15:B20" si="15">$C$46/C15</f>
         <v>169595.5</v>
       </c>
       <c r="C15" s="6">
@@ -4220,8 +4221,8 @@
       <c r="E15" s="6">
         <v>46.72</v>
       </c>
-      <c r="F15" s="35">
-        <f t="shared" ref="F15" si="12">D15*60+E15</f>
+      <c r="F15" s="34">
+        <f t="shared" ref="F15" si="16">D15*60+E15</f>
         <v>4546.72</v>
       </c>
       <c r="G15" s="27">
@@ -4233,7 +4234,7 @@
         <v>0.50172138743240546</v>
       </c>
       <c r="K15" s="2">
-        <f>$C$47/L15</f>
+        <f t="shared" si="13"/>
         <v>339618.33333333331</v>
       </c>
       <c r="L15" s="6">
@@ -4245,8 +4246,8 @@
       <c r="N15" s="6">
         <v>39.585000000000001</v>
       </c>
-      <c r="O15" s="37">
-        <f t="shared" si="11"/>
+      <c r="O15" s="36">
+        <f t="shared" si="14"/>
         <v>7779.585</v>
       </c>
       <c r="P15" s="27">
@@ -4261,14 +4262,14 @@
         <f>K15/$K$14*$O$14/O15</f>
         <v>0.36498562155522002</v>
       </c>
-      <c r="S15" s="39">
+      <c r="S15" s="38">
         <f>R15/L15</f>
         <v>6.0830936925870001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <f>$C$46/C16</f>
+        <f t="shared" si="15"/>
         <v>84797.75</v>
       </c>
       <c r="C16">
@@ -4285,15 +4286,15 @@
         <v>2365.75</v>
       </c>
       <c r="G16" s="27">
-        <f t="shared" ref="G16:G20" si="13">$F$14/F16</f>
+        <f t="shared" ref="G16:G20" si="17">$F$14/F16</f>
         <v>5.7855310155341861</v>
       </c>
       <c r="H16" s="27">
-        <f t="shared" ref="H16:H20" si="14">G16/C16</f>
+        <f t="shared" ref="H16:H20" si="18">G16/C16</f>
         <v>0.48212758462784883</v>
       </c>
       <c r="K16" s="2">
-        <f>$C$47/L16</f>
+        <f t="shared" si="13"/>
         <v>169809.16666666666</v>
       </c>
       <c r="L16">
@@ -4305,30 +4306,30 @@
       <c r="N16">
         <v>52.02</v>
       </c>
-      <c r="O16" s="35">
+      <c r="O16" s="34">
         <f>M16*60+N16</f>
         <v>4072.02</v>
       </c>
       <c r="P16" s="27">
-        <f t="shared" ref="P16:P20" si="15">$O$14/O16</f>
+        <f t="shared" ref="P16:P20" si="19">$O$14/O16</f>
         <v>4.1838252267916163</v>
       </c>
       <c r="Q16" s="27">
-        <f t="shared" ref="Q16:Q20" si="16">P16/L16</f>
+        <f t="shared" ref="Q16:Q20" si="20">P16/L16</f>
         <v>0.34865210223263471</v>
       </c>
       <c r="R16" s="27">
-        <f t="shared" ref="R16:R20" si="17">K16/$K$14*$O$14/O16</f>
+        <f t="shared" ref="R16:R20" si="21">K16/$K$14*$O$14/O16</f>
         <v>0.34865210223263471</v>
       </c>
-      <c r="S16" s="39">
-        <f t="shared" ref="S16:S20" si="18">R16/L16</f>
+      <c r="S16" s="38">
+        <f t="shared" ref="S16:S20" si="22">R16/L16</f>
         <v>2.9054341852719559E-2</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <f>$C$46/C17</f>
+        <f t="shared" si="15"/>
         <v>42398.875</v>
       </c>
       <c r="C17">
@@ -4345,15 +4346,15 @@
         <v>1223.82</v>
       </c>
       <c r="G17" s="27">
+        <f t="shared" si="17"/>
+        <v>11.183932277622528</v>
+      </c>
+      <c r="H17" s="27">
+        <f t="shared" si="18"/>
+        <v>0.465997178234272</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="13"/>
-        <v>11.183932277622528</v>
-      </c>
-      <c r="H17" s="27">
-        <f t="shared" si="14"/>
-        <v>0.465997178234272</v>
-      </c>
-      <c r="K17" s="2">
-        <f>$C$47/L17</f>
         <v>84904.583333333328</v>
       </c>
       <c r="L17">
@@ -4370,25 +4371,25 @@
         <v>2008.19</v>
       </c>
       <c r="P17" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>8.4835697817437588</v>
       </c>
       <c r="Q17" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.35348207423932326</v>
       </c>
       <c r="R17" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.35348207423932326</v>
       </c>
-      <c r="S17" s="39">
-        <f t="shared" si="18"/>
+      <c r="S17" s="38">
+        <f t="shared" si="22"/>
         <v>1.4728419759971802E-2</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <f>$C$46/C18</f>
+        <f t="shared" si="15"/>
         <v>28265.916666666668</v>
       </c>
       <c r="C18">
@@ -4405,15 +4406,15 @@
         <v>835.63</v>
       </c>
       <c r="G18" s="27">
+        <f t="shared" si="17"/>
+        <v>16.379402367076338</v>
+      </c>
+      <c r="H18" s="27">
+        <f t="shared" si="18"/>
+        <v>0.45498339908545382</v>
+      </c>
+      <c r="K18" s="2">
         <f t="shared" si="13"/>
-        <v>16.379402367076338</v>
-      </c>
-      <c r="H18" s="27">
-        <f t="shared" si="14"/>
-        <v>0.45498339908545382</v>
-      </c>
-      <c r="K18" s="2">
-        <f>$C$47/L18</f>
         <v>56603.055555555555</v>
       </c>
       <c r="L18">
@@ -4430,25 +4431,25 @@
         <v>1404.86</v>
       </c>
       <c r="P18" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>12.126916561080819</v>
       </c>
       <c r="Q18" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.33685879336335606</v>
       </c>
       <c r="R18" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.33685879336335611</v>
       </c>
-      <c r="S18" s="39">
-        <f t="shared" si="18"/>
+      <c r="S18" s="38">
+        <f t="shared" si="22"/>
         <v>9.3571887045376702E-3</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <f>$C$46/C19</f>
+        <f t="shared" si="15"/>
         <v>21199.4375</v>
       </c>
       <c r="C19">
@@ -4465,15 +4466,15 @@
         <v>657.32</v>
       </c>
       <c r="G19" s="27">
+        <f t="shared" si="17"/>
+        <v>20.822613034747153</v>
+      </c>
+      <c r="H19" s="27">
+        <f t="shared" si="18"/>
+        <v>0.43380443822389902</v>
+      </c>
+      <c r="K19" s="2">
         <f t="shared" si="13"/>
-        <v>20.822613034747153</v>
-      </c>
-      <c r="H19" s="27">
-        <f t="shared" si="14"/>
-        <v>0.43380443822389902</v>
-      </c>
-      <c r="K19" s="2">
-        <f>$C$47/L19</f>
         <v>42452.291666666664</v>
       </c>
       <c r="L19">
@@ -4490,25 +4491,25 @@
         <v>1096.6099999999999</v>
       </c>
       <c r="P19" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>15.535714611393294</v>
       </c>
       <c r="Q19" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.3236607210706936</v>
       </c>
       <c r="R19" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.32366072107069366</v>
       </c>
-      <c r="S19" s="39">
-        <f t="shared" si="18"/>
+      <c r="S19" s="38">
+        <f t="shared" si="22"/>
         <v>6.7429316889727848E-3</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <f>$C$46/C20</f>
+        <f t="shared" si="15"/>
         <v>16959.55</v>
       </c>
       <c r="C20">
@@ -4525,15 +4526,15 @@
         <v>597.59</v>
       </c>
       <c r="G20" s="27">
+        <f t="shared" si="17"/>
+        <v>22.903863853143459</v>
+      </c>
+      <c r="H20" s="27">
+        <f t="shared" si="18"/>
+        <v>0.38173106421905767</v>
+      </c>
+      <c r="K20" s="2">
         <f t="shared" si="13"/>
-        <v>22.903863853143459</v>
-      </c>
-      <c r="H20" s="27">
-        <f t="shared" si="14"/>
-        <v>0.38173106421905767</v>
-      </c>
-      <c r="K20" s="2">
-        <f>$C$47/L20</f>
         <v>33961.833333333336</v>
       </c>
       <c r="L20">
@@ -4550,19 +4551,19 @@
         <v>915.85</v>
       </c>
       <c r="P20" s="27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>18.601976306163671</v>
       </c>
       <c r="Q20" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.31003293843606117</v>
       </c>
       <c r="R20" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.31003293843606122</v>
       </c>
-      <c r="S20" s="39">
-        <f t="shared" si="18"/>
+      <c r="S20" s="38">
+        <f t="shared" si="22"/>
         <v>5.1672156406010203E-3</v>
       </c>
     </row>
@@ -4613,7 +4614,7 @@
       <c r="Q22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S22" s="38" t="s">
+      <c r="S22" s="37" t="s">
         <v>51</v>
       </c>
       <c r="T22" s="6" t="s">
@@ -4652,18 +4653,22 @@
         <v>55036.17</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="J23" s="40"/>
+      <c r="J23" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="L23" s="6">
         <v>1</v>
       </c>
-      <c r="R23" s="29"/>
+      <c r="R23" s="28" t="s">
+        <v>67</v>
+      </c>
       <c r="T23" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <f>$C$48/C24</f>
+        <f t="shared" ref="B24:B29" si="23">$C$48/C24</f>
         <v>668368.33333333337</v>
       </c>
       <c r="C24" s="6">
@@ -4676,7 +4681,7 @@
         <v>22.85</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" ref="F23:F24" si="19">D24*60+E24</f>
+        <f t="shared" ref="F24" si="24">D24*60+E24</f>
         <v>17722.849999999999</v>
       </c>
       <c r="G24" s="27">
@@ -4684,7 +4689,7 @@
         <v>3.1053792138397607</v>
       </c>
       <c r="H24" s="27">
-        <f t="shared" ref="H24:H29" si="20">G24/C24</f>
+        <f t="shared" ref="H24:H29" si="25">G24/C24</f>
         <v>0.51756320230662678</v>
       </c>
       <c r="L24" s="6">
@@ -4697,7 +4702,7 @@
         <v>36.43</v>
       </c>
       <c r="O24" s="6">
-        <f t="shared" ref="O24:O25" si="21">M24*60+N24</f>
+        <f t="shared" ref="O24:O25" si="26">M24*60+N24</f>
         <v>38076.43</v>
       </c>
       <c r="R24" s="6"/>
@@ -4712,13 +4717,13 @@
         <v>25.52</v>
       </c>
       <c r="W24" s="6">
-        <f t="shared" ref="W24:W28" si="22">U24*60+V24</f>
+        <f t="shared" ref="W24:W28" si="27">U24*60+V24</f>
         <v>75325.52</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <f>$C$48/C25</f>
+        <f t="shared" si="23"/>
         <v>334184.16666666669</v>
       </c>
       <c r="C25">
@@ -4730,16 +4735,16 @@
       <c r="E25">
         <v>45.82</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="36">
         <f>D25*60+E25</f>
         <v>5985.82</v>
       </c>
       <c r="G25" s="27">
-        <f t="shared" ref="G25:G29" si="23">$F$23/F25</f>
+        <f t="shared" ref="G25:G29" si="28">$F$23/F25</f>
         <v>9.1944244898777452</v>
       </c>
       <c r="H25" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.76620204082314547</v>
       </c>
       <c r="J25" s="6"/>
@@ -4753,7 +4758,7 @@
         <v>49.49</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>18709.490000000002</v>
       </c>
       <c r="R25" s="6"/>
@@ -4768,13 +4773,13 @@
         <v>17.600000000000001</v>
       </c>
       <c r="W25" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>36077.599999999999</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <f>$C$48/C26</f>
+        <f t="shared" si="23"/>
         <v>167092.08333333334</v>
       </c>
       <c r="C26">
@@ -4786,16 +4791,16 @@
       <c r="E26">
         <v>23.74</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="34">
         <f>D26*60+E26</f>
         <v>4403.74</v>
       </c>
       <c r="G26" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>12.497597496673283</v>
       </c>
       <c r="H26" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.52073322902805341</v>
       </c>
       <c r="J26" s="6"/>
@@ -4808,7 +4813,7 @@
       <c r="N26">
         <v>25.94</v>
       </c>
-      <c r="O26" s="37">
+      <c r="O26" s="36">
         <f>M26*60+N26</f>
         <v>9025.94</v>
       </c>
@@ -4822,13 +4827,13 @@
         <v>54.67</v>
       </c>
       <c r="W26" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>16434.669999999998</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <f>$C$48/C27</f>
+        <f t="shared" si="23"/>
         <v>111394.72222222222</v>
       </c>
       <c r="C27">
@@ -4845,11 +4850,11 @@
         <v>2937.19</v>
       </c>
       <c r="G27" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>18.737694871629007</v>
       </c>
       <c r="H27" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.5204915242119168</v>
       </c>
       <c r="J27" s="6"/>
@@ -4863,7 +4868,7 @@
         <v>15.47</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" ref="O27:O29" si="24">M27*60+N27</f>
+        <f t="shared" ref="O27:O29" si="29">M27*60+N27</f>
         <v>5595.47</v>
       </c>
       <c r="T27" s="6">
@@ -4876,13 +4881,13 @@
         <v>13.78</v>
       </c>
       <c r="W27" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>10753.78</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <f>$C$48/C28</f>
+        <f t="shared" si="23"/>
         <v>83546.041666666672</v>
       </c>
       <c r="C28">
@@ -4899,11 +4904,11 @@
         <v>2239.5700000000002</v>
       </c>
       <c r="G28" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>24.574436164085068</v>
       </c>
       <c r="H28" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.51196742008510554</v>
       </c>
       <c r="L28" s="6">
@@ -4915,7 +4920,7 @@
       <c r="N28">
         <v>15.05</v>
       </c>
-      <c r="O28" s="35">
+      <c r="O28" s="34">
         <f>M28*60+N28</f>
         <v>4455.05</v>
       </c>
@@ -4930,13 +4935,13 @@
         <v>51.36</v>
       </c>
       <c r="W28" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>7971.36</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <f>$C$48/C29</f>
+        <f t="shared" si="23"/>
         <v>66836.833333333328</v>
       </c>
       <c r="C29">
@@ -4953,11 +4958,11 @@
         <v>1778.97</v>
       </c>
       <c r="G29" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>30.937098433363126</v>
       </c>
       <c r="H29" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.51561830722271873</v>
       </c>
       <c r="L29" s="6">
@@ -4970,7 +4975,7 @@
         <v>31.28</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3571.28</v>
       </c>
       <c r="T29" s="6">
@@ -4983,7 +4988,7 @@
         <v>31.82</v>
       </c>
       <c r="W29" s="6">
-        <f t="shared" ref="W29" si="25">U29*60+V29</f>
+        <f t="shared" ref="W29" si="30">U29*60+V29</f>
         <v>6391.82</v>
       </c>
     </row>
@@ -5021,19 +5026,19 @@
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="46">
+      <c r="C33" s="45">
         <f>C39</f>
         <v>38361.1875</v>
       </c>
-      <c r="D33" s="46">
+      <c r="D33" s="45">
         <f>D39</f>
         <v>81350.385416666672</v>
       </c>
-      <c r="E33" s="46">
+      <c r="E33" s="45">
         <f>E39</f>
         <v>167393.88333333333</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="35">
         <f>F39</f>
         <v>333686.95833333331</v>
       </c>
@@ -5252,19 +5257,19 @@
       <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="34">
+      <c r="C41" s="33">
         <f>C40/C39</f>
         <v>0.12807329737302903</v>
       </c>
-      <c r="D41" s="34">
+      <c r="D41" s="33">
         <f>D40/D39</f>
         <v>7.5751618322951936E-2</v>
       </c>
-      <c r="E41" s="34">
+      <c r="E41" s="33">
         <f>E40/E39</f>
         <v>2.0071743013824271E-2</v>
       </c>
-      <c r="F41" s="34">
+      <c r="F41" s="33">
         <f>F40/F39</f>
         <v>2.1637092259923132E-2</v>
       </c>
@@ -5355,7 +5360,7 @@
         <f>Y7</f>
         <v>1017573</v>
       </c>
-      <c r="D46" s="33">
+      <c r="D46" s="32">
         <f>$C$46/D$43</f>
         <v>169595.5</v>
       </c>
@@ -5384,11 +5389,11 @@
         <f>Y8</f>
         <v>2037710</v>
       </c>
-      <c r="D47" s="36">
+      <c r="D47" s="35">
         <f>$C$47/D$43</f>
         <v>339618.33333333331</v>
       </c>
-      <c r="E47" s="33">
+      <c r="E47" s="32">
         <f>$C$47/E$43</f>
         <v>169809.16666666666</v>
       </c>
@@ -5417,15 +5422,15 @@
         <f>$C$48/D$43</f>
         <v>668368.33333333337</v>
       </c>
-      <c r="E48" s="36">
+      <c r="E48" s="35">
         <f>$C$48/E$43</f>
         <v>334184.16666666669</v>
       </c>
-      <c r="F48" s="33">
+      <c r="F48" s="32">
         <f>$C$48/F$43</f>
         <v>167092.08333333334</v>
       </c>
-      <c r="G48" s="30">
+      <c r="G48" s="29">
         <f>$C$48/G$43</f>
         <v>83546.041666666672</v>
       </c>
@@ -5435,10 +5440,10 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="32">
+      <c r="C49" s="31">
         <v>8101299</v>
       </c>
       <c r="D49" s="15">
@@ -5446,27 +5451,27 @@
         <v>1350216.5</v>
       </c>
       <c r="E49" s="15">
-        <f t="shared" ref="E49:H49" si="26">$C$49/E$43</f>
+        <f t="shared" ref="E49:H49" si="31">$C$49/E$43</f>
         <v>675108.25</v>
       </c>
-      <c r="F49" s="36">
-        <f t="shared" si="26"/>
+      <c r="F49" s="35">
+        <f t="shared" si="31"/>
         <v>337554.125</v>
       </c>
-      <c r="G49" s="33">
-        <f t="shared" si="26"/>
+      <c r="G49" s="32">
+        <f t="shared" si="31"/>
         <v>168777.0625</v>
       </c>
       <c r="H49" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>84388.53125</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="32">
+      <c r="C50" s="31">
         <v>15522778</v>
       </c>
       <c r="D50" s="15">
@@ -5474,19 +5479,19 @@
         <v>2587129.6666666665</v>
       </c>
       <c r="E50" s="15">
-        <f t="shared" ref="E50:H50" si="27">$C$50/E$43</f>
+        <f t="shared" ref="E50:H50" si="32">$C$50/E$43</f>
         <v>1293564.8333333333</v>
       </c>
       <c r="F50" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>646782.41666666663</v>
       </c>
-      <c r="G50" s="36">
-        <f t="shared" si="27"/>
+      <c r="G50" s="35">
+        <f t="shared" si="32"/>
         <v>323391.20833333331</v>
       </c>
-      <c r="H50" s="33">
-        <f t="shared" si="27"/>
+      <c r="H50" s="32">
+        <f t="shared" si="32"/>
         <v>161695.60416666666</v>
       </c>
     </row>
@@ -5503,10 +5508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z61"/>
+  <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5527,7 +5532,7 @@
     <col min="20" max="20" width="11.09765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>20</v>
       </c>
@@ -5535,25 +5540,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C3" s="48" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="R4" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="51"/>
-      <c r="T4" s="55" t="s">
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="U4" s="55"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4" s="59"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -5578,38 +5601,51 @@
       <c r="J5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="S5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N5" t="s">
+      <c r="T5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O5" t="s">
+      <c r="U5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P5" t="s">
+      <c r="V5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="W5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="52" t="s">
+      <c r="X5" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="52" t="s">
+      <c r="Y5" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="U5" s="37" t="s">
+      <c r="Z5" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5" s="36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>$M$49</f>
+        <v>195102</v>
+      </c>
       <c r="D6">
         <v>1</v>
       </c>
@@ -5623,45 +5659,49 @@
         <v>13.51</v>
       </c>
       <c r="H6" s="6">
-        <f>F6*60+G6</f>
+        <f t="shared" ref="H6:H12" si="0">F6*60+G6</f>
         <v>13.51</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="2">
-        <f>$M$50/M6/N6</f>
+      <c r="L6" s="2"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="2">
+        <f>$M$50/S6/T6</f>
         <v>432919</v>
       </c>
-      <c r="M6">
+      <c r="S6" s="6">
         <v>1</v>
       </c>
-      <c r="N6">
+      <c r="T6" s="6">
         <v>1</v>
       </c>
-      <c r="O6">
+      <c r="U6" s="6">
         <v>109</v>
       </c>
-      <c r="P6">
+      <c r="V6" s="6">
         <v>55.97</v>
       </c>
-      <c r="Q6" s="6">
-        <f>O6*60+P6</f>
+      <c r="W6" s="6">
+        <f t="shared" ref="W6:W12" si="1">U6*60+V6</f>
         <v>6595.97</v>
       </c>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="36"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
-        <f>$M$49/E7</f>
+        <f t="shared" ref="C7:C13" si="2">$M$49/E7</f>
         <v>24387.75</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <f>D7*8</f>
+        <f t="shared" ref="E7:E13" si="3">D7*8</f>
         <v>8</v>
       </c>
       <c r="F7">
@@ -5671,7 +5711,7 @@
         <v>12.62</v>
       </c>
       <c r="H7">
-        <f>F7*60+G7</f>
+        <f t="shared" si="0"/>
         <v>12.62</v>
       </c>
       <c r="I7" s="27">
@@ -5682,54 +5722,58 @@
         <f>I7/E7</f>
         <v>0.13381537242472266</v>
       </c>
-      <c r="L7" s="2">
-        <f>$M$50/M7/N7</f>
+      <c r="L7" s="2"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="2">
+        <f>$M$50/S7/T7</f>
         <v>54114.875</v>
       </c>
-      <c r="M7">
+      <c r="S7" s="6">
         <v>1</v>
       </c>
-      <c r="N7">
-        <f>M7*8</f>
+      <c r="T7" s="6">
+        <f t="shared" ref="T7:T12" si="4">S7*8</f>
         <v>8</v>
       </c>
-      <c r="O7">
+      <c r="U7" s="6">
         <v>16</v>
       </c>
-      <c r="P7">
+      <c r="V7" s="6">
         <v>26.61</v>
       </c>
-      <c r="Q7">
-        <f>O7*60+P7</f>
+      <c r="W7" s="6">
+        <f t="shared" si="1"/>
         <v>986.61</v>
       </c>
-      <c r="R7" s="53">
-        <f>$Q$6/Q7</f>
+      <c r="X7" s="49">
+        <f>$W$6/W7</f>
         <v>6.6854886936074029</v>
       </c>
-      <c r="S7" s="53">
-        <f t="shared" ref="S7:S12" si="0">R7/N7</f>
+      <c r="Y7" s="49">
+        <f t="shared" ref="Y7:Y12" si="5">X7/T7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="T7" s="56">
-        <f>L7/$L$6*$Q$6/Q7</f>
+      <c r="Z7" s="60">
+        <f>R7/$R$6*$W$6/W7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="U7" s="57">
-        <f>T7/N7</f>
+      <c r="AA7" s="51">
+        <f t="shared" ref="AA7:AA12" si="6">Z7/T7</f>
         <v>0.10446076083761567</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
-        <f>$M$49/E8</f>
+        <f t="shared" si="2"/>
         <v>12193.875</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
-        <f>D8*8</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F8">
@@ -5739,65 +5783,69 @@
         <v>10.47</v>
       </c>
       <c r="H8">
-        <f>F8*60+G8</f>
+        <f t="shared" si="0"/>
         <v>10.47</v>
       </c>
       <c r="I8" s="27">
-        <f t="shared" ref="I8:I12" si="1">$H$6/H8</f>
+        <f t="shared" ref="I8:I12" si="7">$H$6/H8</f>
         <v>1.2903533906399234</v>
       </c>
       <c r="J8" s="27">
-        <f t="shared" ref="J8:J12" si="2">I8/E8</f>
+        <f t="shared" ref="J8:J12" si="8">I8/E8</f>
         <v>8.0647086914995211E-2</v>
       </c>
-      <c r="L8" s="2">
-        <f>$M$50/M8/N8</f>
-        <v>13528.71875</v>
-      </c>
-      <c r="M8">
+      <c r="L8" s="2"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="2">
+        <f t="shared" ref="R8:R13" si="9">$M$50/T8</f>
+        <v>27057.4375</v>
+      </c>
+      <c r="S8" s="6">
         <v>2</v>
       </c>
-      <c r="N8">
-        <f>M8*8</f>
+      <c r="T8" s="6">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="O8">
+      <c r="U8" s="6">
         <v>8</v>
       </c>
-      <c r="P8">
+      <c r="V8" s="6">
         <v>38.119</v>
       </c>
-      <c r="Q8">
-        <f>O8*60+P8</f>
+      <c r="W8" s="6">
+        <f t="shared" si="1"/>
         <v>518.11900000000003</v>
       </c>
-      <c r="R8" s="53">
-        <f t="shared" ref="R8:R12" si="3">$Q$6/Q8</f>
+      <c r="X8" s="49">
+        <f t="shared" ref="X8:X12" si="10">$W$6/W8</f>
         <v>12.730608219347292</v>
       </c>
-      <c r="S8" s="53">
-        <f t="shared" si="0"/>
+      <c r="Y8" s="49">
+        <f t="shared" si="5"/>
         <v>0.79566301370920578</v>
       </c>
-      <c r="T8" s="56">
-        <f t="shared" ref="T8:T11" si="4">L8/$L$6*$Q$6/Q8</f>
-        <v>0.39783150685460289</v>
-      </c>
-      <c r="U8" s="57">
-        <f t="shared" ref="U8:U12" si="5">T8/N8</f>
-        <v>2.4864469178412681E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z8" s="60">
+        <f t="shared" ref="Z8:Z12" si="11">R8/$R$6*$W$6/W8</f>
+        <v>0.79566301370920578</v>
+      </c>
+      <c r="AA8" s="51">
+        <f t="shared" si="6"/>
+        <v>4.9728938356825361E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
-        <f>$M$49/E9</f>
+        <f t="shared" si="2"/>
         <v>6096.9375</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9">
-        <f>D9*8</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="F9">
@@ -5807,65 +5855,69 @@
         <v>11.82</v>
       </c>
       <c r="H9">
-        <f>F9*60+G9</f>
+        <f t="shared" si="0"/>
         <v>11.82</v>
       </c>
       <c r="I9" s="27">
+        <f t="shared" si="7"/>
+        <v>1.1429780033840946</v>
+      </c>
+      <c r="J9" s="27">
+        <f t="shared" si="8"/>
+        <v>3.5718062605752957E-2</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="2">
+        <f t="shared" si="9"/>
+        <v>13528.71875</v>
+      </c>
+      <c r="S9" s="6">
+        <v>4</v>
+      </c>
+      <c r="T9" s="6">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="U9" s="6">
+        <v>5</v>
+      </c>
+      <c r="V9" s="6">
+        <v>7.15</v>
+      </c>
+      <c r="W9" s="6">
         <f t="shared" si="1"/>
-        <v>1.1429780033840946</v>
-      </c>
-      <c r="J9" s="27">
+        <v>307.14999999999998</v>
+      </c>
+      <c r="X9" s="49">
+        <f t="shared" si="10"/>
+        <v>21.474751749959307</v>
+      </c>
+      <c r="Y9" s="49">
+        <f t="shared" si="5"/>
+        <v>0.67108599218622833</v>
+      </c>
+      <c r="Z9" s="60">
+        <f t="shared" si="11"/>
+        <v>0.67108599218622833</v>
+      </c>
+      <c r="AA9" s="51">
+        <f t="shared" si="6"/>
+        <v>2.0971437255819635E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
         <f t="shared" si="2"/>
-        <v>3.5718062605752957E-2</v>
-      </c>
-      <c r="L9" s="2">
-        <f>$M$50/M9/N9</f>
-        <v>3382.1796875</v>
-      </c>
-      <c r="M9">
-        <v>4</v>
-      </c>
-      <c r="N9">
-        <f>M9*8</f>
-        <v>32</v>
-      </c>
-      <c r="O9">
-        <v>5</v>
-      </c>
-      <c r="P9">
-        <v>7.15</v>
-      </c>
-      <c r="Q9">
-        <f>O9*60+P9</f>
-        <v>307.14999999999998</v>
-      </c>
-      <c r="R9" s="53">
-        <f t="shared" si="3"/>
-        <v>21.474751749959307</v>
-      </c>
-      <c r="S9" s="53">
-        <f t="shared" si="0"/>
-        <v>0.67108599218622833</v>
-      </c>
-      <c r="T9" s="56">
-        <f t="shared" si="4"/>
-        <v>0.16777149804655708</v>
-      </c>
-      <c r="U9" s="57">
-        <f t="shared" si="5"/>
-        <v>5.2428593139549088E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C10" s="2">
-        <f>$M$49/E10</f>
         <v>3048.46875</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10">
-        <f>D10*8</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="F10">
@@ -5875,65 +5927,69 @@
         <v>15.96</v>
       </c>
       <c r="H10">
-        <f>F10*60+G10</f>
+        <f t="shared" si="0"/>
         <v>15.96</v>
       </c>
       <c r="I10" s="27">
+        <f t="shared" si="7"/>
+        <v>0.84649122807017541</v>
+      </c>
+      <c r="J10" s="27">
+        <f t="shared" si="8"/>
+        <v>1.3226425438596491E-2</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="2">
+        <f t="shared" si="9"/>
+        <v>6764.359375</v>
+      </c>
+      <c r="S10" s="6">
+        <v>8</v>
+      </c>
+      <c r="T10" s="6">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="U10" s="6">
+        <v>4</v>
+      </c>
+      <c r="V10" s="6">
+        <v>12.13</v>
+      </c>
+      <c r="W10" s="6">
         <f t="shared" si="1"/>
-        <v>0.84649122807017541</v>
-      </c>
-      <c r="J10" s="27">
+        <v>252.13</v>
+      </c>
+      <c r="X10" s="49">
+        <f t="shared" si="10"/>
+        <v>26.160988379010828</v>
+      </c>
+      <c r="Y10" s="50">
+        <f t="shared" si="5"/>
+        <v>0.40876544342204418</v>
+      </c>
+      <c r="Z10" s="60">
+        <f t="shared" si="11"/>
+        <v>0.40876544342204418</v>
+      </c>
+      <c r="AA10" s="51">
+        <f t="shared" si="6"/>
+        <v>6.3869600534694404E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
         <f t="shared" si="2"/>
-        <v>1.3226425438596491E-2</v>
-      </c>
-      <c r="L10" s="2">
-        <f>$M$50/M10/N10</f>
-        <v>845.544921875</v>
-      </c>
-      <c r="M10">
-        <v>8</v>
-      </c>
-      <c r="N10">
-        <f>M10*8</f>
-        <v>64</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <v>12.13</v>
-      </c>
-      <c r="Q10">
-        <f>O10*60+P10</f>
-        <v>252.13</v>
-      </c>
-      <c r="R10" s="53">
-        <f t="shared" si="3"/>
-        <v>26.160988379010828</v>
-      </c>
-      <c r="S10" s="54">
-        <f t="shared" si="0"/>
-        <v>0.40876544342204418</v>
-      </c>
-      <c r="T10" s="56">
-        <f t="shared" si="4"/>
-        <v>5.1095680427755523E-2</v>
-      </c>
-      <c r="U10" s="57">
-        <f t="shared" si="5"/>
-        <v>7.9837000668368005E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C11" s="2">
-        <f>$M$49/E11</f>
         <v>1524.234375</v>
       </c>
       <c r="D11">
         <v>16</v>
       </c>
       <c r="E11">
-        <f>D11*8</f>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="F11">
@@ -5943,65 +5999,71 @@
         <v>25.34</v>
       </c>
       <c r="H11" s="6">
-        <f>F11*60+G11</f>
+        <f t="shared" si="0"/>
         <v>25.34</v>
       </c>
       <c r="I11" s="27">
+        <f t="shared" si="7"/>
+        <v>0.53314917127071826</v>
+      </c>
+      <c r="J11" s="27">
+        <f t="shared" si="8"/>
+        <v>4.1652279005524864E-3</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="2">
+        <f t="shared" si="9"/>
+        <v>3382.1796875</v>
+      </c>
+      <c r="S11" s="6">
+        <v>16</v>
+      </c>
+      <c r="T11" s="6">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="U11" s="6">
+        <v>3</v>
+      </c>
+      <c r="V11" s="6">
+        <v>36.96</v>
+      </c>
+      <c r="W11" s="6">
         <f t="shared" si="1"/>
-        <v>0.53314917127071826</v>
-      </c>
-      <c r="J11" s="27">
-        <f t="shared" si="2"/>
-        <v>4.1652279005524864E-3</v>
-      </c>
-      <c r="L11" s="2">
-        <f>$M$50/M11/N11</f>
-        <v>1691.08984375</v>
-      </c>
-      <c r="M11">
-        <v>16</v>
-      </c>
-      <c r="N11">
-        <v>16</v>
-      </c>
-      <c r="O11">
-        <v>3</v>
-      </c>
-      <c r="P11">
-        <v>36.96</v>
-      </c>
-      <c r="Q11">
-        <f>O11*60+P11</f>
         <v>216.96</v>
       </c>
-      <c r="R11" s="53">
-        <f t="shared" si="3"/>
+      <c r="X11" s="49">
+        <f t="shared" si="10"/>
         <v>30.40177912979351</v>
       </c>
-      <c r="S11" s="53">
-        <f t="shared" si="0"/>
-        <v>1.9001111956120944</v>
-      </c>
-      <c r="T11" s="56">
-        <f t="shared" si="4"/>
-        <v>0.1187569497257559</v>
-      </c>
-      <c r="U11" s="57">
+      <c r="Y11" s="49">
         <f t="shared" si="5"/>
-        <v>7.4223093578597438E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+        <v>0.2375138994515118</v>
+      </c>
+      <c r="Z11" s="60">
+        <f t="shared" si="11"/>
+        <v>0.2375138994515118</v>
+      </c>
+      <c r="AA11" s="51">
+        <f t="shared" si="6"/>
+        <v>1.8555773394649359E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="2">
-        <f>$M$49/E12</f>
+        <f t="shared" si="2"/>
         <v>762.1171875</v>
       </c>
       <c r="D12">
         <v>32</v>
       </c>
       <c r="E12">
-        <f>D12*8</f>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="F12">
@@ -6011,132 +6073,165 @@
         <v>44.57</v>
       </c>
       <c r="H12" s="6">
-        <f>F12*60+G12</f>
+        <f t="shared" si="0"/>
         <v>44.57</v>
       </c>
       <c r="I12" s="27">
+        <f t="shared" si="7"/>
+        <v>0.303118689701593</v>
+      </c>
+      <c r="J12" s="27">
+        <f t="shared" si="8"/>
+        <v>1.1840573816468477E-3</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="2"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="2">
+        <f t="shared" si="9"/>
+        <v>1691.08984375</v>
+      </c>
+      <c r="S12" s="6">
+        <v>32</v>
+      </c>
+      <c r="T12" s="6">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="U12" s="6">
+        <v>4</v>
+      </c>
+      <c r="V12" s="6">
+        <v>56.72</v>
+      </c>
+      <c r="W12" s="6">
         <f t="shared" si="1"/>
-        <v>0.303118689701593</v>
-      </c>
-      <c r="J12" s="27">
-        <f t="shared" si="2"/>
-        <v>1.1840573816468477E-3</v>
-      </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="2">
-        <f>$M$50/M12/N12</f>
-        <v>422.7724609375</v>
-      </c>
-      <c r="M12">
-        <v>32</v>
-      </c>
-      <c r="N12">
-        <v>32</v>
-      </c>
-      <c r="O12">
-        <v>4</v>
-      </c>
-      <c r="P12">
-        <v>56.72</v>
-      </c>
-      <c r="Q12" s="6">
-        <f>O12*60+P12</f>
         <v>296.72000000000003</v>
       </c>
-      <c r="R12" s="53">
-        <f t="shared" si="3"/>
+      <c r="X12" s="49">
+        <f t="shared" si="10"/>
         <v>22.229610407117821</v>
       </c>
-      <c r="S12" s="53">
-        <f t="shared" si="0"/>
-        <v>0.69467532522243192</v>
-      </c>
-      <c r="T12" s="56">
-        <f>L12/$L$6*$Q$6/Q12</f>
-        <v>2.1708603913200997E-2</v>
-      </c>
-      <c r="U12" s="57">
+      <c r="Y12" s="49">
         <f t="shared" si="5"/>
-        <v>6.7839387228753117E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+        <v>8.683441565280399E-2</v>
+      </c>
+      <c r="Z12" s="60">
+        <f t="shared" si="11"/>
+        <v>8.683441565280399E-2</v>
+      </c>
+      <c r="AA12" s="51">
+        <f t="shared" si="6"/>
+        <v>3.3919693614376558E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="C13" s="2">
-        <f>$M$49/E13</f>
+        <f t="shared" si="2"/>
         <v>381.05859375</v>
       </c>
       <c r="D13">
         <v>64</v>
       </c>
       <c r="E13">
-        <f>D13*8</f>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="K13" s="26"/>
-      <c r="M13">
+      <c r="L13" s="2"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="2">
+        <f t="shared" si="9"/>
+        <v>845.544921875</v>
+      </c>
+      <c r="S13" s="6">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
+      <c r="T13" s="6">
+        <f t="shared" ref="T13" si="12">S13*8</f>
+        <v>512</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O14" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="T14" s="6" t="s">
+      <c r="W14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C15" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="M16" t="s">
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I16" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="57"/>
+      <c r="P16" t="s">
         <v>17</v>
       </c>
-      <c r="N16" t="s">
+      <c r="Q16" t="s">
         <v>18</v>
       </c>
-      <c r="O16" t="s">
+      <c r="R16" t="s">
         <v>19</v>
       </c>
-      <c r="P16" t="s">
+      <c r="S16" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="T16" t="s">
         <v>21</v>
       </c>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6" t="s">
+      <c r="W16" s="6"/>
+      <c r="X16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="V16" s="6" t="s">
+      <c r="Y16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="W16" s="6" t="s">
+      <c r="Z16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="X16" s="6" t="s">
+      <c r="AA16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y16" s="6" t="s">
+      <c r="AB16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Z16" s="6"/>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>17</v>
       </c>
@@ -6158,79 +6253,109 @@
       <c r="J17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="M17">
+      <c r="K17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="P17">
         <v>1</v>
       </c>
-      <c r="N17">
+      <c r="Q17">
         <v>1</v>
       </c>
-      <c r="T17" s="26"/>
-      <c r="U17" s="6">
+      <c r="R17">
+        <v>352</v>
+      </c>
+      <c r="S17">
+        <v>9.84</v>
+      </c>
+      <c r="T17" s="6">
+        <f>R17*60+S17</f>
+        <v>21129.84</v>
+      </c>
+      <c r="W17" s="26"/>
+      <c r="X17">
         <v>1</v>
       </c>
-      <c r="V17" s="6">
-        <f>U17*8</f>
-        <v>8</v>
-      </c>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="6"/>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="2">
+        <f>$M$51</f>
+        <v>1017573</v>
+      </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="H18" s="28"/>
-      <c r="L18" s="2">
-        <f>$M$52/N18</f>
+      <c r="F18">
+        <v>295</v>
+      </c>
+      <c r="G18">
+        <v>8.94</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" ref="H18:H23" si="13">F18*60+G18</f>
+        <v>17708.939999999999</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" ref="O18:O24" si="14">$M$52/Q18</f>
         <v>254713.75</v>
       </c>
-      <c r="M18">
+      <c r="P18">
         <v>1</v>
       </c>
-      <c r="N18">
-        <f>M18*8</f>
+      <c r="Q18">
+        <f t="shared" ref="Q18:Q24" si="15">P18*8</f>
         <v>8</v>
       </c>
-      <c r="O18">
+      <c r="R18">
         <v>66</v>
       </c>
-      <c r="P18">
+      <c r="S18">
         <v>13.31</v>
       </c>
-      <c r="Q18">
-        <f>O18*60+P18</f>
+      <c r="T18">
+        <f>R18*60+S18</f>
         <v>3973.31</v>
       </c>
-      <c r="T18" s="26"/>
-      <c r="U18" s="6">
-        <v>2</v>
-      </c>
-      <c r="V18" s="6">
-        <f>U18*8</f>
-        <v>16</v>
-      </c>
       <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="X18" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="6">
+        <f t="shared" ref="Y18:Y24" si="16">X18*8</f>
+        <v>8</v>
+      </c>
+      <c r="Z18">
+        <v>657</v>
+      </c>
+      <c r="AA18">
+        <v>53.48</v>
+      </c>
+      <c r="AB18" s="6">
+        <f t="shared" ref="AB18:AB23" si="17">Z18*60+AA18</f>
+        <v>39473.480000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
-        <f>$M$51/E19</f>
+        <f t="shared" ref="C19:C25" si="18">$M$51/E19</f>
         <v>127196.625</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <f>D19*8</f>
+        <f t="shared" ref="E19:E25" si="19">D19*8</f>
         <v>8</v>
       </c>
       <c r="F19">
@@ -6239,54 +6364,72 @@
       <c r="G19">
         <v>18.350000000000001</v>
       </c>
-      <c r="H19" s="24">
-        <f>F19*60+G19</f>
+      <c r="H19" s="52">
+        <f t="shared" si="13"/>
         <v>2478.35</v>
       </c>
-      <c r="L19" s="2">
-        <f>$M$52/N19</f>
+      <c r="I19" s="53">
+        <f>$H$18/H19</f>
+        <v>7.1454556458934366</v>
+      </c>
+      <c r="J19" s="27">
+        <f t="shared" ref="J19:J24" si="20">I19/E19</f>
+        <v>0.89318195573667958</v>
+      </c>
+      <c r="K19" s="2">
+        <f>C19/$C$18</f>
+        <v>0.125</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="14"/>
         <v>127356.875</v>
       </c>
-      <c r="M19">
+      <c r="P19">
         <v>2</v>
       </c>
-      <c r="N19">
-        <f>M19*8</f>
+      <c r="Q19">
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
-      <c r="O19">
+      <c r="R19">
         <v>31</v>
       </c>
-      <c r="P19">
+      <c r="S19">
         <v>48.35</v>
       </c>
-      <c r="Q19" s="24">
-        <f>O19*60+P19</f>
+      <c r="T19" s="24">
+        <f>R19*60+S19</f>
         <v>1908.35</v>
       </c>
-      <c r="T19" s="26"/>
-      <c r="U19" s="6">
-        <v>4</v>
-      </c>
-      <c r="V19" s="6">
-        <f>U19*8</f>
-        <v>32</v>
-      </c>
       <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="X19" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y19" s="6">
+        <f t="shared" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="Z19" s="6">
+        <v>284</v>
+      </c>
+      <c r="AA19" s="6">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="AB19" s="6">
+        <f t="shared" si="17"/>
+        <v>17044.89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
-        <f>$M$51/E20</f>
+        <f t="shared" si="18"/>
         <v>63598.3125</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20">
-        <f>D20*8</f>
+        <f t="shared" si="19"/>
         <v>16</v>
       </c>
       <c r="F20">
@@ -6296,55 +6439,71 @@
         <v>4.05</v>
       </c>
       <c r="H20">
-        <f>F20*60+G20</f>
+        <f t="shared" si="13"/>
         <v>1264.05</v>
       </c>
-      <c r="L20" s="2">
-        <f>$M$52/N20</f>
+      <c r="I20" s="53">
+        <f t="shared" ref="I20:I24" si="21">$H$18/H20</f>
+        <v>14.009683161267354</v>
+      </c>
+      <c r="J20" s="27">
+        <f t="shared" si="20"/>
+        <v>0.87560519757920963</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" ref="K20:K24" si="22">C20/$C$18</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="14"/>
         <v>63678.4375</v>
       </c>
-      <c r="M20">
+      <c r="P20">
         <v>4</v>
       </c>
-      <c r="N20">
-        <f>M20*8</f>
+      <c r="Q20">
+        <f t="shared" si="15"/>
         <v>32</v>
       </c>
-      <c r="O20">
+      <c r="R20">
         <v>16</v>
       </c>
-      <c r="P20">
+      <c r="S20">
         <v>30.21</v>
       </c>
-      <c r="Q20">
-        <f>O20*60+P20</f>
+      <c r="T20">
+        <f>R20*60+S20</f>
         <v>990.21</v>
       </c>
-      <c r="T20" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="U20" s="6">
-        <v>8</v>
-      </c>
-      <c r="V20" s="6">
-        <f>U20*8</f>
-        <v>64</v>
-      </c>
       <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-    </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="X20" s="6">
+        <v>4</v>
+      </c>
+      <c r="Y20" s="6">
+        <f t="shared" si="16"/>
+        <v>32</v>
+      </c>
+      <c r="Z20" s="6">
+        <v>73</v>
+      </c>
+      <c r="AA20" s="6">
+        <v>5.21</v>
+      </c>
+      <c r="AB20" s="6">
+        <f t="shared" si="17"/>
+        <v>4385.21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
-        <f>$M$51/E21</f>
+        <f t="shared" si="18"/>
         <v>31799.15625</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="E21">
-        <f>D21*8</f>
+        <f t="shared" si="19"/>
         <v>32</v>
       </c>
       <c r="F21">
@@ -6354,55 +6513,71 @@
         <v>17.45</v>
       </c>
       <c r="H21">
-        <f>F21*60+G21</f>
+        <f t="shared" si="13"/>
         <v>677.45</v>
       </c>
-      <c r="L21" s="2">
-        <f>$M$52/N21</f>
+      <c r="I21" s="53">
+        <f t="shared" si="21"/>
+        <v>26.140586021108565</v>
+      </c>
+      <c r="J21" s="27">
+        <f t="shared" si="20"/>
+        <v>0.81689331315964264</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="22"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="14"/>
         <v>31839.21875</v>
       </c>
-      <c r="M21">
+      <c r="P21">
         <v>8</v>
       </c>
-      <c r="N21">
-        <f>M21*8</f>
+      <c r="Q21">
+        <f t="shared" si="15"/>
         <v>64</v>
       </c>
-      <c r="O21">
+      <c r="R21">
         <v>9</v>
       </c>
-      <c r="P21">
+      <c r="S21">
         <v>54.84</v>
       </c>
-      <c r="Q21">
-        <f>O21*60+P21</f>
+      <c r="T21">
+        <f>R21*60+S21</f>
         <v>594.84</v>
       </c>
-      <c r="T21" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="U21" s="6">
-        <v>16</v>
-      </c>
-      <c r="V21" s="6">
-        <f>U21*8</f>
-        <v>128</v>
-      </c>
       <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="6"/>
-    </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="X21" s="6">
+        <v>8</v>
+      </c>
+      <c r="Y21" s="6">
+        <f t="shared" si="16"/>
+        <v>64</v>
+      </c>
+      <c r="Z21">
+        <v>65</v>
+      </c>
+      <c r="AA21">
+        <v>12.01</v>
+      </c>
+      <c r="AB21" s="6">
+        <f t="shared" si="17"/>
+        <v>3912.01</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
-        <f>$M$51/E22</f>
+        <f t="shared" si="18"/>
         <v>15899.578125</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
       <c r="E22">
-        <f>D22*8</f>
+        <f t="shared" si="19"/>
         <v>64</v>
       </c>
       <c r="F22">
@@ -6412,57 +6587,71 @@
         <v>21</v>
       </c>
       <c r="H22">
-        <f>F22*60+G22</f>
+        <f t="shared" si="13"/>
         <v>441</v>
       </c>
-      <c r="L22" s="2">
-        <f>$M$52/N22</f>
+      <c r="I22" s="53">
+        <f t="shared" si="21"/>
+        <v>40.15632653061224</v>
+      </c>
+      <c r="J22" s="27">
+        <f t="shared" si="20"/>
+        <v>0.62744260204081626</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="22"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="14"/>
         <v>15919.609375</v>
       </c>
-      <c r="M22">
+      <c r="P22">
         <v>16</v>
       </c>
-      <c r="N22">
-        <f>M22*8</f>
+      <c r="Q22">
+        <f t="shared" si="15"/>
         <v>128</v>
       </c>
-      <c r="O22">
+      <c r="R22">
         <v>8</v>
       </c>
-      <c r="P22">
+      <c r="S22">
         <v>19.97</v>
       </c>
-      <c r="Q22" s="6">
-        <f t="shared" ref="Q22:Q23" si="6">O22*60+P22</f>
+      <c r="T22" s="6">
+        <f t="shared" ref="T22:T23" si="23">R22*60+S22</f>
         <v>499.97</v>
       </c>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6">
-        <v>32</v>
-      </c>
-      <c r="V22" s="6">
-        <f>U22*8</f>
-        <v>256</v>
-      </c>
-      <c r="W22" s="6">
-        <v>25</v>
-      </c>
+      <c r="W22" s="6"/>
       <c r="X22" s="6">
-        <v>46.04</v>
-      </c>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-    </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="6">
+        <f t="shared" si="16"/>
+        <v>128</v>
+      </c>
+      <c r="Z22" s="6">
+        <v>34</v>
+      </c>
+      <c r="AA22" s="6">
+        <v>38.03</v>
+      </c>
+      <c r="AB22" s="24">
+        <f t="shared" si="17"/>
+        <v>2078.0300000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
-        <f>$M$51/E23</f>
+        <f t="shared" si="18"/>
         <v>7949.7890625</v>
       </c>
       <c r="D23">
         <v>16</v>
       </c>
       <c r="E23">
-        <f>D23*8</f>
+        <f t="shared" si="19"/>
         <v>128</v>
       </c>
       <c r="F23">
@@ -6472,92 +6661,137 @@
         <v>23.6</v>
       </c>
       <c r="H23" s="6">
-        <f>F23*60+G23</f>
+        <f t="shared" si="13"/>
         <v>383.6</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="2">
-        <f>$M$52/N23</f>
+      <c r="I23" s="53">
+        <f t="shared" si="21"/>
+        <v>46.165119916579762</v>
+      </c>
+      <c r="J23" s="27">
+        <f t="shared" si="20"/>
+        <v>0.36066499934827939</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="22"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="O23" s="2">
+        <f t="shared" si="14"/>
         <v>7959.8046875</v>
       </c>
-      <c r="M23">
+      <c r="P23">
         <v>32</v>
       </c>
-      <c r="N23">
-        <f>M23*8</f>
+      <c r="Q23">
+        <f t="shared" si="15"/>
         <v>256</v>
       </c>
-      <c r="O23">
+      <c r="R23">
         <v>8</v>
       </c>
-      <c r="P23" s="6">
+      <c r="S23" s="6">
         <v>36.68</v>
       </c>
-      <c r="Q23" s="6">
-        <f t="shared" si="6"/>
+      <c r="T23" s="6">
+        <f t="shared" si="23"/>
         <v>516.67999999999995</v>
       </c>
-      <c r="T23" s="26"/>
-      <c r="U23">
-        <v>64</v>
-      </c>
-      <c r="V23">
-        <f>U23*8</f>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B24" s="49"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6">
+        <v>32</v>
+      </c>
+      <c r="Y23" s="6">
+        <f t="shared" si="16"/>
+        <v>256</v>
+      </c>
+      <c r="Z23" s="6">
+        <v>25</v>
+      </c>
+      <c r="AA23" s="6">
+        <v>46.04</v>
+      </c>
+      <c r="AB23" s="42">
+        <f t="shared" si="17"/>
+        <v>1546.04</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
       <c r="C24" s="2">
-        <f>$M$51/E24</f>
+        <f t="shared" si="18"/>
         <v>3974.89453125</v>
       </c>
       <c r="D24">
         <v>32</v>
       </c>
       <c r="E24">
-        <f>D24*8</f>
+        <f t="shared" si="19"/>
         <v>256</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>50.21</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" ref="H23:H24" si="7">F24*60+G24</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="26"/>
-      <c r="L24" s="2">
-        <f>$M$52/N24</f>
+        <f t="shared" ref="H24" si="24">F24*60+G24</f>
+        <v>410.21</v>
+      </c>
+      <c r="I24" s="53">
+        <f t="shared" si="21"/>
+        <v>43.170424904317301</v>
+      </c>
+      <c r="J24" s="27">
+        <f t="shared" si="20"/>
+        <v>0.16863447228248946</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="22"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="N24" s="26"/>
+      <c r="O24" s="2">
+        <f t="shared" si="14"/>
         <v>3979.90234375</v>
       </c>
-      <c r="M24">
+      <c r="P24">
         <v>64</v>
       </c>
-      <c r="N24">
-        <f>M24*8</f>
+      <c r="Q24">
+        <f t="shared" si="15"/>
         <v>512</v>
       </c>
-    </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="W24" s="26"/>
+      <c r="X24">
+        <v>64</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="16"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B25" s="26"/>
       <c r="C25" s="2">
-        <f>$M$51/E25</f>
+        <f t="shared" si="18"/>
         <v>1987.447265625</v>
       </c>
       <c r="D25">
         <v>64</v>
       </c>
       <c r="E25">
-        <f>D25*8</f>
+        <f t="shared" si="19"/>
         <v>512</v>
       </c>
       <c r="U25" s="2"/>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="U26" s="2"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>11</v>
       </c>
@@ -6566,10 +6800,10 @@
       </c>
       <c r="U27" s="2"/>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>1</v>
       </c>
@@ -6611,15 +6845,17 @@
       </c>
       <c r="U29" s="2"/>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B30" s="46" t="s">
+        <v>65</v>
+      </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="H30" s="29"/>
+      <c r="H30" s="6"/>
       <c r="L30" s="26"/>
       <c r="M30">
         <v>1</v>
@@ -6629,16 +6865,16 @@
       </c>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
-        <f>$M$53/D31/E31</f>
+        <f t="shared" ref="C31:C37" si="25">$M$53/D31/E31</f>
         <v>501276.25</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <f>D31*8</f>
+        <f t="shared" ref="E31:E37" si="26">D31*8</f>
         <v>8</v>
       </c>
       <c r="F31">
@@ -6656,14 +6892,14 @@
         <v>0</v>
       </c>
       <c r="J31" s="27">
-        <f>I31/E31</f>
+        <f t="shared" ref="J31:J36" si="27">I31/E31</f>
         <v>0</v>
       </c>
       <c r="M31" s="6">
         <v>1</v>
       </c>
       <c r="N31" s="6">
-        <f>M31*8</f>
+        <f t="shared" ref="N31:N37" si="28">M31*8</f>
         <v>8</v>
       </c>
       <c r="O31">
@@ -6674,21 +6910,21 @@
         <v>11.82</v>
       </c>
       <c r="Q31" s="6">
-        <f t="shared" ref="Q31:Q32" si="8">O31*60+P31</f>
+        <f t="shared" ref="Q31:Q33" si="29">O31*60+P31</f>
         <v>20891.82</v>
       </c>
       <c r="U31" s="15"/>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
-        <f>$M$53/D32/E32</f>
+        <f t="shared" si="25"/>
         <v>125319.0625</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32">
-        <f>D32*8</f>
+        <f t="shared" si="26"/>
         <v>16</v>
       </c>
       <c r="F32">
@@ -6706,14 +6942,14 @@
         <v>0</v>
       </c>
       <c r="J32" s="27">
-        <f>I32/E32</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M32" s="6">
         <v>2</v>
       </c>
       <c r="N32" s="6">
-        <f>M32*8</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="O32">
@@ -6723,21 +6959,21 @@
         <v>0.92</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="29"/>
         <v>9480.92</v>
       </c>
       <c r="U32" s="15"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
-        <f>$M$53/D33/E33</f>
+        <f t="shared" si="25"/>
         <v>31329.765625</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33">
-        <f>D33*8</f>
+        <f t="shared" si="26"/>
         <v>32</v>
       </c>
       <c r="F33">
@@ -6755,28 +6991,38 @@
         <v>0</v>
       </c>
       <c r="J33" s="27">
-        <f>I33/E33</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="L33" s="26"/>
+      <c r="L33" s="6"/>
       <c r="M33" s="6">
         <v>4</v>
       </c>
       <c r="N33" s="6">
-        <f>M33*8</f>
+        <f t="shared" si="28"/>
         <v>32</v>
+      </c>
+      <c r="O33">
+        <v>75</v>
+      </c>
+      <c r="P33">
+        <v>58.41</v>
+      </c>
+      <c r="Q33" s="6">
+        <f t="shared" si="29"/>
+        <v>4558.41</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
-        <f>$M$53/D34/E34</f>
+        <f t="shared" si="25"/>
         <v>7832.44140625</v>
       </c>
       <c r="D34">
         <v>8</v>
       </c>
       <c r="E34">
-        <f>D34*8</f>
+        <f t="shared" si="26"/>
         <v>64</v>
       </c>
       <c r="F34">
@@ -6790,11 +7036,11 @@
         <v>1216.44</v>
       </c>
       <c r="I34" s="27">
-        <f t="shared" ref="I34:I36" si="9">$H$30/H34</f>
+        <f t="shared" ref="I34:I36" si="30">$H$30/H34</f>
         <v>0</v>
       </c>
       <c r="J34" s="27">
-        <f>I34/E34</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L34" s="6"/>
@@ -6802,7 +7048,7 @@
         <v>8</v>
       </c>
       <c r="N34" s="6">
-        <f>M34*8</f>
+        <f t="shared" si="28"/>
         <v>64</v>
       </c>
       <c r="O34">
@@ -6818,14 +7064,14 @@
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
-        <f>$M$53/D35/E35</f>
+        <f t="shared" si="25"/>
         <v>1958.1103515625</v>
       </c>
       <c r="D35">
         <v>16</v>
       </c>
       <c r="E35">
-        <f>D35*8</f>
+        <f t="shared" si="26"/>
         <v>128</v>
       </c>
       <c r="F35">
@@ -6835,15 +7081,15 @@
         <v>1.01</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" ref="H35:H36" si="10">F35*60+G35</f>
+        <f t="shared" ref="H35:H36" si="31">F35*60+G35</f>
         <v>781.01</v>
       </c>
       <c r="I35" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J35" s="27">
-        <f>I35/E35</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L35" s="6"/>
@@ -6851,7 +7097,7 @@
         <v>16</v>
       </c>
       <c r="N35" s="6">
-        <f>M35*8</f>
+        <f t="shared" si="28"/>
         <v>128</v>
       </c>
       <c r="O35">
@@ -6861,21 +7107,21 @@
         <v>46.78</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" ref="Q35" si="11">O35*60+P35</f>
+        <f t="shared" ref="Q35:Q36" si="32">O35*60+P35</f>
         <v>1246.78</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="2">
-        <f>$M$53/D36/E36</f>
+        <f t="shared" si="25"/>
         <v>489.527587890625</v>
       </c>
       <c r="D36">
         <v>32</v>
       </c>
       <c r="E36">
-        <f>D36*8</f>
+        <f t="shared" si="26"/>
         <v>256</v>
       </c>
       <c r="F36">
@@ -6885,37 +7131,47 @@
         <v>21.01</v>
       </c>
       <c r="H36" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="31"/>
         <v>681.01</v>
       </c>
       <c r="I36" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J36" s="27">
-        <f>I36/E36</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="L36" s="26"/>
+      <c r="L36" s="6"/>
       <c r="M36" s="6">
         <v>32</v>
       </c>
       <c r="N36" s="6">
-        <f>M36*8</f>
+        <f t="shared" si="28"/>
         <v>256</v>
+      </c>
+      <c r="O36">
+        <v>18</v>
+      </c>
+      <c r="P36">
+        <v>28.038</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="32"/>
+        <v>1108.038</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="26"/>
       <c r="C37" s="2">
-        <f>$M$53/D37/E37</f>
+        <f t="shared" si="25"/>
         <v>122.38189697265625</v>
       </c>
       <c r="D37">
         <v>64</v>
       </c>
       <c r="E37">
-        <f>D37*8</f>
+        <f t="shared" si="26"/>
         <v>512</v>
       </c>
       <c r="I37" s="27"/>
@@ -6925,7 +7181,7 @@
         <v>64</v>
       </c>
       <c r="N37">
-        <f>M37*8</f>
+        <f t="shared" si="28"/>
         <v>512</v>
       </c>
     </row>
@@ -6962,7 +7218,7 @@
         <v>1</v>
       </c>
       <c r="N40">
-        <f>M40*8</f>
+        <f t="shared" ref="N40:N46" si="33">M40*8</f>
         <v>8</v>
       </c>
       <c r="O40">
@@ -7001,7 +7257,7 @@
         <v>2</v>
       </c>
       <c r="N41">
-        <f>M41*8</f>
+        <f t="shared" si="33"/>
         <v>16</v>
       </c>
       <c r="O41">
@@ -7025,7 +7281,7 @@
       </c>
       <c r="F42">
         <f>Q7</f>
-        <v>986.61</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <f>H19</f>
@@ -7035,7 +7291,7 @@
         <v>4</v>
       </c>
       <c r="N42">
-        <f>M42*8</f>
+        <f t="shared" si="33"/>
         <v>32</v>
       </c>
       <c r="O42">
@@ -7059,21 +7315,21 @@
       </c>
       <c r="E43">
         <f>Q8</f>
-        <v>518.11900000000003</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <f>H20</f>
         <v>1264.05</v>
       </c>
       <c r="G43" s="2">
-        <f>Q19</f>
+        <f>T19</f>
         <v>1908.35</v>
       </c>
       <c r="M43">
         <v>8</v>
       </c>
       <c r="N43">
-        <f>M43*8</f>
+        <f t="shared" si="33"/>
         <v>64</v>
       </c>
       <c r="O43">
@@ -7093,14 +7349,14 @@
       </c>
       <c r="D44">
         <f>Q9</f>
-        <v>307.14999999999998</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <f>H21</f>
         <v>677.45</v>
       </c>
       <c r="F44">
-        <f>Q20</f>
+        <f>T20</f>
         <v>990.21</v>
       </c>
       <c r="G44">
@@ -7112,7 +7368,7 @@
         <v>16</v>
       </c>
       <c r="N44">
-        <f>M44*8</f>
+        <f t="shared" si="33"/>
         <v>128</v>
       </c>
       <c r="O44">
@@ -7122,7 +7378,7 @@
         <v>41.149000000000001</v>
       </c>
       <c r="Q44" s="6">
-        <f t="shared" ref="Q44:Q45" si="12">O44*60+P44</f>
+        <f t="shared" ref="Q44:Q45" si="34">O44*60+P44</f>
         <v>1301.1489999999999</v>
       </c>
     </row>
@@ -7135,7 +7391,7 @@
         <v>441</v>
       </c>
       <c r="E45" s="20">
-        <f>Q21</f>
+        <f>T21</f>
         <v>594.84</v>
       </c>
       <c r="F45">
@@ -7151,7 +7407,7 @@
         <v>32</v>
       </c>
       <c r="N45" s="6">
-        <f>M45*8</f>
+        <f t="shared" si="33"/>
         <v>256</v>
       </c>
       <c r="O45">
@@ -7161,7 +7417,7 @@
         <v>22.97</v>
       </c>
       <c r="Q45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="34"/>
         <v>1162.97</v>
       </c>
     </row>
@@ -7170,7 +7426,7 @@
         <v>128</v>
       </c>
       <c r="D46">
-        <f>Q22</f>
+        <f>T22</f>
         <v>499.97</v>
       </c>
       <c r="E46">
@@ -7182,15 +7438,15 @@
         <v>1246.78</v>
       </c>
       <c r="G46">
-        <f>Y21</f>
-        <v>0</v>
+        <f>AB22</f>
+        <v>2078.0300000000002</v>
       </c>
       <c r="L46" s="26"/>
       <c r="M46">
         <v>64</v>
       </c>
       <c r="N46">
-        <f>M46*8</f>
+        <f t="shared" si="33"/>
         <v>512</v>
       </c>
     </row>
@@ -7204,11 +7460,11 @@
       </c>
       <c r="E47">
         <f>Q36</f>
-        <v>0</v>
+        <v>1108.038</v>
       </c>
       <c r="F47">
-        <f>Y22</f>
-        <v>0</v>
+        <f>AB23</f>
+        <v>1546.04</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
@@ -7216,11 +7472,11 @@
         <v>512</v>
       </c>
       <c r="D48">
-        <f>Q34</f>
-        <v>2237.1799999999998</v>
+        <f>AB24</f>
+        <v>0</v>
       </c>
       <c r="E48">
-        <f>Y23</f>
+        <f>AB24</f>
         <v>0</v>
       </c>
       <c r="M48" t="s">
@@ -7255,32 +7511,32 @@
       <c r="M49" s="2">
         <v>195102</v>
       </c>
-      <c r="N49" s="41">
-        <f>$M$49/N$48</f>
+      <c r="N49" s="40">
+        <f t="shared" ref="N49:T49" si="35">$M$49/N$48</f>
         <v>24387.75</v>
       </c>
-      <c r="O49" s="42">
-        <f>$M$49/O$48</f>
+      <c r="O49" s="41">
+        <f t="shared" si="35"/>
         <v>12193.875</v>
       </c>
       <c r="P49" s="27">
-        <f>$M$49/P$48</f>
+        <f t="shared" si="35"/>
         <v>6096.9375</v>
       </c>
       <c r="Q49" s="27">
-        <f>$M$49/Q$48</f>
+        <f t="shared" si="35"/>
         <v>3048.46875</v>
       </c>
       <c r="R49" s="27">
-        <f>$M$49/R$48</f>
+        <f t="shared" si="35"/>
         <v>1524.234375</v>
       </c>
       <c r="S49" s="27">
-        <f>$M$49/S$48</f>
+        <f t="shared" si="35"/>
         <v>762.1171875</v>
       </c>
       <c r="T49" s="2">
-        <f>$M$49/T$48</f>
+        <f t="shared" si="35"/>
         <v>381.05859375</v>
       </c>
     </row>
@@ -7291,32 +7547,32 @@
       <c r="M50" s="2">
         <v>432919</v>
       </c>
-      <c r="N50" s="43">
-        <f>$M$50/N$48</f>
+      <c r="N50" s="42">
+        <f t="shared" ref="N50:T50" si="36">$M$50/N$48</f>
         <v>54114.875</v>
       </c>
-      <c r="O50" s="41">
-        <f>$M$50/O$48</f>
+      <c r="O50" s="40">
+        <f t="shared" si="36"/>
         <v>27057.4375</v>
       </c>
-      <c r="P50" s="42">
-        <f>$M$50/P$48</f>
+      <c r="P50" s="41">
+        <f t="shared" si="36"/>
         <v>13528.71875</v>
       </c>
       <c r="Q50" s="27">
-        <f>$M$50/Q$48</f>
+        <f t="shared" si="36"/>
         <v>6764.359375</v>
       </c>
       <c r="R50" s="27">
-        <f>$M$50/R$48</f>
+        <f t="shared" si="36"/>
         <v>3382.1796875</v>
       </c>
       <c r="S50" s="27">
-        <f>$M$50/S$48</f>
+        <f t="shared" si="36"/>
         <v>1691.08984375</v>
       </c>
       <c r="T50" s="2">
-        <f>$M$50/T$48</f>
+        <f t="shared" si="36"/>
         <v>845.544921875</v>
       </c>
     </row>
@@ -7327,32 +7583,32 @@
       <c r="M51" s="2">
         <v>1017573</v>
       </c>
-      <c r="N51" s="44">
-        <f>$M$51/N$48</f>
+      <c r="N51" s="43">
+        <f t="shared" ref="N51:T51" si="37">$M$51/N$48</f>
         <v>127196.625</v>
       </c>
-      <c r="O51" s="43">
-        <f>$M$51/O$48</f>
+      <c r="O51" s="42">
+        <f t="shared" si="37"/>
         <v>63598.3125</v>
       </c>
-      <c r="P51" s="41">
-        <f>$M$51/P$48</f>
+      <c r="P51" s="40">
+        <f t="shared" si="37"/>
         <v>31799.15625</v>
       </c>
-      <c r="Q51" s="42">
-        <f>$M$51/Q$48</f>
+      <c r="Q51" s="41">
+        <f t="shared" si="37"/>
         <v>15899.578125</v>
       </c>
       <c r="R51" s="27">
-        <f>$M$51/R$48</f>
+        <f t="shared" si="37"/>
         <v>7949.7890625</v>
       </c>
       <c r="S51" s="27">
-        <f>$M$51/S$48</f>
+        <f t="shared" si="37"/>
         <v>3974.89453125</v>
       </c>
       <c r="T51" s="2">
-        <f>$M$51/T$48</f>
+        <f t="shared" si="37"/>
         <v>1987.447265625</v>
       </c>
     </row>
@@ -7364,31 +7620,31 @@
         <v>2037710</v>
       </c>
       <c r="N52" s="27">
-        <f>$M$52/N$48</f>
+        <f t="shared" ref="N52:T52" si="38">$M$52/N$48</f>
         <v>254713.75</v>
       </c>
-      <c r="O52" s="44">
-        <f>$M$52/O$48</f>
+      <c r="O52" s="43">
+        <f t="shared" si="38"/>
         <v>127356.875</v>
       </c>
-      <c r="P52" s="43">
-        <f>$M$52/P$48</f>
+      <c r="P52" s="42">
+        <f t="shared" si="38"/>
         <v>63678.4375</v>
       </c>
-      <c r="Q52" s="41">
-        <f>$M$52/Q$48</f>
+      <c r="Q52" s="40">
+        <f t="shared" si="38"/>
         <v>31839.21875</v>
       </c>
-      <c r="R52" s="42">
-        <f>$M$52/R$48</f>
+      <c r="R52" s="41">
+        <f t="shared" si="38"/>
         <v>15919.609375</v>
       </c>
       <c r="S52" s="27">
-        <f>$M$52/S$48</f>
+        <f t="shared" si="38"/>
         <v>7959.8046875</v>
       </c>
       <c r="T52" s="2">
-        <f>$M$52/T$48</f>
+        <f t="shared" si="38"/>
         <v>3979.90234375</v>
       </c>
     </row>
@@ -7400,31 +7656,31 @@
         <v>4010210</v>
       </c>
       <c r="N53" s="27">
-        <f>$M$53/N$48</f>
+        <f t="shared" ref="N53:T53" si="39">$M$53/N$48</f>
         <v>501276.25</v>
       </c>
       <c r="O53" s="27">
-        <f>$M$53/O$48</f>
+        <f t="shared" si="39"/>
         <v>250638.125</v>
       </c>
-      <c r="P53" s="44">
-        <f>$M$53/P$48</f>
+      <c r="P53" s="43">
+        <f t="shared" si="39"/>
         <v>125319.0625</v>
       </c>
-      <c r="Q53" s="43">
-        <f>$M$53/Q$48</f>
+      <c r="Q53" s="42">
+        <f t="shared" si="39"/>
         <v>62659.53125</v>
       </c>
-      <c r="R53" s="41">
-        <f>$M$53/R$48</f>
+      <c r="R53" s="40">
+        <f t="shared" si="39"/>
         <v>31329.765625</v>
       </c>
-      <c r="S53" s="42">
-        <f>$M$53/S$48</f>
+      <c r="S53" s="41">
+        <f t="shared" si="39"/>
         <v>15664.8828125</v>
       </c>
       <c r="T53" s="25">
-        <f>$M$53/T$48</f>
+        <f t="shared" si="39"/>
         <v>7832.44140625</v>
       </c>
     </row>
@@ -7435,32 +7691,32 @@
       <c r="M54" s="15">
         <v>8101299</v>
       </c>
-      <c r="N54" s="45">
-        <f>$M$54/N$48</f>
+      <c r="N54" s="44">
+        <f t="shared" ref="N54:T54" si="40">$M$54/N$48</f>
         <v>1012662.375</v>
       </c>
-      <c r="O54" s="45">
-        <f>$M$54/O$48</f>
+      <c r="O54" s="44">
+        <f t="shared" si="40"/>
         <v>506331.1875</v>
       </c>
-      <c r="P54" s="45">
-        <f>$M$54/P$48</f>
+      <c r="P54" s="44">
+        <f t="shared" si="40"/>
         <v>253165.59375</v>
       </c>
-      <c r="Q54" s="44">
-        <f>$M$54/Q$48</f>
+      <c r="Q54" s="43">
+        <f t="shared" si="40"/>
         <v>126582.796875</v>
       </c>
-      <c r="R54" s="43">
-        <f>$M$54/R$48</f>
+      <c r="R54" s="42">
+        <f t="shared" si="40"/>
         <v>63291.3984375</v>
       </c>
-      <c r="S54" s="41">
-        <f>$M$54/S$48</f>
+      <c r="S54" s="40">
+        <f t="shared" si="40"/>
         <v>31645.69921875</v>
       </c>
-      <c r="T54" s="42">
-        <f>$M$54/T$48</f>
+      <c r="T54" s="41">
+        <f t="shared" si="40"/>
         <v>15822.849609375</v>
       </c>
     </row>
@@ -7471,32 +7727,32 @@
       <c r="M55" s="15">
         <v>15522778</v>
       </c>
-      <c r="N55" s="45">
-        <f>$M$55/N$48</f>
+      <c r="N55" s="44">
+        <f t="shared" ref="N55:T55" si="41">$M$55/N$48</f>
         <v>1940347.25</v>
       </c>
-      <c r="O55" s="45">
-        <f>$M$55/O$48</f>
+      <c r="O55" s="44">
+        <f t="shared" si="41"/>
         <v>970173.625</v>
       </c>
-      <c r="P55" s="45">
-        <f>$M$55/P$48</f>
+      <c r="P55" s="44">
+        <f t="shared" si="41"/>
         <v>485086.8125</v>
       </c>
-      <c r="Q55" s="45">
-        <f>$M$55/Q$48</f>
+      <c r="Q55" s="44">
+        <f t="shared" si="41"/>
         <v>242543.40625</v>
       </c>
-      <c r="R55" s="44">
-        <f>$M$55/R$48</f>
+      <c r="R55" s="43">
+        <f t="shared" si="41"/>
         <v>121271.703125</v>
       </c>
-      <c r="S55" s="43">
-        <f>$M$55/S$48</f>
+      <c r="S55" s="42">
+        <f t="shared" si="41"/>
         <v>60635.8515625</v>
       </c>
-      <c r="T55" s="41">
-        <f>$M$55/T$48</f>
+      <c r="T55" s="40">
+        <f t="shared" si="41"/>
         <v>30317.92578125</v>
       </c>
     </row>
@@ -7568,9 +7824,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="R4:S4"/>
+  <mergeCells count="4">
     <mergeCell ref="T4:U4"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="Z4:AA4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -7580,34 +7838,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:V14"/>
+  <dimension ref="B3:AA14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>42</v>
       </c>
@@ -7626,7 +7884,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>43</v>
@@ -7656,7 +7914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -7684,8 +7942,20 @@
       <c r="L8">
         <v>40.08</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>9.9</v>
+      </c>
+      <c r="P8">
+        <v>9</v>
+      </c>
+      <c r="Q8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2</v>
       </c>
@@ -7702,7 +7972,7 @@
         <v>38.21</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>4</v>
       </c>
@@ -7743,7 +8013,7 @@
         <v>44.93</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -7772,7 +8042,7 @@
         <v>48.64</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>16</v>
       </c>
@@ -7825,7 +8095,7 @@
         <v>48.03</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>32</v>
       </c>
@@ -7865,8 +8135,32 @@
       <c r="Q13">
         <v>6.01</v>
       </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <v>8</v>
+      </c>
+      <c r="T13">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+      <c r="V13">
+        <v>29.94</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>52.39</v>
+      </c>
+      <c r="Z13">
+        <v>9</v>
+      </c>
+      <c r="AA13">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Added pipe05 serial run
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="68">
   <si>
     <t>pipe01</t>
   </si>
@@ -219,13 +219,13 @@
     <t>check the iterative solvers</t>
   </si>
   <si>
-    <t>calculate</t>
-  </si>
-  <si>
     <t>SizeUp</t>
   </si>
   <si>
     <t>not enough memory on siet0003</t>
+  </si>
+  <si>
+    <t>running</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -530,7 +530,6 @@
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -541,16 +540,16 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -670,6 +669,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1203,11 +1203,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209669840"/>
-        <c:axId val="130707296"/>
+        <c:axId val="208370616"/>
+        <c:axId val="208371400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209669840"/>
+        <c:axId val="208370616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,7 +1225,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="130707296"/>
+        <c:crossAx val="208371400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1233,7 +1233,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130707296"/>
+        <c:axId val="208371400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1258,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209669840"/>
+        <c:crossAx val="208370616"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1271,6 +1271,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1612,11 +1613,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209783576"/>
-        <c:axId val="209346000"/>
+        <c:axId val="208372184"/>
+        <c:axId val="208372576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209783576"/>
+        <c:axId val="208372184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1635,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209346000"/>
+        <c:crossAx val="208372576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1642,7 +1643,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209346000"/>
+        <c:axId val="208372576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1668,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="209783576"/>
+        <c:crossAx val="208372184"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1680,6 +1681,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1739,6 +1741,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2109,11 +2112,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="210078168"/>
-        <c:axId val="210045104"/>
+        <c:axId val="208373360"/>
+        <c:axId val="208373752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="210078168"/>
+        <c:axId val="208373360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2134,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210045104"/>
+        <c:crossAx val="208373752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2139,7 +2142,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210045104"/>
+        <c:axId val="208373752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2164,7 +2167,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210078168"/>
+        <c:crossAx val="208373360"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2177,6 +2180,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2236,6 +2240,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2573,7 +2578,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SimplyHPC A8'!$R$3</c:f>
+              <c:f>'SimplyHPC A8'!$O$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2649,10 +2654,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SimplyHPC A8'!$Q$7:$Q$12</c:f>
+              <c:f>'SimplyHPC A8'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2776,11 +2784,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="210583448"/>
-        <c:axId val="210583840"/>
+        <c:axId val="208376496"/>
+        <c:axId val="210550712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="210583448"/>
+        <c:axId val="208376496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2806,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210583840"/>
+        <c:crossAx val="210550712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2806,7 +2814,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210583840"/>
+        <c:axId val="210550712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +2839,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210583448"/>
+        <c:crossAx val="208376496"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2844,6 +2852,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2903,6 +2912,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3084,11 +3094,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="210586584"/>
-        <c:axId val="210586976"/>
+        <c:axId val="210551496"/>
+        <c:axId val="210551888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="210586584"/>
+        <c:axId val="210551496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3106,7 +3116,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210586976"/>
+        <c:crossAx val="210551888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3114,7 +3124,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210586976"/>
+        <c:axId val="210551888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3139,7 +3149,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="210586584"/>
+        <c:crossAx val="210551496"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3598,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3619,10 +3629,10 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="57" t="s">
+      <c r="R3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="57"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -4114,10 +4124,10 @@
       <c r="P12" t="s">
         <v>60</v>
       </c>
-      <c r="R12" s="57" t="s">
+      <c r="R12" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="S12" s="57"/>
+      <c r="S12" s="58"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -4660,7 +4670,7 @@
         <v>1</v>
       </c>
       <c r="R23" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T23" s="6">
         <v>1</v>
@@ -5510,8 +5520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5534,47 +5544,41 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>20</v>
-      </c>
-      <c r="B1">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="6"/>
+      <c r="O3" s="46" t="s">
+        <v>6</v>
+      </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="47" t="s">
-        <v>6</v>
-      </c>
+      <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="55"/>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
       <c r="S4" s="55"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="54" t="s">
+      <c r="T4" s="6"/>
+      <c r="U4" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="59" t="s">
+      <c r="V4" s="53"/>
+      <c r="W4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="59"/>
+      <c r="X4" s="59"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -5602,42 +5606,39 @@
         <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+      <c r="O5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="R5" s="6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="W5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="48" t="s">
+      <c r="U5" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="Y5" s="48" t="s">
+      <c r="V5" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="Z5" s="36" t="s">
+      <c r="W5" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="AA5" s="36" t="s">
+      <c r="X5" s="36" t="s">
         <v>48</v>
       </c>
     </row>
@@ -5664,44 +5665,41 @@
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="2"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="2">
-        <f>$M$50/S6/T6</f>
+      <c r="O6" s="2">
+        <f>$M$50/P6/Q6</f>
         <v>432919</v>
       </c>
+      <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>109</v>
+      </c>
       <c r="S6" s="6">
-        <v>1</v>
+        <v>55.97</v>
       </c>
       <c r="T6" s="6">
-        <v>1</v>
-      </c>
-      <c r="U6" s="6">
-        <v>109</v>
-      </c>
-      <c r="V6" s="6">
-        <v>55.97</v>
-      </c>
-      <c r="W6" s="6">
-        <f t="shared" ref="W6:W12" si="1">U6*60+V6</f>
+        <f>R6*60+S6</f>
         <v>6595.97</v>
       </c>
-      <c r="X6" s="49"/>
-      <c r="Y6" s="49"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="36"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C13" si="2">$M$49/E7</f>
+        <f t="shared" ref="C7:C13" si="1">$M$49/E7</f>
         <v>24387.75</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E13" si="3">D7*8</f>
+        <f t="shared" ref="E7:E13" si="2">D7*8</f>
         <v>8</v>
       </c>
       <c r="F7">
@@ -5722,58 +5720,62 @@
         <f>I7/E7</f>
         <v>0.13381537242472266</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="2">
-        <f>$M$50/S7/T7</f>
+      <c r="K7" s="57">
+        <f>C7/$C$6*$H$6/H7</f>
+        <v>0.13381537242472266</v>
+      </c>
+      <c r="L7" s="57">
+        <f t="shared" ref="L7:L12" si="3">K7/E7</f>
+        <v>1.6726921553090333E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <f>$M$50/P7/Q7</f>
         <v>54114.875</v>
       </c>
+      <c r="P7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6">
+        <f>P7*8</f>
+        <v>8</v>
+      </c>
+      <c r="R7" s="6">
+        <v>16</v>
+      </c>
       <c r="S7" s="6">
-        <v>1</v>
+        <v>26.61</v>
       </c>
       <c r="T7" s="6">
-        <f t="shared" ref="T7:T12" si="4">S7*8</f>
-        <v>8</v>
-      </c>
-      <c r="U7" s="6">
-        <v>16</v>
-      </c>
-      <c r="V7" s="6">
-        <v>26.61</v>
-      </c>
-      <c r="W7" s="6">
-        <f t="shared" si="1"/>
+        <f>R7*60+S7</f>
         <v>986.61</v>
       </c>
-      <c r="X7" s="49">
-        <f>$W$6/W7</f>
+      <c r="U7" s="48">
+        <f>$T$6/T7</f>
         <v>6.6854886936074029</v>
       </c>
-      <c r="Y7" s="49">
-        <f t="shared" ref="Y7:Y12" si="5">X7/T7</f>
+      <c r="V7" s="48">
+        <f>U7/Q7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="Z7" s="60">
-        <f>R7/$R$6*$W$6/W7</f>
+      <c r="W7" s="57">
+        <f>O7/$O$6*$T$6/T7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="AA7" s="51">
-        <f t="shared" ref="AA7:AA12" si="6">Z7/T7</f>
+      <c r="X7" s="50">
+        <f>W7/Q7</f>
         <v>0.10446076083761567</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12193.875</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="F8">
@@ -5787,65 +5789,69 @@
         <v>10.47</v>
       </c>
       <c r="I8" s="27">
-        <f t="shared" ref="I8:I12" si="7">$H$6/H8</f>
+        <f t="shared" ref="I8:I12" si="4">$H$6/H8</f>
         <v>1.2903533906399234</v>
       </c>
       <c r="J8" s="27">
-        <f t="shared" ref="J8:J12" si="8">I8/E8</f>
+        <f t="shared" ref="J8:J12" si="5">I8/E8</f>
         <v>8.0647086914995211E-2</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="2">
-        <f t="shared" ref="R8:R13" si="9">$M$50/T8</f>
+      <c r="K8" s="57">
+        <f t="shared" ref="K8:K11" si="6">C8/$C$6*$H$6/H8</f>
+        <v>8.0647086914995211E-2</v>
+      </c>
+      <c r="L8" s="57">
+        <f t="shared" si="3"/>
+        <v>5.0404429321872007E-3</v>
+      </c>
+      <c r="O8" s="2">
+        <f>$M$50/Q8</f>
         <v>27057.4375</v>
       </c>
+      <c r="P8" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>P8*8</f>
+        <v>16</v>
+      </c>
+      <c r="R8" s="6">
+        <v>8</v>
+      </c>
       <c r="S8" s="6">
-        <v>2</v>
+        <v>38.119</v>
       </c>
       <c r="T8" s="6">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="U8" s="6">
-        <v>8</v>
-      </c>
-      <c r="V8" s="6">
-        <v>38.119</v>
-      </c>
-      <c r="W8" s="6">
-        <f t="shared" si="1"/>
+        <f>R8*60+S8</f>
         <v>518.11900000000003</v>
       </c>
-      <c r="X8" s="49">
-        <f t="shared" ref="X8:X12" si="10">$W$6/W8</f>
+      <c r="U8" s="48">
+        <f>$T$6/T8</f>
         <v>12.730608219347292</v>
       </c>
-      <c r="Y8" s="49">
-        <f t="shared" si="5"/>
+      <c r="V8" s="48">
+        <f>U8/Q8</f>
         <v>0.79566301370920578</v>
       </c>
-      <c r="Z8" s="60">
-        <f t="shared" ref="Z8:Z12" si="11">R8/$R$6*$W$6/W8</f>
+      <c r="W8" s="57">
+        <f>O8/$O$6*$T$6/T8</f>
         <v>0.79566301370920578</v>
       </c>
-      <c r="AA8" s="51">
-        <f t="shared" si="6"/>
+      <c r="X8" s="50">
+        <f>W8/Q8</f>
         <v>4.9728938356825361E-2</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6096.9375</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="F9">
@@ -5859,65 +5865,69 @@
         <v>11.82</v>
       </c>
       <c r="I9" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1.1429780033840946</v>
       </c>
       <c r="J9" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.5718062605752957E-2</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="2">
-        <f t="shared" si="9"/>
+      <c r="K9" s="57">
+        <f t="shared" si="6"/>
+        <v>3.5718062605752957E-2</v>
+      </c>
+      <c r="L9" s="57">
+        <f t="shared" si="3"/>
+        <v>1.1161894564297799E-3</v>
+      </c>
+      <c r="O9" s="2">
+        <f>$M$50/Q9</f>
         <v>13528.71875</v>
       </c>
+      <c r="P9" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>P9*8</f>
+        <v>32</v>
+      </c>
+      <c r="R9" s="6">
+        <v>5</v>
+      </c>
       <c r="S9" s="6">
-        <v>4</v>
+        <v>7.15</v>
       </c>
       <c r="T9" s="6">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="U9" s="6">
-        <v>5</v>
-      </c>
-      <c r="V9" s="6">
-        <v>7.15</v>
-      </c>
-      <c r="W9" s="6">
-        <f t="shared" si="1"/>
+        <f>R9*60+S9</f>
         <v>307.14999999999998</v>
       </c>
-      <c r="X9" s="49">
-        <f t="shared" si="10"/>
+      <c r="U9" s="48">
+        <f>$T$6/T9</f>
         <v>21.474751749959307</v>
       </c>
-      <c r="Y9" s="49">
-        <f t="shared" si="5"/>
+      <c r="V9" s="48">
+        <f>U9/Q9</f>
         <v>0.67108599218622833</v>
       </c>
-      <c r="Z9" s="60">
-        <f t="shared" si="11"/>
+      <c r="W9" s="57">
+        <f>O9/$O$6*$T$6/T9</f>
         <v>0.67108599218622833</v>
       </c>
-      <c r="AA9" s="51">
-        <f t="shared" si="6"/>
+      <c r="X9" s="50">
+        <f>W9/Q9</f>
         <v>2.0971437255819635E-2</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3048.46875</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="F10">
@@ -5931,65 +5941,69 @@
         <v>15.96</v>
       </c>
       <c r="I10" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.84649122807017541</v>
       </c>
       <c r="J10" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.3226425438596491E-2</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="2">
-        <f t="shared" si="9"/>
+      <c r="K10" s="57">
+        <f t="shared" si="6"/>
+        <v>1.3226425438596491E-2</v>
+      </c>
+      <c r="L10" s="57">
+        <f t="shared" si="3"/>
+        <v>2.0666289747807017E-4</v>
+      </c>
+      <c r="O10" s="2">
+        <f>$M$50/Q10</f>
         <v>6764.359375</v>
       </c>
+      <c r="P10" s="6">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="6">
+        <f>P10*8</f>
+        <v>64</v>
+      </c>
+      <c r="R10" s="6">
+        <v>4</v>
+      </c>
       <c r="S10" s="6">
-        <v>8</v>
+        <v>12.13</v>
       </c>
       <c r="T10" s="6">
-        <f t="shared" si="4"/>
-        <v>64</v>
-      </c>
-      <c r="U10" s="6">
-        <v>4</v>
-      </c>
-      <c r="V10" s="6">
-        <v>12.13</v>
-      </c>
-      <c r="W10" s="6">
-        <f t="shared" si="1"/>
+        <f>R10*60+S10</f>
         <v>252.13</v>
       </c>
-      <c r="X10" s="49">
-        <f t="shared" si="10"/>
+      <c r="U10" s="48">
+        <f>$T$6/T10</f>
         <v>26.160988379010828</v>
       </c>
-      <c r="Y10" s="50">
-        <f t="shared" si="5"/>
+      <c r="V10" s="49">
+        <f>U10/Q10</f>
         <v>0.40876544342204418</v>
       </c>
-      <c r="Z10" s="60">
-        <f t="shared" si="11"/>
+      <c r="W10" s="57">
+        <f>O10/$O$6*$T$6/T10</f>
         <v>0.40876544342204418</v>
       </c>
-      <c r="AA10" s="51">
-        <f t="shared" si="6"/>
+      <c r="X10" s="50">
+        <f>W10/Q10</f>
         <v>6.3869600534694404E-3</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1524.234375</v>
       </c>
       <c r="D11">
         <v>16</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="F11">
@@ -6003,67 +6017,71 @@
         <v>25.34</v>
       </c>
       <c r="I11" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.53314917127071826</v>
       </c>
       <c r="J11" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>4.1652279005524864E-3</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="K11" s="57">
+        <f t="shared" si="6"/>
+        <v>4.1652279005524864E-3</v>
+      </c>
+      <c r="L11" s="57">
+        <f t="shared" si="3"/>
+        <v>3.25408429730663E-5</v>
+      </c>
       <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="2">
-        <f t="shared" si="9"/>
+      <c r="O11" s="2">
+        <f>$M$50/Q11</f>
         <v>3382.1796875</v>
       </c>
+      <c r="P11" s="6">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="6">
+        <f>P11*8</f>
+        <v>128</v>
+      </c>
+      <c r="R11" s="6">
+        <v>3</v>
+      </c>
       <c r="S11" s="6">
-        <v>16</v>
+        <v>36.96</v>
       </c>
       <c r="T11" s="6">
-        <f t="shared" si="4"/>
-        <v>128</v>
-      </c>
-      <c r="U11" s="6">
-        <v>3</v>
-      </c>
-      <c r="V11" s="6">
-        <v>36.96</v>
-      </c>
-      <c r="W11" s="6">
-        <f t="shared" si="1"/>
+        <f>R11*60+S11</f>
         <v>216.96</v>
       </c>
-      <c r="X11" s="49">
-        <f t="shared" si="10"/>
+      <c r="U11" s="48">
+        <f>$T$6/T11</f>
         <v>30.40177912979351</v>
       </c>
-      <c r="Y11" s="49">
-        <f t="shared" si="5"/>
+      <c r="V11" s="48">
+        <f>U11/Q11</f>
         <v>0.2375138994515118</v>
       </c>
-      <c r="Z11" s="60">
-        <f t="shared" si="11"/>
+      <c r="W11" s="57">
+        <f>O11/$O$6*$T$6/T11</f>
         <v>0.2375138994515118</v>
       </c>
-      <c r="AA11" s="51">
-        <f t="shared" si="6"/>
+      <c r="X11" s="50">
+        <f>W11/Q11</f>
         <v>1.8555773394649359E-3</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="C12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>762.1171875</v>
       </c>
       <c r="D12">
         <v>32</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="F12">
@@ -6077,97 +6095,96 @@
         <v>44.57</v>
       </c>
       <c r="I12" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.303118689701593</v>
       </c>
       <c r="J12" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.1840573816468477E-3</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="2"/>
+      <c r="K12" s="57">
+        <f>C12/$C$6*$H$6/H12</f>
+        <v>1.1840573816468477E-3</v>
+      </c>
+      <c r="L12" s="57">
+        <f t="shared" si="3"/>
+        <v>4.6252241470579987E-6</v>
+      </c>
       <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="2">
-        <f t="shared" si="9"/>
+      <c r="O12" s="2">
+        <f>$M$50/Q12</f>
         <v>1691.08984375</v>
       </c>
+      <c r="P12" s="6">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="6">
+        <f>P12*8</f>
+        <v>256</v>
+      </c>
+      <c r="R12" s="6">
+        <v>4</v>
+      </c>
       <c r="S12" s="6">
-        <v>32</v>
+        <v>56.72</v>
       </c>
       <c r="T12" s="6">
-        <f t="shared" si="4"/>
-        <v>256</v>
-      </c>
-      <c r="U12" s="6">
-        <v>4</v>
-      </c>
-      <c r="V12" s="6">
-        <v>56.72</v>
-      </c>
-      <c r="W12" s="6">
-        <f t="shared" si="1"/>
+        <f>R12*60+S12</f>
         <v>296.72000000000003</v>
       </c>
-      <c r="X12" s="49">
-        <f t="shared" si="10"/>
+      <c r="U12" s="48">
+        <f>$T$6/T12</f>
         <v>22.229610407117821</v>
       </c>
-      <c r="Y12" s="49">
-        <f t="shared" si="5"/>
+      <c r="V12" s="48">
+        <f>U12/Q12</f>
         <v>8.683441565280399E-2</v>
       </c>
-      <c r="Z12" s="60">
-        <f t="shared" si="11"/>
+      <c r="W12" s="57">
+        <f>O12/$O$6*$T$6/T12</f>
         <v>8.683441565280399E-2</v>
       </c>
-      <c r="AA12" s="51">
-        <f t="shared" si="6"/>
+      <c r="X12" s="50">
+        <f>W12/Q12</f>
         <v>3.3919693614376558E-4</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="C13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>381.05859375</v>
       </c>
       <c r="D13">
         <v>64</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="K13" s="26"/>
       <c r="L13" s="2"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="2">
-        <f t="shared" si="9"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="2">
+        <f t="shared" ref="O13" si="7">$M$50/Q13</f>
         <v>845.544921875</v>
       </c>
-      <c r="S13" s="6">
+      <c r="P13" s="6">
         <v>64</v>
       </c>
-      <c r="T13" s="6">
-        <f t="shared" ref="T13" si="12">S13*8</f>
+      <c r="Q13" s="6">
+        <f t="shared" ref="Q13" si="8">P13*8</f>
         <v>512</v>
       </c>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="O14" s="47" t="s">
+      <c r="O14" s="46" t="s">
         <v>10</v>
       </c>
       <c r="W14" s="6" t="s">
@@ -6180,7 +6197,7 @@
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="46" t="s">
         <v>9</v>
       </c>
       <c r="W15" s="6"/>
@@ -6191,14 +6208,14 @@
       <c r="AB15" s="6"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="I16" s="57" t="s">
+      <c r="I16" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57" t="s">
+      <c r="J16" s="58"/>
+      <c r="K16" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="L16" s="57"/>
+      <c r="L16" s="58"/>
       <c r="P16" t="s">
         <v>17</v>
       </c>
@@ -6303,18 +6320,18 @@
         <v>8.94</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" ref="H18:H23" si="13">F18*60+G18</f>
+        <f t="shared" ref="H18:H23" si="9">F18*60+G18</f>
         <v>17708.939999999999</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" ref="O18:O24" si="14">$M$52/Q18</f>
+        <f t="shared" ref="O18:O24" si="10">$M$52/Q18</f>
         <v>254713.75</v>
       </c>
       <c r="P18">
         <v>1</v>
       </c>
       <c r="Q18">
-        <f t="shared" ref="Q18:Q24" si="15">P18*8</f>
+        <f t="shared" ref="Q18:Q24" si="11">P18*8</f>
         <v>8</v>
       </c>
       <c r="R18">
@@ -6332,7 +6349,7 @@
         <v>1</v>
       </c>
       <c r="Y18" s="6">
-        <f t="shared" ref="Y18:Y24" si="16">X18*8</f>
+        <f t="shared" ref="Y18:Y24" si="12">X18*8</f>
         <v>8</v>
       </c>
       <c r="Z18">
@@ -6342,20 +6359,20 @@
         <v>53.48</v>
       </c>
       <c r="AB18" s="6">
-        <f t="shared" ref="AB18:AB23" si="17">Z18*60+AA18</f>
+        <f t="shared" ref="AB18:AB23" si="13">Z18*60+AA18</f>
         <v>39473.480000000003</v>
       </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
-        <f t="shared" ref="C19:C25" si="18">$M$51/E19</f>
+        <f t="shared" ref="C19:C25" si="14">$M$51/E19</f>
         <v>127196.625</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19:E25" si="19">D19*8</f>
+        <f t="shared" ref="E19:E25" si="15">D19*8</f>
         <v>8</v>
       </c>
       <c r="F19">
@@ -6364,31 +6381,35 @@
       <c r="G19">
         <v>18.350000000000001</v>
       </c>
-      <c r="H19" s="52">
-        <f t="shared" si="13"/>
+      <c r="H19" s="51">
+        <f t="shared" si="9"/>
         <v>2478.35</v>
       </c>
-      <c r="I19" s="53">
+      <c r="I19" s="52">
         <f>$H$18/H19</f>
         <v>7.1454556458934366</v>
       </c>
       <c r="J19" s="27">
-        <f t="shared" ref="J19:J24" si="20">I19/E19</f>
+        <f t="shared" ref="J19:J24" si="16">I19/E19</f>
         <v>0.89318195573667958</v>
       </c>
       <c r="K19" s="2">
-        <f>C19/$C$18</f>
-        <v>0.125</v>
+        <f>C19/$C$18*$H$18/H19</f>
+        <v>0.89318195573667958</v>
+      </c>
+      <c r="L19" s="2">
+        <f>K19/E19</f>
+        <v>0.11164774446708495</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>127356.875</v>
       </c>
       <c r="P19">
         <v>2</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="R19">
@@ -6406,7 +6427,7 @@
         <v>2</v>
       </c>
       <c r="Y19" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="Z19" s="6">
@@ -6416,20 +6437,20 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="AB19" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>17044.89</v>
       </c>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>63598.3125</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
       <c r="F20">
@@ -6439,30 +6460,34 @@
         <v>4.05</v>
       </c>
       <c r="H20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>1264.05</v>
       </c>
-      <c r="I20" s="53">
-        <f t="shared" ref="I20:I24" si="21">$H$18/H20</f>
+      <c r="I20" s="52">
+        <f t="shared" ref="I20:I24" si="17">$H$18/H20</f>
         <v>14.009683161267354</v>
       </c>
       <c r="J20" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>0.87560519757920963</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" ref="K20:K24" si="22">C20/$C$18</f>
-        <v>6.25E-2</v>
+        <f t="shared" ref="K20:K24" si="18">C20/$C$18*$H$18/H20</f>
+        <v>0.87560519757920963</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" ref="L20:L24" si="19">K20/E20</f>
+        <v>5.4725324848700602E-2</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>63678.4375</v>
       </c>
       <c r="P20">
         <v>4</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="R20">
@@ -6480,7 +6505,7 @@
         <v>4</v>
       </c>
       <c r="Y20" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="Z20" s="6">
@@ -6490,20 +6515,20 @@
         <v>5.21</v>
       </c>
       <c r="AB20" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>4385.21</v>
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>31799.15625</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="E21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>32</v>
       </c>
       <c r="F21">
@@ -6513,30 +6538,34 @@
         <v>17.45</v>
       </c>
       <c r="H21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>677.45</v>
       </c>
-      <c r="I21" s="53">
-        <f t="shared" si="21"/>
+      <c r="I21" s="52">
+        <f t="shared" si="17"/>
         <v>26.140586021108565</v>
       </c>
       <c r="J21" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>0.81689331315964264</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="22"/>
-        <v>3.125E-2</v>
+        <f t="shared" si="18"/>
+        <v>0.81689331315964264</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="19"/>
+        <v>2.5527916036238833E-2</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>31839.21875</v>
       </c>
       <c r="P21">
         <v>8</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="R21">
@@ -6554,7 +6583,7 @@
         <v>8</v>
       </c>
       <c r="Y21" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>64</v>
       </c>
       <c r="Z21">
@@ -6564,20 +6593,20 @@
         <v>12.01</v>
       </c>
       <c r="AB21" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>3912.01</v>
       </c>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>15899.578125</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
       <c r="E22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>64</v>
       </c>
       <c r="F22">
@@ -6587,30 +6616,34 @@
         <v>21</v>
       </c>
       <c r="H22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>441</v>
       </c>
-      <c r="I22" s="53">
-        <f t="shared" si="21"/>
+      <c r="I22" s="52">
+        <f t="shared" si="17"/>
         <v>40.15632653061224</v>
       </c>
       <c r="J22" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>0.62744260204081626</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="22"/>
-        <v>1.5625E-2</v>
+        <f t="shared" si="18"/>
+        <v>0.62744260204081626</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="19"/>
+        <v>9.803790656887754E-3</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>15919.609375</v>
       </c>
       <c r="P22">
         <v>16</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>128</v>
       </c>
       <c r="R22">
@@ -6620,7 +6653,7 @@
         <v>19.97</v>
       </c>
       <c r="T22" s="6">
-        <f t="shared" ref="T22:T23" si="23">R22*60+S22</f>
+        <f t="shared" ref="T22:T23" si="20">R22*60+S22</f>
         <v>499.97</v>
       </c>
       <c r="W22" s="6"/>
@@ -6628,7 +6661,7 @@
         <v>16</v>
       </c>
       <c r="Y22" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>128</v>
       </c>
       <c r="Z22" s="6">
@@ -6638,20 +6671,20 @@
         <v>38.03</v>
       </c>
       <c r="AB22" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>2078.0300000000002</v>
       </c>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>7949.7890625</v>
       </c>
       <c r="D23">
         <v>16</v>
       </c>
       <c r="E23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>128</v>
       </c>
       <c r="F23">
@@ -6661,31 +6694,35 @@
         <v>23.6</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>383.6</v>
       </c>
-      <c r="I23" s="53">
-        <f t="shared" si="21"/>
+      <c r="I23" s="52">
+        <f t="shared" si="17"/>
         <v>46.165119916579762</v>
       </c>
       <c r="J23" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>0.36066499934827939</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="22"/>
-        <v>7.8125E-3</v>
+        <f t="shared" si="18"/>
+        <v>0.36066499934827939</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="19"/>
+        <v>2.8176953074084327E-3</v>
       </c>
       <c r="N23" s="6"/>
       <c r="O23" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>7959.8046875</v>
       </c>
       <c r="P23">
         <v>32</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>256</v>
       </c>
       <c r="R23">
@@ -6695,7 +6732,7 @@
         <v>36.68</v>
       </c>
       <c r="T23" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>516.67999999999995</v>
       </c>
       <c r="W23" s="6"/>
@@ -6703,7 +6740,7 @@
         <v>32</v>
       </c>
       <c r="Y23" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>256</v>
       </c>
       <c r="Z23" s="6">
@@ -6713,21 +6750,21 @@
         <v>46.04</v>
       </c>
       <c r="AB23" s="42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1546.04</v>
       </c>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>3974.89453125</v>
       </c>
       <c r="D24">
         <v>32</v>
       </c>
       <c r="E24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>256</v>
       </c>
       <c r="F24">
@@ -6737,31 +6774,35 @@
         <v>50.21</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" ref="H24" si="24">F24*60+G24</f>
+        <f t="shared" ref="H24" si="21">F24*60+G24</f>
         <v>410.21</v>
       </c>
-      <c r="I24" s="53">
-        <f t="shared" si="21"/>
+      <c r="I24" s="52">
+        <f t="shared" si="17"/>
         <v>43.170424904317301</v>
       </c>
       <c r="J24" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>0.16863447228248946</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="22"/>
-        <v>3.90625E-3</v>
+        <f t="shared" si="18"/>
+        <v>0.16863447228248946</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="19"/>
+        <v>6.5872840735347444E-4</v>
       </c>
       <c r="N24" s="26"/>
       <c r="O24" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>3979.90234375</v>
       </c>
       <c r="P24">
         <v>64</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>512</v>
       </c>
       <c r="W24" s="26"/>
@@ -6769,21 +6810,21 @@
         <v>64</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>512</v>
       </c>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B25" s="26"/>
       <c r="C25" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>1987.447265625</v>
       </c>
       <c r="D25">
         <v>64</v>
       </c>
       <c r="E25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>512</v>
       </c>
       <c r="U25" s="2"/>
@@ -6792,10 +6833,10 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="C27" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="L27" t="s">
+      <c r="O27" t="s">
         <v>50</v>
       </c>
       <c r="U27" s="2"/>
@@ -6828,53 +6869,63 @@
       <c r="J29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="P29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N29" s="6" t="s">
+      <c r="Q29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O29" s="6" t="s">
+      <c r="R29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="T29" s="6" t="s">
         <v>21</v>
       </c>
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B30" s="46" t="s">
-        <v>65</v>
-      </c>
+      <c r="B30" s="6"/>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="H30" s="6"/>
-      <c r="L30" s="26"/>
-      <c r="M30">
+      <c r="F30">
+        <f>19*60+13</f>
+        <v>1153</v>
+      </c>
+      <c r="G30">
+        <v>53.45</v>
+      </c>
+      <c r="H30" s="6">
+        <f>F30*60+G30</f>
+        <v>69233.45</v>
+      </c>
+      <c r="O30" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="P30">
         <v>1</v>
       </c>
-      <c r="N30">
+      <c r="Q30">
         <v>1</v>
       </c>
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
-        <f t="shared" ref="C31:C37" si="25">$M$53/D31/E31</f>
+        <f t="shared" ref="C31:C37" si="22">$M$53/D31/E31</f>
         <v>501276.25</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <f t="shared" ref="E31:E37" si="26">D31*8</f>
+        <f t="shared" ref="E31:E37" si="23">D31*8</f>
         <v>8</v>
       </c>
       <c r="F31">
@@ -6889,42 +6940,42 @@
       </c>
       <c r="I31" s="27">
         <f>$H$30/H31</f>
-        <v>0</v>
+        <v>7.5381242623393474</v>
       </c>
       <c r="J31" s="27">
-        <f t="shared" ref="J31:J36" si="27">I31/E31</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="6">
+        <f t="shared" ref="J31:J36" si="24">I31/E31</f>
+        <v>0.94226553279241843</v>
+      </c>
+      <c r="P31" s="6">
         <v>1</v>
       </c>
-      <c r="N31" s="6">
-        <f t="shared" ref="N31:N37" si="28">M31*8</f>
+      <c r="Q31" s="6">
+        <f t="shared" ref="Q31:Q37" si="25">P31*8</f>
         <v>8</v>
       </c>
-      <c r="O31">
+      <c r="R31">
         <f>5*60+48</f>
         <v>348</v>
       </c>
-      <c r="P31">
+      <c r="S31">
         <v>11.82</v>
       </c>
-      <c r="Q31" s="6">
-        <f t="shared" ref="Q31:Q33" si="29">O31*60+P31</f>
+      <c r="T31" s="6">
+        <f t="shared" ref="T31:T33" si="26">R31*60+S31</f>
         <v>20891.82</v>
       </c>
       <c r="U31" s="15"/>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>125319.0625</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>16</v>
       </c>
       <c r="F32">
@@ -6939,41 +6990,41 @@
       </c>
       <c r="I32" s="27">
         <f>$H$30/H32</f>
-        <v>0</v>
+        <v>15.843257282775351</v>
       </c>
       <c r="J32" s="27">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="6">
+        <f t="shared" si="24"/>
+        <v>0.99020358017345944</v>
+      </c>
+      <c r="P32" s="6">
         <v>2</v>
       </c>
-      <c r="N32" s="6">
-        <f t="shared" si="28"/>
+      <c r="Q32" s="6">
+        <f t="shared" si="25"/>
         <v>16</v>
       </c>
-      <c r="O32">
+      <c r="R32">
         <v>158</v>
       </c>
-      <c r="P32">
+      <c r="S32">
         <v>0.92</v>
       </c>
-      <c r="Q32" s="6">
-        <f t="shared" si="29"/>
+      <c r="T32" s="6">
+        <f t="shared" si="26"/>
         <v>9480.92</v>
       </c>
       <c r="U32" s="15"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>31329.765625</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>32</v>
       </c>
       <c r="F33">
@@ -6988,41 +7039,41 @@
       </c>
       <c r="I33" s="27">
         <f>$H$30/H33</f>
-        <v>0</v>
+        <v>32.587654681270678</v>
       </c>
       <c r="J33" s="27">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6">
+        <f t="shared" si="24"/>
+        <v>1.0183642087897087</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6">
         <v>4</v>
       </c>
-      <c r="N33" s="6">
-        <f t="shared" si="28"/>
+      <c r="Q33" s="6">
+        <f t="shared" si="25"/>
         <v>32</v>
       </c>
-      <c r="O33">
+      <c r="R33">
         <v>75</v>
       </c>
-      <c r="P33">
+      <c r="S33">
         <v>58.41</v>
       </c>
-      <c r="Q33" s="6">
-        <f t="shared" si="29"/>
+      <c r="T33" s="6">
+        <f t="shared" si="26"/>
         <v>4558.41</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>7832.44140625</v>
       </c>
       <c r="D34">
         <v>8</v>
       </c>
       <c r="E34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>64</v>
       </c>
       <c r="F34">
@@ -7036,42 +7087,42 @@
         <v>1216.44</v>
       </c>
       <c r="I34" s="27">
-        <f t="shared" ref="I34:I36" si="30">$H$30/H34</f>
-        <v>0</v>
+        <f t="shared" ref="I34:I36" si="27">$H$30/H34</f>
+        <v>56.914808786294429</v>
       </c>
       <c r="J34" s="27">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6">
+        <f t="shared" si="24"/>
+        <v>0.88929388728585046</v>
+      </c>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6">
         <v>8</v>
       </c>
-      <c r="N34" s="6">
-        <f t="shared" si="28"/>
+      <c r="Q34" s="6">
+        <f t="shared" si="25"/>
         <v>64</v>
       </c>
-      <c r="O34">
+      <c r="R34">
         <v>37</v>
       </c>
-      <c r="P34">
+      <c r="S34">
         <v>17.18</v>
       </c>
-      <c r="Q34" s="24">
-        <f>O34*60+P34</f>
+      <c r="T34" s="24">
+        <f>R34*60+S34</f>
         <v>2237.1799999999998</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>1958.1103515625</v>
       </c>
       <c r="D35">
         <v>16</v>
       </c>
       <c r="E35">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>128</v>
       </c>
       <c r="F35">
@@ -7081,47 +7132,47 @@
         <v>1.01</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" ref="H35:H36" si="31">F35*60+G35</f>
+        <f t="shared" ref="H35:H36" si="28">F35*60+G35</f>
         <v>781.01</v>
       </c>
       <c r="I35" s="27">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>88.646048065965857</v>
       </c>
       <c r="J35" s="27">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6">
+        <f t="shared" si="24"/>
+        <v>0.69254725051535826</v>
+      </c>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6">
         <v>16</v>
       </c>
-      <c r="N35" s="6">
-        <f t="shared" si="28"/>
+      <c r="Q35" s="6">
+        <f t="shared" si="25"/>
         <v>128</v>
       </c>
-      <c r="O35">
+      <c r="R35">
         <v>20</v>
       </c>
-      <c r="P35">
+      <c r="S35">
         <v>46.78</v>
       </c>
-      <c r="Q35" s="6">
-        <f t="shared" ref="Q35:Q36" si="32">O35*60+P35</f>
+      <c r="T35" s="6">
+        <f t="shared" ref="T35:T36" si="29">R35*60+S35</f>
         <v>1246.78</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>489.527587890625</v>
       </c>
       <c r="D36">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>256</v>
       </c>
       <c r="F36">
@@ -7131,57 +7182,57 @@
         <v>21.01</v>
       </c>
       <c r="H36" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>681.01</v>
       </c>
       <c r="I36" s="27">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>101.66289775480536</v>
       </c>
       <c r="J36" s="27">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6">
+        <f t="shared" si="24"/>
+        <v>0.39712069435470843</v>
+      </c>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6">
         <v>32</v>
       </c>
-      <c r="N36" s="6">
-        <f t="shared" si="28"/>
+      <c r="Q36" s="6">
+        <f t="shared" si="25"/>
         <v>256</v>
       </c>
-      <c r="O36">
+      <c r="R36">
         <v>18</v>
       </c>
-      <c r="P36">
+      <c r="S36">
         <v>28.038</v>
       </c>
-      <c r="Q36">
-        <f t="shared" si="32"/>
+      <c r="T36">
+        <f t="shared" si="29"/>
         <v>1108.038</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="26"/>
       <c r="C37" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>122.38189697265625</v>
       </c>
       <c r="D37">
         <v>64</v>
       </c>
       <c r="E37">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>512</v>
       </c>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
-      <c r="L37" s="26"/>
-      <c r="M37">
+      <c r="O37" s="26"/>
+      <c r="P37">
         <v>64</v>
       </c>
-      <c r="N37">
-        <f t="shared" si="28"/>
+      <c r="Q37">
+        <f t="shared" si="25"/>
         <v>512</v>
       </c>
     </row>
@@ -7218,7 +7269,7 @@
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" ref="N40:N46" si="33">M40*8</f>
+        <f t="shared" ref="N40:N46" si="30">M40*8</f>
         <v>8</v>
       </c>
       <c r="O40">
@@ -7257,7 +7308,7 @@
         <v>2</v>
       </c>
       <c r="N41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
       <c r="O41">
@@ -7279,9 +7330,9 @@
         <f>H7</f>
         <v>12.62</v>
       </c>
-      <c r="F42">
-        <f>Q7</f>
-        <v>0</v>
+      <c r="F42" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="G42">
         <f>H19</f>
@@ -7291,7 +7342,7 @@
         <v>4</v>
       </c>
       <c r="N42">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>32</v>
       </c>
       <c r="O42">
@@ -7313,9 +7364,9 @@
         <f>H8</f>
         <v>10.47</v>
       </c>
-      <c r="E43">
-        <f>Q8</f>
-        <v>0</v>
+      <c r="E43" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="F43">
         <f>H20</f>
@@ -7329,7 +7380,7 @@
         <v>8</v>
       </c>
       <c r="N43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>64</v>
       </c>
       <c r="O43">
@@ -7347,9 +7398,9 @@
       <c r="C44">
         <v>32</v>
       </c>
-      <c r="D44">
-        <f>Q9</f>
-        <v>0</v>
+      <c r="D44" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E44">
         <f>H21</f>
@@ -7368,7 +7419,7 @@
         <v>16</v>
       </c>
       <c r="N44">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>128</v>
       </c>
       <c r="O44">
@@ -7378,7 +7429,7 @@
         <v>41.149000000000001</v>
       </c>
       <c r="Q44" s="6">
-        <f t="shared" ref="Q44:Q45" si="34">O44*60+P44</f>
+        <f t="shared" ref="Q44:Q45" si="31">O44*60+P44</f>
         <v>1301.1489999999999</v>
       </c>
     </row>
@@ -7399,7 +7450,7 @@
         <v>1216.44</v>
       </c>
       <c r="G45" s="2">
-        <f>Q34</f>
+        <f>T34</f>
         <v>2237.1799999999998</v>
       </c>
       <c r="H45" s="2"/>
@@ -7407,7 +7458,7 @@
         <v>32</v>
       </c>
       <c r="N45" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>256</v>
       </c>
       <c r="O45">
@@ -7417,7 +7468,7 @@
         <v>22.97</v>
       </c>
       <c r="Q45" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="31"/>
         <v>1162.97</v>
       </c>
     </row>
@@ -7434,7 +7485,7 @@
         <v>781.01</v>
       </c>
       <c r="F46">
-        <f>Q35</f>
+        <f>T35</f>
         <v>1246.78</v>
       </c>
       <c r="G46">
@@ -7446,7 +7497,7 @@
         <v>64</v>
       </c>
       <c r="N46">
-        <f t="shared" si="33"/>
+        <f t="shared" si="30"/>
         <v>512</v>
       </c>
     </row>
@@ -7459,7 +7510,7 @@
         <v>681.01</v>
       </c>
       <c r="E47">
-        <f>Q36</f>
+        <f>T36</f>
         <v>1108.038</v>
       </c>
       <c r="F47">
@@ -7512,31 +7563,31 @@
         <v>195102</v>
       </c>
       <c r="N49" s="40">
-        <f t="shared" ref="N49:T49" si="35">$M$49/N$48</f>
+        <f t="shared" ref="N49:T49" si="32">$M$49/N$48</f>
         <v>24387.75</v>
       </c>
       <c r="O49" s="41">
-        <f t="shared" si="35"/>
+        <f t="shared" si="32"/>
         <v>12193.875</v>
       </c>
       <c r="P49" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="32"/>
         <v>6096.9375</v>
       </c>
       <c r="Q49" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="32"/>
         <v>3048.46875</v>
       </c>
       <c r="R49" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="32"/>
         <v>1524.234375</v>
       </c>
       <c r="S49" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="32"/>
         <v>762.1171875</v>
       </c>
       <c r="T49" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="32"/>
         <v>381.05859375</v>
       </c>
     </row>
@@ -7548,31 +7599,31 @@
         <v>432919</v>
       </c>
       <c r="N50" s="42">
-        <f t="shared" ref="N50:T50" si="36">$M$50/N$48</f>
+        <f t="shared" ref="N50:T50" si="33">$M$50/N$48</f>
         <v>54114.875</v>
       </c>
       <c r="O50" s="40">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>27057.4375</v>
       </c>
       <c r="P50" s="41">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>13528.71875</v>
       </c>
       <c r="Q50" s="27">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>6764.359375</v>
       </c>
       <c r="R50" s="27">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>3382.1796875</v>
       </c>
       <c r="S50" s="27">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>1691.08984375</v>
       </c>
       <c r="T50" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>845.544921875</v>
       </c>
     </row>
@@ -7584,31 +7635,31 @@
         <v>1017573</v>
       </c>
       <c r="N51" s="43">
-        <f t="shared" ref="N51:T51" si="37">$M$51/N$48</f>
+        <f t="shared" ref="N51:T51" si="34">$M$51/N$48</f>
         <v>127196.625</v>
       </c>
       <c r="O51" s="42">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>63598.3125</v>
       </c>
       <c r="P51" s="40">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>31799.15625</v>
       </c>
       <c r="Q51" s="41">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>15899.578125</v>
       </c>
       <c r="R51" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>7949.7890625</v>
       </c>
       <c r="S51" s="27">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>3974.89453125</v>
       </c>
       <c r="T51" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>1987.447265625</v>
       </c>
     </row>
@@ -7620,31 +7671,31 @@
         <v>2037710</v>
       </c>
       <c r="N52" s="27">
-        <f t="shared" ref="N52:T52" si="38">$M$52/N$48</f>
+        <f t="shared" ref="N52:T52" si="35">$M$52/N$48</f>
         <v>254713.75</v>
       </c>
       <c r="O52" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>127356.875</v>
       </c>
       <c r="P52" s="42">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>63678.4375</v>
       </c>
       <c r="Q52" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>31839.21875</v>
       </c>
       <c r="R52" s="41">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>15919.609375</v>
       </c>
       <c r="S52" s="27">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>7959.8046875</v>
       </c>
       <c r="T52" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>3979.90234375</v>
       </c>
     </row>
@@ -7656,31 +7707,31 @@
         <v>4010210</v>
       </c>
       <c r="N53" s="27">
-        <f t="shared" ref="N53:T53" si="39">$M$53/N$48</f>
+        <f t="shared" ref="N53:T53" si="36">$M$53/N$48</f>
         <v>501276.25</v>
       </c>
       <c r="O53" s="27">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>250638.125</v>
       </c>
       <c r="P53" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>125319.0625</v>
       </c>
       <c r="Q53" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>62659.53125</v>
       </c>
       <c r="R53" s="40">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>31329.765625</v>
       </c>
       <c r="S53" s="41">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>15664.8828125</v>
       </c>
       <c r="T53" s="25">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>7832.44140625</v>
       </c>
     </row>
@@ -7692,31 +7743,31 @@
         <v>8101299</v>
       </c>
       <c r="N54" s="44">
-        <f t="shared" ref="N54:T54" si="40">$M$54/N$48</f>
+        <f t="shared" ref="N54:T54" si="37">$M$54/N$48</f>
         <v>1012662.375</v>
       </c>
       <c r="O54" s="44">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>506331.1875</v>
       </c>
       <c r="P54" s="44">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>253165.59375</v>
       </c>
       <c r="Q54" s="43">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>126582.796875</v>
       </c>
       <c r="R54" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>63291.3984375</v>
       </c>
       <c r="S54" s="40">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>31645.69921875</v>
       </c>
       <c r="T54" s="41">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>15822.849609375</v>
       </c>
     </row>
@@ -7728,31 +7779,31 @@
         <v>15522778</v>
       </c>
       <c r="N55" s="44">
-        <f t="shared" ref="N55:T55" si="41">$M$55/N$48</f>
+        <f t="shared" ref="N55:T55" si="38">$M$55/N$48</f>
         <v>1940347.25</v>
       </c>
       <c r="O55" s="44">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>970173.625</v>
       </c>
       <c r="P55" s="44">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>485086.8125</v>
       </c>
       <c r="Q55" s="44">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>242543.40625</v>
       </c>
       <c r="R55" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>121271.703125</v>
       </c>
       <c r="S55" s="42">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>60635.8515625</v>
       </c>
       <c r="T55" s="40">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>30317.92578125</v>
       </c>
     </row>
@@ -7824,11 +7875,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="T4:U4"/>
+  <mergeCells count="3">
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="W4:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Estimated pipe07 serial running time
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
   </bookViews>
   <sheets>
     <sheet name="HSR Cluster" sheetId="1" r:id="rId1"/>
     <sheet name="SimplyHPC A8" sheetId="2" r:id="rId2"/>
     <sheet name="Depl. Time" sheetId="3" r:id="rId3"/>
     <sheet name="Export Gnuplot" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="72">
   <si>
     <t>pipe01</t>
   </si>
@@ -43,12 +44,6 @@
   </si>
   <si>
     <t>pipe02</t>
-  </si>
-  <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Elements</t>
   </si>
   <si>
     <t>pipe06</t>
@@ -216,9 +211,6 @@
     <t>Weak Scaling</t>
   </si>
   <si>
-    <t>check the iterative solvers</t>
-  </si>
-  <si>
     <t>SizeUp</t>
   </si>
   <si>
@@ -227,13 +219,35 @@
   <si>
     <t>running</t>
   </si>
+  <si>
+    <t>4--8</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>8--8</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>1--1</t>
+  </si>
+  <si>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>estimated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -477,7 +491,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -523,7 +537,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -540,6 +553,9 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,9 +563,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="7" fillId="12" borderId="6" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2340,7 +2360,7 @@
                 <c:pt idx="1">
                   <c:v>4369.8999999999996</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00E+00">
+                <c:pt idx="2">
                   <c:v>2124.5300000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
@@ -2362,7 +2382,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SimplyHPC A8'!$O$14</c:f>
+              <c:f>'SimplyHPC A8'!$O$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3606,10 +3626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y50"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4:Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3630,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S3" s="58"/>
     </row>
@@ -3651,10 +3671,10 @@
         <v>5</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>6</v>
@@ -3672,22 +3692,16 @@
         <v>5</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -3709,7 +3723,7 @@
       <c r="H5" s="6"/>
       <c r="J5" s="26"/>
       <c r="K5" s="2">
-        <f t="shared" ref="K5:K11" si="1">$C$45/L5</f>
+        <f>$C$45/L5</f>
         <v>432919</v>
       </c>
       <c r="L5" s="6">
@@ -3722,23 +3736,18 @@
         <v>25.87</v>
       </c>
       <c r="O5" s="26">
-        <f t="shared" ref="O5" si="2">M5*60+N5</f>
+        <f t="shared" ref="O5" si="1">M5*60+N5</f>
         <v>5965.87</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
-      <c r="X5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>195102</v>
-      </c>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <f t="shared" ref="B6:B11" si="3">$C$44/C6</f>
+        <f t="shared" ref="B6:B11" si="2">$C$44/C6</f>
         <v>32517</v>
       </c>
       <c r="C6">
@@ -3751,7 +3760,7 @@
         <v>54.62</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ref="F6:F11" si="4">D6*60+E6</f>
+        <f t="shared" ref="F6:F11" si="3">D6*60+E6</f>
         <v>894.62</v>
       </c>
       <c r="G6" s="27">
@@ -3763,7 +3772,7 @@
         <v>0.4267765457214609</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K5:K11" si="4">$C$45/L6</f>
         <v>72153.166666666672</v>
       </c>
       <c r="L6">
@@ -3795,16 +3804,11 @@
         <f>R6/L6</f>
         <v>8.886717062570644E-2</v>
       </c>
-      <c r="X6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>432919</v>
-      </c>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16258.5</v>
       </c>
       <c r="C7">
@@ -3817,7 +3821,7 @@
         <v>6.45</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>486.45</v>
       </c>
       <c r="G7" s="27">
@@ -3829,7 +3833,7 @@
         <v>0.39243790043512522</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="1"/>
+        <f>$C$45/L7</f>
         <v>36076.583333333336</v>
       </c>
       <c r="L7">
@@ -3861,16 +3865,11 @@
         <f t="shared" ref="S7:S11" si="11">R7/L7</f>
         <v>5.5695497509985453E-2</v>
       </c>
-      <c r="X7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>1017573</v>
-      </c>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8129.25</v>
       </c>
       <c r="C8">
@@ -3883,7 +3882,7 @@
         <v>34.65</v>
       </c>
       <c r="F8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>274.64999999999998</v>
       </c>
       <c r="G8" s="27">
@@ -3895,7 +3894,7 @@
         <v>0.34753580314339466</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>18038.291666666668</v>
       </c>
       <c r="L8">
@@ -3927,16 +3926,11 @@
         <f t="shared" si="11"/>
         <v>1.9752108614994077E-2</v>
       </c>
-      <c r="X8" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>2037710</v>
-      </c>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5419.5</v>
       </c>
       <c r="C9">
@@ -3949,7 +3943,7 @@
         <v>39.74</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>219.74</v>
       </c>
       <c r="G9" s="27">
@@ -3961,7 +3955,7 @@
         <v>0.28958680966394623</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12025.527777777777</v>
       </c>
       <c r="L9">
@@ -3993,16 +3987,11 @@
         <f t="shared" si="11"/>
         <v>1.2217460462568129E-2</v>
       </c>
-      <c r="X9" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>4010210</v>
-      </c>
+      <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4064.625</v>
       </c>
       <c r="C10">
@@ -4015,7 +4004,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>188.05</v>
       </c>
       <c r="G10" s="27">
@@ -4027,7 +4016,7 @@
         <v>0.25379076929894528</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9019.1458333333339</v>
       </c>
       <c r="L10">
@@ -4062,7 +4051,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3251.7</v>
       </c>
       <c r="C11">
@@ -4075,7 +4064,7 @@
         <v>51.94</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>171.94</v>
       </c>
       <c r="G11" s="27">
@@ -4087,7 +4076,7 @@
         <v>0.22205585281687409</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7215.3166666666666</v>
       </c>
       <c r="L11">
@@ -4122,16 +4111,16 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R12" s="58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S12" s="58"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -4146,13 +4135,13 @@
         <v>5</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L13" t="s">
         <v>2</v>
@@ -4167,16 +4156,16 @@
         <v>5</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -4337,7 +4326,7 @@
         <v>2.9054341852719559E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <f t="shared" si="15"/>
         <v>42398.875</v>
@@ -4397,7 +4386,7 @@
         <v>1.4728419759971802E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <f t="shared" si="15"/>
         <v>28265.916666666668</v>
@@ -4457,7 +4446,7 @@
         <v>9.3571887045376702E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <f t="shared" si="15"/>
         <v>21199.4375</v>
@@ -4517,7 +4506,7 @@
         <v>6.7429316889727848E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <f t="shared" si="15"/>
         <v>16959.55</v>
@@ -4577,13 +4566,17 @@
         <v>5.1672156406010203E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R21" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="S21" s="55"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -4598,13 +4591,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>2</v>
@@ -4619,34 +4612,40 @@
         <v>5</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="S22" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="T22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U22" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="V22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="U22" s="6" t="s">
+      <c r="W22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="V22" s="6" t="s">
+      <c r="X22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="W22" s="6" t="s">
+      <c r="Y22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="X22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y22" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="C23">
         <v>1</v>
@@ -4663,20 +4662,28 @@
         <v>55036.17</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="J23" s="39" t="s">
-        <v>64</v>
+      <c r="J23" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="2">
+        <f>$C$49/L23</f>
+        <v>8101299</v>
       </c>
       <c r="L23" s="6">
         <v>1</v>
       </c>
-      <c r="R23" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="T23" s="6">
+      <c r="O23" s="51">
+        <f>Sheet1!P20</f>
+        <v>110000</v>
+      </c>
+      <c r="U23" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V23" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <f t="shared" ref="B24:B29" si="23">$C$48/C24</f>
         <v>668368.33333333337</v>
@@ -4702,36 +4709,56 @@
         <f t="shared" ref="H24:H29" si="25">G24/C24</f>
         <v>0.51756320230662678</v>
       </c>
+      <c r="K24" s="2">
+        <f t="shared" ref="K24:K29" si="26">$C$49/L24</f>
+        <v>1350216.5</v>
+      </c>
       <c r="L24" s="6">
         <v>6</v>
       </c>
       <c r="M24" s="6">
+        <f>10*60+34</f>
         <v>634</v>
       </c>
       <c r="N24">
-        <v>36.43</v>
+        <v>12.69</v>
       </c>
       <c r="O24" s="6">
-        <f t="shared" ref="O24:O25" si="26">M24*60+N24</f>
-        <v>38076.43</v>
-      </c>
-      <c r="R24" s="6"/>
-      <c r="T24" s="6">
+        <f t="shared" ref="O24:O25" si="27">M24*60+N24</f>
+        <v>38052.69</v>
+      </c>
+      <c r="P24" s="27">
+        <f>$O$23/O24</f>
+        <v>2.8907286186600736</v>
+      </c>
+      <c r="Q24" s="27">
+        <f t="shared" ref="Q24:Q29" si="28">P24/L24</f>
+        <v>0.48178810311001224</v>
+      </c>
+      <c r="R24" s="27">
+        <f>K24/$K$23*$O$23/O24</f>
+        <v>0.48178810311001224</v>
+      </c>
+      <c r="S24" s="38">
+        <f>R24/L24</f>
+        <v>8.0298017185002041E-2</v>
+      </c>
+      <c r="V24" s="6">
         <v>6</v>
       </c>
-      <c r="U24" s="6">
+      <c r="W24" s="6">
         <f>20*60+55</f>
         <v>1255</v>
       </c>
-      <c r="V24">
+      <c r="X24">
         <v>25.52</v>
       </c>
-      <c r="W24" s="6">
-        <f t="shared" ref="W24:W28" si="27">U24*60+V24</f>
+      <c r="Y24" s="6">
+        <f t="shared" ref="Y24:Y28" si="29">W24*60+X24</f>
         <v>75325.52</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <f t="shared" si="23"/>
         <v>334184.16666666669</v>
@@ -4750,7 +4777,7 @@
         <v>5985.82</v>
       </c>
       <c r="G25" s="27">
-        <f t="shared" ref="G25:G29" si="28">$F$23/F25</f>
+        <f t="shared" ref="G25:G29" si="30">$F$23/F25</f>
         <v>9.1944244898777452</v>
       </c>
       <c r="H25" s="27">
@@ -4758,6 +4785,10 @@
         <v>0.76620204082314547</v>
       </c>
       <c r="J25" s="6"/>
+      <c r="K25" s="2">
+        <f t="shared" si="26"/>
+        <v>675108.25</v>
+      </c>
       <c r="L25" s="6">
         <v>12</v>
       </c>
@@ -4768,26 +4799,41 @@
         <v>49.49</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>18709.490000000002</v>
       </c>
-      <c r="R25" s="6"/>
-      <c r="T25" s="6">
+      <c r="P25" s="27">
+        <f t="shared" ref="P25:P29" si="31">$O$23/O25</f>
+        <v>5.8793692398884199</v>
+      </c>
+      <c r="Q25" s="27">
+        <f t="shared" si="28"/>
+        <v>0.48994743665736834</v>
+      </c>
+      <c r="R25" s="27">
+        <f t="shared" ref="R25:R29" si="32">K25/$K$23*$O$23/O25</f>
+        <v>0.48994743665736828</v>
+      </c>
+      <c r="S25" s="38">
+        <f t="shared" ref="S25:S29" si="33">R25/L25</f>
+        <v>4.0828953054780688E-2</v>
+      </c>
+      <c r="V25" s="6">
         <v>12</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <f>10*60+1</f>
         <v>601</v>
       </c>
-      <c r="V25">
+      <c r="X25">
         <v>17.600000000000001</v>
       </c>
-      <c r="W25" s="6">
-        <f t="shared" si="27"/>
+      <c r="Y25" s="6">
+        <f t="shared" si="29"/>
         <v>36077.599999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <f t="shared" si="23"/>
         <v>167092.08333333334</v>
@@ -4806,7 +4852,7 @@
         <v>4403.74</v>
       </c>
       <c r="G26" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>12.497597496673283</v>
       </c>
       <c r="H26" s="27">
@@ -4814,6 +4860,10 @@
         <v>0.52073322902805341</v>
       </c>
       <c r="J26" s="6"/>
+      <c r="K26" s="2">
+        <f t="shared" si="26"/>
+        <v>337554.125</v>
+      </c>
       <c r="L26" s="6">
         <v>24</v>
       </c>
@@ -4827,21 +4877,37 @@
         <f>M26*60+N26</f>
         <v>9025.94</v>
       </c>
-      <c r="T26" s="6">
+      <c r="P26" s="27">
+        <f t="shared" si="31"/>
+        <v>12.187096302434981</v>
+      </c>
+      <c r="Q26" s="27">
+        <f t="shared" si="28"/>
+        <v>0.50779567926812419</v>
+      </c>
+      <c r="R26" s="27">
+        <f t="shared" si="32"/>
+        <v>0.50779567926812419</v>
+      </c>
+      <c r="S26" s="38">
+        <f t="shared" si="33"/>
+        <v>2.1158153302838507E-2</v>
+      </c>
+      <c r="V26" s="6">
         <v>24</v>
       </c>
-      <c r="U26" s="6">
+      <c r="W26" s="6">
         <v>273</v>
       </c>
-      <c r="V26">
+      <c r="X26">
         <v>54.67</v>
       </c>
-      <c r="W26" s="6">
-        <f t="shared" si="27"/>
+      <c r="Y26" s="6">
+        <f t="shared" si="29"/>
         <v>16434.669999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <f t="shared" si="23"/>
         <v>111394.72222222222</v>
@@ -4860,7 +4926,7 @@
         <v>2937.19</v>
       </c>
       <c r="G27" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>18.737694871629007</v>
       </c>
       <c r="H27" s="27">
@@ -4868,6 +4934,10 @@
         <v>0.5204915242119168</v>
       </c>
       <c r="J27" s="6"/>
+      <c r="K27" s="2">
+        <f t="shared" si="26"/>
+        <v>225036.08333333334</v>
+      </c>
       <c r="L27" s="6">
         <v>36</v>
       </c>
@@ -4878,24 +4948,40 @@
         <v>15.47</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" ref="O27:O29" si="29">M27*60+N27</f>
+        <f t="shared" ref="O27:O29" si="34">M27*60+N27</f>
         <v>5595.47</v>
       </c>
-      <c r="T27" s="6">
+      <c r="P27" s="27">
+        <f t="shared" si="31"/>
+        <v>19.658759675237288</v>
+      </c>
+      <c r="Q27" s="27">
+        <f t="shared" si="28"/>
+        <v>0.54607665764548019</v>
+      </c>
+      <c r="R27" s="27">
+        <f t="shared" si="32"/>
+        <v>0.5460766576454803</v>
+      </c>
+      <c r="S27" s="38">
+        <f t="shared" si="33"/>
+        <v>1.5168796045707787E-2</v>
+      </c>
+      <c r="V27" s="6">
         <v>36</v>
       </c>
-      <c r="U27" s="6">
+      <c r="W27" s="6">
         <v>179</v>
       </c>
-      <c r="V27">
+      <c r="X27">
         <v>13.78</v>
       </c>
-      <c r="W27" s="6">
-        <f t="shared" si="27"/>
+      <c r="Y27" s="6">
+        <f t="shared" si="29"/>
         <v>10753.78</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <f t="shared" si="23"/>
         <v>83546.041666666672</v>
@@ -4914,13 +5000,17 @@
         <v>2239.5700000000002</v>
       </c>
       <c r="G28" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>24.574436164085068</v>
       </c>
       <c r="H28" s="27">
         <f t="shared" si="25"/>
         <v>0.51196742008510554</v>
       </c>
+      <c r="K28" s="2">
+        <f t="shared" si="26"/>
+        <v>168777.0625</v>
+      </c>
       <c r="L28" s="6">
         <v>48</v>
       </c>
@@ -4934,22 +5024,37 @@
         <f>M28*60+N28</f>
         <v>4455.05</v>
       </c>
-      <c r="R28" s="6"/>
-      <c r="T28" s="6">
+      <c r="P28" s="27">
+        <f t="shared" si="31"/>
+        <v>24.691080908182848</v>
+      </c>
+      <c r="Q28" s="27">
+        <f t="shared" si="28"/>
+        <v>0.51439751892047603</v>
+      </c>
+      <c r="R28" s="27">
+        <f t="shared" si="32"/>
+        <v>0.51439751892047592</v>
+      </c>
+      <c r="S28" s="38">
+        <f t="shared" si="33"/>
+        <v>1.0716614977509914E-2</v>
+      </c>
+      <c r="V28" s="6">
         <v>48</v>
       </c>
-      <c r="U28" s="6">
+      <c r="W28" s="6">
         <v>132</v>
       </c>
-      <c r="V28">
+      <c r="X28">
         <v>51.36</v>
       </c>
-      <c r="W28" s="6">
-        <f t="shared" si="27"/>
+      <c r="Y28" s="6">
+        <f t="shared" si="29"/>
         <v>7971.36</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <f t="shared" si="23"/>
         <v>66836.833333333328</v>
@@ -4968,13 +5073,17 @@
         <v>1778.97</v>
       </c>
       <c r="G29" s="27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>30.937098433363126</v>
       </c>
       <c r="H29" s="27">
         <f t="shared" si="25"/>
         <v>0.51561830722271873</v>
       </c>
+      <c r="K29" s="2">
+        <f t="shared" si="26"/>
+        <v>135021.65</v>
+      </c>
       <c r="L29" s="6">
         <v>60</v>
       </c>
@@ -4985,39 +5094,55 @@
         <v>31.28</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>3571.28</v>
       </c>
-      <c r="T29" s="6">
+      <c r="P29" s="27">
+        <f t="shared" si="31"/>
+        <v>30.801281333303464</v>
+      </c>
+      <c r="Q29" s="27">
+        <f t="shared" si="28"/>
+        <v>0.51335468888839109</v>
+      </c>
+      <c r="R29" s="27">
+        <f t="shared" si="32"/>
+        <v>0.51335468888839109</v>
+      </c>
+      <c r="S29" s="38">
+        <f t="shared" si="33"/>
+        <v>8.5559114814731854E-3</v>
+      </c>
+      <c r="V29" s="6">
         <v>60</v>
       </c>
-      <c r="U29">
+      <c r="W29">
         <v>106</v>
       </c>
-      <c r="V29">
+      <c r="X29">
         <v>31.82</v>
       </c>
-      <c r="W29" s="6">
-        <f t="shared" ref="W29" si="30">U29*60+V29</f>
+      <c r="Y29" s="6">
+        <f t="shared" ref="Y29" si="35">W29*60+X29</f>
         <v>6391.82</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H31" s="6"/>
       <c r="K31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H32" s="6"/>
       <c r="K32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L32" t="s">
         <v>2</v>
@@ -5036,15 +5161,15 @@
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="45">
+      <c r="C33" s="44">
         <f>C39</f>
         <v>38361.1875</v>
       </c>
-      <c r="D33" s="45">
+      <c r="D33" s="44">
         <f>D39</f>
         <v>81350.385416666672</v>
       </c>
-      <c r="E33" s="45">
+      <c r="E33" s="44">
         <f>E39</f>
         <v>167393.88333333333</v>
       </c>
@@ -5201,7 +5326,7 @@
         <v>4455.05</v>
       </c>
       <c r="F37">
-        <f>W28</f>
+        <f>Y28</f>
         <v>7971.36</v>
       </c>
       <c r="K37">
@@ -5223,7 +5348,7 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C39" s="2">
         <f>AVERAGE(D44,E45,F46,G47)</f>
@@ -5244,7 +5369,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C40" s="2">
         <f>STDEV(G47,F46,E45,D44)</f>
@@ -5265,7 +5390,7 @@
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C41" s="33">
         <f>C40/C39</f>
@@ -5309,7 +5434,6 @@
         <v>0</v>
       </c>
       <c r="C44" s="13">
-        <f>Y5</f>
         <v>195102</v>
       </c>
       <c r="D44" s="14">
@@ -5338,7 +5462,6 @@
         <v>6</v>
       </c>
       <c r="C45" s="13">
-        <f>Y6</f>
         <v>432919</v>
       </c>
       <c r="D45" s="18">
@@ -5364,10 +5487,9 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C46" s="13">
-        <f>Y7</f>
         <v>1017573</v>
       </c>
       <c r="D46" s="32">
@@ -5393,10 +5515,9 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C47" s="13">
-        <f>Y8</f>
         <v>2037710</v>
       </c>
       <c r="D47" s="35">
@@ -5422,10 +5543,9 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C48" s="13">
-        <f>Y9</f>
         <v>4010210</v>
       </c>
       <c r="D48" s="15">
@@ -5451,7 +5571,7 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C49" s="31">
         <v>8101299</v>
@@ -5461,25 +5581,25 @@
         <v>1350216.5</v>
       </c>
       <c r="E49" s="15">
-        <f t="shared" ref="E49:H49" si="31">$C$49/E$43</f>
+        <f t="shared" ref="E49:H49" si="36">$C$49/E$43</f>
         <v>675108.25</v>
       </c>
       <c r="F49" s="35">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>337554.125</v>
       </c>
       <c r="G49" s="32">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>168777.0625</v>
       </c>
       <c r="H49" s="15">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>84388.53125</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C50" s="31">
         <v>15522778</v>
@@ -5489,19 +5609,19 @@
         <v>2587129.6666666665</v>
       </c>
       <c r="E50" s="15">
-        <f t="shared" ref="E50:H50" si="32">$C$50/E$43</f>
+        <f t="shared" ref="E50:H50" si="37">$C$50/E$43</f>
         <v>1293564.8333333333</v>
       </c>
       <c r="F50" s="15">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>646782.41666666663</v>
       </c>
       <c r="G50" s="35">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>323391.20833333331</v>
       </c>
       <c r="H50" s="32">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>161695.60416666666</v>
       </c>
     </row>
@@ -5520,8 +5640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5548,10 +5668,10 @@
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="O3" s="45" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="6"/>
@@ -5563,83 +5683,83 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
+        <v>11</v>
+      </c>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
       <c r="Q4" s="56"/>
       <c r="R4" s="56"/>
-      <c r="S4" s="55"/>
+      <c r="S4" s="54"/>
       <c r="T4" s="6"/>
-      <c r="U4" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" s="53"/>
-      <c r="W4" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="X4" s="59"/>
+      <c r="U4" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="52"/>
+      <c r="W4" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="X4" s="60"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="U5" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="V5" s="47" t="s">
+      <c r="U5" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="W5" s="36" t="s">
-        <v>58</v>
-      </c>
       <c r="X5" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -5685,8 +5805,8 @@
         <f>R6*60+S6</f>
         <v>6595.97</v>
       </c>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
       <c r="W6" s="36"/>
       <c r="X6" s="36"/>
     </row>
@@ -5749,11 +5869,11 @@
         <f>R7*60+S7</f>
         <v>986.61</v>
       </c>
-      <c r="U7" s="48">
+      <c r="U7" s="47">
         <f>$T$6/T7</f>
         <v>6.6854886936074029</v>
       </c>
-      <c r="V7" s="48">
+      <c r="V7" s="47">
         <f>U7/Q7</f>
         <v>0.83568608670092537</v>
       </c>
@@ -5761,7 +5881,7 @@
         <f>O7/$O$6*$T$6/T7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="X7" s="50">
+      <c r="X7" s="49">
         <f>W7/Q7</f>
         <v>0.10446076083761567</v>
       </c>
@@ -5825,11 +5945,11 @@
         <f>R8*60+S8</f>
         <v>518.11900000000003</v>
       </c>
-      <c r="U8" s="48">
+      <c r="U8" s="47">
         <f>$T$6/T8</f>
         <v>12.730608219347292</v>
       </c>
-      <c r="V8" s="48">
+      <c r="V8" s="47">
         <f>U8/Q8</f>
         <v>0.79566301370920578</v>
       </c>
@@ -5837,7 +5957,7 @@
         <f>O8/$O$6*$T$6/T8</f>
         <v>0.79566301370920578</v>
       </c>
-      <c r="X8" s="50">
+      <c r="X8" s="49">
         <f>W8/Q8</f>
         <v>4.9728938356825361E-2</v>
       </c>
@@ -5901,11 +6021,11 @@
         <f>R9*60+S9</f>
         <v>307.14999999999998</v>
       </c>
-      <c r="U9" s="48">
+      <c r="U9" s="47">
         <f>$T$6/T9</f>
         <v>21.474751749959307</v>
       </c>
-      <c r="V9" s="48">
+      <c r="V9" s="47">
         <f>U9/Q9</f>
         <v>0.67108599218622833</v>
       </c>
@@ -5913,7 +6033,7 @@
         <f>O9/$O$6*$T$6/T9</f>
         <v>0.67108599218622833</v>
       </c>
-      <c r="X9" s="50">
+      <c r="X9" s="49">
         <f>W9/Q9</f>
         <v>2.0971437255819635E-2</v>
       </c>
@@ -5977,11 +6097,11 @@
         <f>R10*60+S10</f>
         <v>252.13</v>
       </c>
-      <c r="U10" s="48">
+      <c r="U10" s="47">
         <f>$T$6/T10</f>
         <v>26.160988379010828</v>
       </c>
-      <c r="V10" s="49">
+      <c r="V10" s="48">
         <f>U10/Q10</f>
         <v>0.40876544342204418</v>
       </c>
@@ -5989,7 +6109,7 @@
         <f>O10/$O$6*$T$6/T10</f>
         <v>0.40876544342204418</v>
       </c>
-      <c r="X10" s="50">
+      <c r="X10" s="49">
         <f>W10/Q10</f>
         <v>6.3869600534694404E-3</v>
       </c>
@@ -6054,11 +6174,11 @@
         <f>R11*60+S11</f>
         <v>216.96</v>
       </c>
-      <c r="U11" s="48">
+      <c r="U11" s="47">
         <f>$T$6/T11</f>
         <v>30.40177912979351</v>
       </c>
-      <c r="V11" s="48">
+      <c r="V11" s="47">
         <f>U11/Q11</f>
         <v>0.2375138994515118</v>
       </c>
@@ -6066,7 +6186,7 @@
         <f>O11/$O$6*$T$6/T11</f>
         <v>0.2375138994515118</v>
       </c>
-      <c r="X11" s="50">
+      <c r="X11" s="49">
         <f>W11/Q11</f>
         <v>1.8555773394649359E-3</v>
       </c>
@@ -6132,11 +6252,11 @@
         <f>R12*60+S12</f>
         <v>296.72000000000003</v>
       </c>
-      <c r="U12" s="48">
+      <c r="U12" s="47">
         <f>$T$6/T12</f>
         <v>22.229610407117821</v>
       </c>
-      <c r="V12" s="48">
+      <c r="V12" s="47">
         <f>U12/Q12</f>
         <v>8.683441565280399E-2</v>
       </c>
@@ -6144,7 +6264,7 @@
         <f>O12/$O$6*$T$6/T12</f>
         <v>8.683441565280399E-2</v>
       </c>
-      <c r="X12" s="50">
+      <c r="X12" s="49">
         <f>W12/Q12</f>
         <v>3.3919693614376558E-4</v>
       </c>
@@ -6184,11 +6304,8 @@
       <c r="X13" s="6"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="O14" s="46" t="s">
-        <v>10</v>
-      </c>
       <c r="W14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
@@ -6197,8 +6314,11 @@
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C15" s="46" t="s">
-        <v>9</v>
+      <c r="C15" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" s="45" t="s">
+        <v>8</v>
       </c>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
@@ -6209,72 +6329,72 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="I16" s="58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J16" s="58"/>
       <c r="K16" s="58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L16" s="58"/>
       <c r="P16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" t="s">
         <v>17</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>18</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>19</v>
-      </c>
-      <c r="S16" t="s">
-        <v>20</v>
-      </c>
-      <c r="T16" t="s">
-        <v>21</v>
       </c>
       <c r="W16" s="6"/>
       <c r="X16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Y16" s="6" t="s">
+      <c r="AA16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Z16" s="6" t="s">
+      <c r="AB16" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="AA16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB16" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>18</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>19</v>
       </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
-      </c>
       <c r="I17" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N17" s="6"/>
       <c r="P17">
@@ -6381,11 +6501,11 @@
       <c r="G19">
         <v>18.350000000000001</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H19" s="50">
         <f t="shared" si="9"/>
         <v>2478.35</v>
       </c>
-      <c r="I19" s="52">
+      <c r="I19" s="51">
         <f>$H$18/H19</f>
         <v>7.1454556458934366</v>
       </c>
@@ -6463,7 +6583,7 @@
         <f t="shared" si="9"/>
         <v>1264.05</v>
       </c>
-      <c r="I20" s="52">
+      <c r="I20" s="51">
         <f t="shared" ref="I20:I24" si="17">$H$18/H20</f>
         <v>14.009683161267354</v>
       </c>
@@ -6541,7 +6661,7 @@
         <f t="shared" si="9"/>
         <v>677.45</v>
       </c>
-      <c r="I21" s="52">
+      <c r="I21" s="51">
         <f t="shared" si="17"/>
         <v>26.140586021108565</v>
       </c>
@@ -6619,7 +6739,7 @@
         <f t="shared" si="9"/>
         <v>441</v>
       </c>
-      <c r="I22" s="52">
+      <c r="I22" s="51">
         <f t="shared" si="17"/>
         <v>40.15632653061224</v>
       </c>
@@ -6697,7 +6817,7 @@
         <f t="shared" si="9"/>
         <v>383.6</v>
       </c>
-      <c r="I23" s="52">
+      <c r="I23" s="51">
         <f t="shared" si="17"/>
         <v>46.165119916579762</v>
       </c>
@@ -6749,7 +6869,7 @@
       <c r="AA23" s="6">
         <v>46.04</v>
       </c>
-      <c r="AB23" s="42">
+      <c r="AB23" s="41">
         <f t="shared" si="13"/>
         <v>1546.04</v>
       </c>
@@ -6777,7 +6897,7 @@
         <f t="shared" ref="H24" si="21">F24*60+G24</f>
         <v>410.21</v>
       </c>
-      <c r="I24" s="52">
+      <c r="I24" s="51">
         <f t="shared" si="17"/>
         <v>43.170424904317301</v>
       </c>
@@ -6833,15 +6953,19 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C27" s="46" t="s">
-        <v>11</v>
+      <c r="C27" s="45" t="s">
+        <v>9</v>
       </c>
       <c r="O27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K28" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="58"/>
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
@@ -6849,45 +6973,55 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
         <v>17</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>18</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>19</v>
       </c>
-      <c r="G29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" t="s">
-        <v>21</v>
-      </c>
       <c r="I29" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="P29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="R29" s="6" t="s">
+      <c r="T29" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="S29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="T29" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
+      <c r="C30" s="2">
+        <f t="shared" ref="C30:C37" si="22">$M$53/D30/E30</f>
+        <v>4010210</v>
+      </c>
       <c r="D30">
         <v>1</v>
       </c>
@@ -6906,7 +7040,7 @@
         <v>69233.45</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P30">
         <v>1</v>
@@ -6918,7 +7052,7 @@
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
-        <f t="shared" ref="C31:C37" si="22">$M$53/D31/E31</f>
+        <f t="shared" si="22"/>
         <v>501276.25</v>
       </c>
       <c r="D31">
@@ -6943,8 +7077,16 @@
         <v>7.5381242623393474</v>
       </c>
       <c r="J31" s="27">
-        <f t="shared" ref="J31:J36" si="24">I31/E31</f>
+        <f>I31/E31</f>
         <v>0.94226553279241843</v>
+      </c>
+      <c r="K31" s="2">
+        <f>C31/$C$30*$H$30/H31</f>
+        <v>0.94226553279241843</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" ref="L31:L36" si="24">K31/E31</f>
+        <v>0.1177831915990523</v>
       </c>
       <c r="P31" s="6">
         <v>1</v>
@@ -6993,8 +7135,16 @@
         <v>15.843257282775351</v>
       </c>
       <c r="J32" s="27">
+        <f>I32/E32</f>
+        <v>0.99020358017345944</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" ref="K32:K36" si="27">C32/$C$30*$H$30/H32</f>
+        <v>0.49510179008672972</v>
+      </c>
+      <c r="L32" s="2">
         <f t="shared" si="24"/>
-        <v>0.99020358017345944</v>
+        <v>3.0943861880420608E-2</v>
       </c>
       <c r="P32" s="6">
         <v>2</v>
@@ -7033,7 +7183,7 @@
       <c r="G33">
         <v>24.53</v>
       </c>
-      <c r="H33" s="24">
+      <c r="H33" s="50">
         <f>F33*60+G33</f>
         <v>2124.5300000000002</v>
       </c>
@@ -7042,8 +7192,16 @@
         <v>32.587654681270678</v>
       </c>
       <c r="J33" s="27">
+        <f t="shared" ref="J31:J36" si="28">I33/E33</f>
+        <v>1.0183642087897087</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="27"/>
+        <v>0.25459105219742717</v>
+      </c>
+      <c r="L33" s="2">
         <f t="shared" si="24"/>
-        <v>1.0183642087897087</v>
+        <v>7.9559703811695991E-3</v>
       </c>
       <c r="O33" s="6"/>
       <c r="P33" s="6">
@@ -7087,12 +7245,20 @@
         <v>1216.44</v>
       </c>
       <c r="I34" s="27">
-        <f t="shared" ref="I34:I36" si="27">$H$30/H34</f>
+        <f t="shared" ref="I34:I36" si="29">$H$30/H34</f>
         <v>56.914808786294429</v>
       </c>
       <c r="J34" s="27">
+        <f t="shared" si="28"/>
+        <v>0.88929388728585046</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="27"/>
+        <v>0.11116173591073131</v>
+      </c>
+      <c r="L34" s="2">
         <f t="shared" si="24"/>
-        <v>0.88929388728585046</v>
+        <v>1.7369021236051767E-3</v>
       </c>
       <c r="O34" s="6"/>
       <c r="P34" s="6">
@@ -7132,16 +7298,24 @@
         <v>1.01</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" ref="H35:H36" si="28">F35*60+G35</f>
+        <f t="shared" ref="H35:H36" si="30">F35*60+G35</f>
         <v>781.01</v>
       </c>
       <c r="I35" s="27">
+        <f t="shared" si="29"/>
+        <v>88.646048065965857</v>
+      </c>
+      <c r="J35" s="27">
+        <f t="shared" si="28"/>
+        <v>0.69254725051535826</v>
+      </c>
+      <c r="K35" s="2">
         <f t="shared" si="27"/>
-        <v>88.646048065965857</v>
-      </c>
-      <c r="J35" s="27">
+        <v>4.3284203157209891E-2</v>
+      </c>
+      <c r="L35" s="2">
         <f t="shared" si="24"/>
-        <v>0.69254725051535826</v>
+        <v>3.3815783716570227E-4</v>
       </c>
       <c r="O35" s="6"/>
       <c r="P35" s="6">
@@ -7158,7 +7332,7 @@
         <v>46.78</v>
       </c>
       <c r="T35" s="6">
-        <f t="shared" ref="T35:T36" si="29">R35*60+S35</f>
+        <f t="shared" ref="T35:T36" si="31">R35*60+S35</f>
         <v>1246.78</v>
       </c>
     </row>
@@ -7182,16 +7356,24 @@
         <v>21.01</v>
       </c>
       <c r="H36" s="6">
+        <f t="shared" si="30"/>
+        <v>681.01</v>
+      </c>
+      <c r="I36" s="27">
+        <f t="shared" si="29"/>
+        <v>101.66289775480536</v>
+      </c>
+      <c r="J36" s="27">
         <f t="shared" si="28"/>
-        <v>681.01</v>
-      </c>
-      <c r="I36" s="27">
+        <v>0.39712069435470843</v>
+      </c>
+      <c r="K36" s="2">
         <f t="shared" si="27"/>
-        <v>101.66289775480536</v>
-      </c>
-      <c r="J36" s="27">
+        <v>1.2410021698584638E-2</v>
+      </c>
+      <c r="L36" s="2">
         <f t="shared" si="24"/>
-        <v>0.39712069435470843</v>
+        <v>4.8476647260096243E-5</v>
       </c>
       <c r="O36" s="6"/>
       <c r="P36" s="6">
@@ -7208,7 +7390,7 @@
         <v>28.038</v>
       </c>
       <c r="T36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>1108.038</v>
       </c>
     </row>
@@ -7238,38 +7420,38 @@
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M39" t="s">
+        <v>15</v>
+      </c>
+      <c r="N39" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" t="s">
         <v>17</v>
       </c>
-      <c r="N39" t="s">
+      <c r="P39" t="s">
         <v>18</v>
       </c>
-      <c r="O39" t="s">
+      <c r="Q39" t="s">
         <v>19</v>
-      </c>
-      <c r="P39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
       <c r="E40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F40" s="2"/>
       <c r="M40">
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" ref="N40:N46" si="30">M40*8</f>
+        <f t="shared" ref="N40:N46" si="32">M40*8</f>
         <v>8</v>
       </c>
       <c r="O40">
@@ -7285,7 +7467,7 @@
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D41" s="22">
         <f>L58</f>
@@ -7308,7 +7490,7 @@
         <v>2</v>
       </c>
       <c r="N41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>16</v>
       </c>
       <c r="O41">
@@ -7342,7 +7524,7 @@
         <v>4</v>
       </c>
       <c r="N42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>32</v>
       </c>
       <c r="O42">
@@ -7380,7 +7562,7 @@
         <v>8</v>
       </c>
       <c r="N43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>64</v>
       </c>
       <c r="O43">
@@ -7419,7 +7601,7 @@
         <v>16</v>
       </c>
       <c r="N44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>128</v>
       </c>
       <c r="O44">
@@ -7429,7 +7611,7 @@
         <v>41.149000000000001</v>
       </c>
       <c r="Q44" s="6">
-        <f t="shared" ref="Q44:Q45" si="31">O44*60+P44</f>
+        <f t="shared" ref="Q44:Q45" si="33">O44*60+P44</f>
         <v>1301.1489999999999</v>
       </c>
     </row>
@@ -7458,7 +7640,7 @@
         <v>32</v>
       </c>
       <c r="N45" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>256</v>
       </c>
       <c r="O45">
@@ -7468,7 +7650,7 @@
         <v>22.97</v>
       </c>
       <c r="Q45" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1162.97</v>
       </c>
     </row>
@@ -7497,7 +7679,7 @@
         <v>64</v>
       </c>
       <c r="N46">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>512</v>
       </c>
     </row>
@@ -7531,7 +7713,7 @@
         <v>0</v>
       </c>
       <c r="M48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N48">
         <v>8</v>
@@ -7562,32 +7744,32 @@
       <c r="M49" s="2">
         <v>195102</v>
       </c>
-      <c r="N49" s="40">
-        <f t="shared" ref="N49:T49" si="32">$M$49/N$48</f>
+      <c r="N49" s="39">
+        <f t="shared" ref="N49:T49" si="34">$M$49/N$48</f>
         <v>24387.75</v>
       </c>
-      <c r="O49" s="41">
-        <f t="shared" si="32"/>
+      <c r="O49" s="40">
+        <f t="shared" si="34"/>
         <v>12193.875</v>
       </c>
       <c r="P49" s="27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>6096.9375</v>
       </c>
       <c r="Q49" s="27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>3048.46875</v>
       </c>
       <c r="R49" s="27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>1524.234375</v>
       </c>
       <c r="S49" s="27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>762.1171875</v>
       </c>
       <c r="T49" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>381.05859375</v>
       </c>
     </row>
@@ -7598,224 +7780,224 @@
       <c r="M50" s="2">
         <v>432919</v>
       </c>
-      <c r="N50" s="42">
-        <f t="shared" ref="N50:T50" si="33">$M$50/N$48</f>
+      <c r="N50" s="41">
+        <f t="shared" ref="N50:T50" si="35">$M$50/N$48</f>
         <v>54114.875</v>
       </c>
-      <c r="O50" s="40">
-        <f t="shared" si="33"/>
+      <c r="O50" s="39">
+        <f t="shared" si="35"/>
         <v>27057.4375</v>
       </c>
-      <c r="P50" s="41">
-        <f t="shared" si="33"/>
+      <c r="P50" s="40">
+        <f t="shared" si="35"/>
         <v>13528.71875</v>
       </c>
       <c r="Q50" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>6764.359375</v>
       </c>
       <c r="R50" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>3382.1796875</v>
       </c>
       <c r="S50" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1691.08984375</v>
       </c>
       <c r="T50" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>845.544921875</v>
       </c>
     </row>
     <row r="51" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L51" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M51" s="2">
         <v>1017573</v>
       </c>
-      <c r="N51" s="43">
-        <f t="shared" ref="N51:T51" si="34">$M$51/N$48</f>
+      <c r="N51" s="42">
+        <f t="shared" ref="N51:T51" si="36">$M$51/N$48</f>
         <v>127196.625</v>
       </c>
-      <c r="O51" s="42">
-        <f t="shared" si="34"/>
+      <c r="O51" s="41">
+        <f t="shared" si="36"/>
         <v>63598.3125</v>
       </c>
-      <c r="P51" s="40">
-        <f t="shared" si="34"/>
+      <c r="P51" s="39">
+        <f t="shared" si="36"/>
         <v>31799.15625</v>
       </c>
-      <c r="Q51" s="41">
-        <f t="shared" si="34"/>
+      <c r="Q51" s="40">
+        <f t="shared" si="36"/>
         <v>15899.578125</v>
       </c>
       <c r="R51" s="27">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>7949.7890625</v>
       </c>
       <c r="S51" s="27">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3974.89453125</v>
       </c>
       <c r="T51" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1987.447265625</v>
       </c>
     </row>
     <row r="52" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M52" s="2">
         <v>2037710</v>
       </c>
       <c r="N52" s="27">
-        <f t="shared" ref="N52:T52" si="35">$M$52/N$48</f>
+        <f t="shared" ref="N52:T52" si="37">$M$52/N$48</f>
         <v>254713.75</v>
       </c>
-      <c r="O52" s="43">
-        <f t="shared" si="35"/>
+      <c r="O52" s="42">
+        <f t="shared" si="37"/>
         <v>127356.875</v>
       </c>
-      <c r="P52" s="42">
-        <f t="shared" si="35"/>
+      <c r="P52" s="41">
+        <f t="shared" si="37"/>
         <v>63678.4375</v>
       </c>
-      <c r="Q52" s="40">
-        <f t="shared" si="35"/>
+      <c r="Q52" s="39">
+        <f t="shared" si="37"/>
         <v>31839.21875</v>
       </c>
-      <c r="R52" s="41">
-        <f t="shared" si="35"/>
+      <c r="R52" s="40">
+        <f t="shared" si="37"/>
         <v>15919.609375</v>
       </c>
       <c r="S52" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>7959.8046875</v>
       </c>
       <c r="T52" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>3979.90234375</v>
       </c>
     </row>
     <row r="53" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L53" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M53" s="2">
         <v>4010210</v>
       </c>
       <c r="N53" s="27">
-        <f t="shared" ref="N53:T53" si="36">$M$53/N$48</f>
+        <f t="shared" ref="N53:T53" si="38">$M$53/N$48</f>
         <v>501276.25</v>
       </c>
       <c r="O53" s="27">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>250638.125</v>
       </c>
-      <c r="P53" s="43">
-        <f t="shared" si="36"/>
+      <c r="P53" s="42">
+        <f t="shared" si="38"/>
         <v>125319.0625</v>
       </c>
-      <c r="Q53" s="42">
-        <f t="shared" si="36"/>
+      <c r="Q53" s="41">
+        <f t="shared" si="38"/>
         <v>62659.53125</v>
       </c>
-      <c r="R53" s="40">
-        <f t="shared" si="36"/>
+      <c r="R53" s="39">
+        <f t="shared" si="38"/>
         <v>31329.765625</v>
       </c>
-      <c r="S53" s="41">
-        <f t="shared" si="36"/>
+      <c r="S53" s="40">
+        <f t="shared" si="38"/>
         <v>15664.8828125</v>
       </c>
       <c r="T53" s="25">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>7832.44140625</v>
       </c>
     </row>
     <row r="54" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L54" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M54" s="15">
         <v>8101299</v>
       </c>
-      <c r="N54" s="44">
-        <f t="shared" ref="N54:T54" si="37">$M$54/N$48</f>
+      <c r="N54" s="43">
+        <f t="shared" ref="N54:T54" si="39">$M$54/N$48</f>
         <v>1012662.375</v>
       </c>
-      <c r="O54" s="44">
-        <f t="shared" si="37"/>
+      <c r="O54" s="43">
+        <f t="shared" si="39"/>
         <v>506331.1875</v>
       </c>
-      <c r="P54" s="44">
-        <f t="shared" si="37"/>
+      <c r="P54" s="43">
+        <f t="shared" si="39"/>
         <v>253165.59375</v>
       </c>
-      <c r="Q54" s="43">
-        <f t="shared" si="37"/>
+      <c r="Q54" s="42">
+        <f t="shared" si="39"/>
         <v>126582.796875</v>
       </c>
-      <c r="R54" s="42">
-        <f t="shared" si="37"/>
+      <c r="R54" s="41">
+        <f t="shared" si="39"/>
         <v>63291.3984375</v>
       </c>
-      <c r="S54" s="40">
-        <f t="shared" si="37"/>
+      <c r="S54" s="39">
+        <f t="shared" si="39"/>
         <v>31645.69921875</v>
       </c>
-      <c r="T54" s="41">
-        <f t="shared" si="37"/>
+      <c r="T54" s="40">
+        <f t="shared" si="39"/>
         <v>15822.849609375</v>
       </c>
     </row>
     <row r="55" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M55" s="15">
         <v>15522778</v>
       </c>
-      <c r="N55" s="44">
-        <f t="shared" ref="N55:T55" si="38">$M$55/N$48</f>
+      <c r="N55" s="43">
+        <f t="shared" ref="N55:T55" si="40">$M$55/N$48</f>
         <v>1940347.25</v>
       </c>
-      <c r="O55" s="44">
-        <f t="shared" si="38"/>
+      <c r="O55" s="43">
+        <f t="shared" si="40"/>
         <v>970173.625</v>
       </c>
-      <c r="P55" s="44">
-        <f t="shared" si="38"/>
+      <c r="P55" s="43">
+        <f t="shared" si="40"/>
         <v>485086.8125</v>
       </c>
-      <c r="Q55" s="44">
-        <f t="shared" si="38"/>
+      <c r="Q55" s="43">
+        <f t="shared" si="40"/>
         <v>242543.40625</v>
       </c>
-      <c r="R55" s="43">
-        <f t="shared" si="38"/>
+      <c r="R55" s="42">
+        <f t="shared" si="40"/>
         <v>121271.703125</v>
       </c>
-      <c r="S55" s="42">
-        <f t="shared" si="38"/>
+      <c r="S55" s="41">
+        <f t="shared" si="40"/>
         <v>60635.8515625</v>
       </c>
-      <c r="T55" s="40">
-        <f t="shared" si="38"/>
+      <c r="T55" s="39">
+        <f t="shared" si="40"/>
         <v>30317.92578125</v>
       </c>
     </row>
     <row r="57" spans="12:20" x14ac:dyDescent="0.25">
       <c r="L57" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N57" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="12:20" x14ac:dyDescent="0.25">
@@ -7878,7 +8060,7 @@
   <mergeCells count="3">
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="K28:L28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -7899,14 +8081,14 @@
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -7917,48 +8099,48 @@
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
         <v>4</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>4</v>
@@ -8226,7 +8408,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8237,24 +8419,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
       <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8386,7 +8568,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -8443,27 +8625,27 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>29</v>
-      </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -8552,7 +8734,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -8610,21 +8792,21 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
         <v>36</v>
       </c>
-      <c r="B41" t="s">
+      <c r="E41" t="s">
         <v>37</v>
-      </c>
-      <c r="D41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -8699,4 +8881,441 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:P32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4" s="62">
+        <v>144300</v>
+      </c>
+      <c r="D4" s="51">
+        <f>C4/60/60</f>
+        <v>40.083333333333336</v>
+      </c>
+      <c r="F4" s="62">
+        <v>140400</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>199</v>
+      </c>
+      <c r="C5" s="62">
+        <v>143600</v>
+      </c>
+      <c r="D5" s="51"/>
+      <c r="E5" s="2">
+        <f>C4-C5</f>
+        <v>700</v>
+      </c>
+      <c r="F5" s="62">
+        <v>139800</v>
+      </c>
+      <c r="H5" s="2">
+        <f>F4-F5</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>198</v>
+      </c>
+      <c r="C6" s="62">
+        <v>142900</v>
+      </c>
+      <c r="D6" s="51"/>
+      <c r="E6" s="2">
+        <f>C5-C6</f>
+        <v>700</v>
+      </c>
+      <c r="F6" s="62">
+        <v>139100</v>
+      </c>
+      <c r="H6" s="2">
+        <f>F5-F6</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>197</v>
+      </c>
+      <c r="C7" s="62">
+        <v>142200</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="2">
+        <f>C6-C7</f>
+        <v>700</v>
+      </c>
+      <c r="F7" s="62">
+        <v>138400</v>
+      </c>
+      <c r="H7" s="2">
+        <f>F6-F7</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>196</v>
+      </c>
+      <c r="C8" s="62">
+        <v>141600</v>
+      </c>
+      <c r="D8" s="51"/>
+      <c r="E8" s="2">
+        <f>C7-C8</f>
+        <v>600</v>
+      </c>
+      <c r="F8" s="62">
+        <v>137800</v>
+      </c>
+      <c r="H8" s="2">
+        <f>F7-F8</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>195</v>
+      </c>
+      <c r="C9" s="62">
+        <v>140900</v>
+      </c>
+      <c r="D9" s="51"/>
+      <c r="E9" s="2">
+        <f>C8-C9</f>
+        <v>700</v>
+      </c>
+      <c r="F9" s="62">
+        <v>137100</v>
+      </c>
+      <c r="H9" s="2">
+        <f>F8-F9</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>194</v>
+      </c>
+      <c r="C10" s="62">
+        <v>140200</v>
+      </c>
+      <c r="D10" s="51"/>
+      <c r="E10" s="2">
+        <f>C9-C10</f>
+        <v>700</v>
+      </c>
+      <c r="F10" s="62">
+        <v>136500</v>
+      </c>
+      <c r="H10" s="2">
+        <f>F9-F10</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>193</v>
+      </c>
+      <c r="C11" s="62">
+        <v>139500</v>
+      </c>
+      <c r="D11" s="51"/>
+      <c r="E11" s="2">
+        <f>C10-C11</f>
+        <v>700</v>
+      </c>
+      <c r="F11" s="62">
+        <v>135800</v>
+      </c>
+      <c r="H11" s="2">
+        <f>F10-F11</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>192</v>
+      </c>
+      <c r="C12" s="62"/>
+      <c r="D12" s="51"/>
+      <c r="F12" s="62">
+        <v>135200</v>
+      </c>
+      <c r="H12" s="2">
+        <f>F11-F12</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>191</v>
+      </c>
+      <c r="C13" s="62"/>
+      <c r="D13" s="51"/>
+      <c r="F13" s="62">
+        <v>134500</v>
+      </c>
+      <c r="H13" s="2">
+        <f>F12-F13</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>B13-1</f>
+        <v>190</v>
+      </c>
+      <c r="C14" s="62"/>
+      <c r="F14" s="62"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <f t="shared" ref="B15:B21" si="0">B14-1</f>
+        <v>189</v>
+      </c>
+      <c r="C15" s="62"/>
+      <c r="F15" s="62"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>188</v>
+      </c>
+      <c r="C16" s="62"/>
+      <c r="F16" s="62"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="C17" s="62"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+      <c r="C18" s="62"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="C19" s="62"/>
+      <c r="K19" s="62">
+        <v>104100</v>
+      </c>
+      <c r="O19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="C20" s="62"/>
+      <c r="K20" s="62">
+        <v>103500</v>
+      </c>
+      <c r="M20" s="2">
+        <f>K19-K20</f>
+        <v>600</v>
+      </c>
+      <c r="O20">
+        <v>200</v>
+      </c>
+      <c r="P20" s="2">
+        <f>O20*AVERAGE(M20:M28)</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <f t="shared" si="0"/>
+        <v>183</v>
+      </c>
+      <c r="C21" s="62"/>
+      <c r="K21" s="62">
+        <v>103000</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" ref="M21:M28" si="1">K20-K21</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <f>B21-1</f>
+        <v>182</v>
+      </c>
+      <c r="C22" s="62"/>
+      <c r="K22" s="62">
+        <v>102400</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <f t="shared" ref="B23:B32" si="2">B22-1</f>
+        <v>181</v>
+      </c>
+      <c r="K23" s="62">
+        <v>101900</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="K24" s="62">
+        <v>101300</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+      <c r="K25" s="62">
+        <v>100800</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+      <c r="K26" s="62">
+        <v>100300</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+      <c r="K27" s="62">
+        <v>99700</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+      <c r="K28" s="62">
+        <v>99150</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="K29" s="62"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+      <c r="K30" s="62"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="K31" s="62"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="K32" s="62"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Small fixes in xlsx file. Removed the discussion about the costs
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HSR Cluster" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -537,6 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -3628,8 +3629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4:Y9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3649,10 +3650,10 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="58" t="s">
+      <c r="R3" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="58"/>
+      <c r="S3" s="59"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -4113,10 +4114,10 @@
       <c r="P12" t="s">
         <v>58</v>
       </c>
-      <c r="R12" s="58" t="s">
+      <c r="R12" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="58"/>
+      <c r="S12" s="59"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -4569,10 +4570,10 @@
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
-      <c r="R21" s="55" t="s">
+      <c r="R21" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="S21" s="55"/>
+      <c r="S21" s="56"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
@@ -4662,7 +4663,7 @@
         <v>55036.17</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="J23" s="63" t="s">
+      <c r="J23" s="64" t="s">
         <v>71</v>
       </c>
       <c r="K23" s="2">
@@ -4672,9 +4673,9 @@
       <c r="L23" s="6">
         <v>1</v>
       </c>
-      <c r="O23" s="51">
+      <c r="O23" s="52">
         <f>Sheet1!P20</f>
-        <v>110000</v>
+        <v>110142.85714285713</v>
       </c>
       <c r="U23" s="28" t="s">
         <v>63</v>
@@ -4729,19 +4730,19 @@
       </c>
       <c r="P24" s="27">
         <f>$O$23/O24</f>
-        <v>2.8907286186600736</v>
+        <v>2.8944828116713199</v>
       </c>
       <c r="Q24" s="27">
         <f t="shared" ref="Q24:Q29" si="28">P24/L24</f>
-        <v>0.48178810311001224</v>
+        <v>0.48241380194521999</v>
       </c>
       <c r="R24" s="27">
         <f>K24/$K$23*$O$23/O24</f>
-        <v>0.48178810311001224</v>
+        <v>0.48241380194521999</v>
       </c>
       <c r="S24" s="38">
         <f>R24/L24</f>
-        <v>8.0298017185002041E-2</v>
+        <v>8.0402300324203327E-2</v>
       </c>
       <c r="V24" s="6">
         <v>6</v>
@@ -4804,19 +4805,19 @@
       </c>
       <c r="P25" s="27">
         <f t="shared" ref="P25:P29" si="31">$O$23/O25</f>
-        <v>5.8793692398884199</v>
+        <v>5.8870047843558062</v>
       </c>
       <c r="Q25" s="27">
         <f t="shared" si="28"/>
-        <v>0.48994743665736834</v>
+        <v>0.4905837320296505</v>
       </c>
       <c r="R25" s="27">
         <f t="shared" ref="R25:R29" si="32">K25/$K$23*$O$23/O25</f>
-        <v>0.48994743665736828</v>
+        <v>0.49058373202965055</v>
       </c>
       <c r="S25" s="38">
         <f t="shared" ref="S25:S29" si="33">R25/L25</f>
-        <v>4.0828953054780688E-2</v>
+        <v>4.0881977669137544E-2</v>
       </c>
       <c r="V25" s="6">
         <v>12</v>
@@ -4879,19 +4880,19 @@
       </c>
       <c r="P26" s="27">
         <f t="shared" si="31"/>
-        <v>12.187096302434981</v>
+        <v>12.20292370023035</v>
       </c>
       <c r="Q26" s="27">
         <f t="shared" si="28"/>
-        <v>0.50779567926812419</v>
+        <v>0.50845515417626463</v>
       </c>
       <c r="R26" s="27">
         <f t="shared" si="32"/>
-        <v>0.50779567926812419</v>
+        <v>0.50845515417626452</v>
       </c>
       <c r="S26" s="38">
         <f t="shared" si="33"/>
-        <v>2.1158153302838507E-2</v>
+        <v>2.1185631424011021E-2</v>
       </c>
       <c r="V26" s="6">
         <v>24</v>
@@ -4953,19 +4954,19 @@
       </c>
       <c r="P27" s="27">
         <f t="shared" si="31"/>
-        <v>19.658759675237288</v>
+        <v>19.684290531958375</v>
       </c>
       <c r="Q27" s="27">
         <f t="shared" si="28"/>
-        <v>0.54607665764548019</v>
+        <v>0.5467858481099549</v>
       </c>
       <c r="R27" s="27">
         <f t="shared" si="32"/>
-        <v>0.5460766576454803</v>
+        <v>0.5467858481099549</v>
       </c>
       <c r="S27" s="38">
         <f t="shared" si="33"/>
-        <v>1.5168796045707787E-2</v>
+        <v>1.5188495780832081E-2</v>
       </c>
       <c r="V27" s="6">
         <v>36</v>
@@ -5026,19 +5027,19 @@
       </c>
       <c r="P28" s="27">
         <f t="shared" si="31"/>
-        <v>24.691080908182848</v>
+        <v>24.723147247024642</v>
       </c>
       <c r="Q28" s="27">
         <f t="shared" si="28"/>
-        <v>0.51439751892047603</v>
+        <v>0.5150655676463467</v>
       </c>
       <c r="R28" s="27">
         <f t="shared" si="32"/>
-        <v>0.51439751892047592</v>
+        <v>0.5150655676463467</v>
       </c>
       <c r="S28" s="38">
         <f t="shared" si="33"/>
-        <v>1.0716614977509914E-2</v>
+        <v>1.0730532659298889E-2</v>
       </c>
       <c r="V28" s="6">
         <v>48</v>
@@ -5099,19 +5100,19 @@
       </c>
       <c r="P29" s="27">
         <f t="shared" si="31"/>
-        <v>30.801281333303464</v>
+        <v>30.841282997372687</v>
       </c>
       <c r="Q29" s="27">
         <f t="shared" si="28"/>
-        <v>0.51335468888839109</v>
+        <v>0.51402138328954483</v>
       </c>
       <c r="R29" s="27">
         <f t="shared" si="32"/>
-        <v>0.51335468888839109</v>
+        <v>0.51402138328954472</v>
       </c>
       <c r="S29" s="38">
         <f t="shared" si="33"/>
-        <v>8.5559114814731854E-3</v>
+        <v>8.5670230548257446E-3</v>
       </c>
       <c r="V29" s="6">
         <v>60</v>
@@ -5161,15 +5162,15 @@
       <c r="B33" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="44">
+      <c r="C33" s="45">
         <f>C39</f>
         <v>38361.1875</v>
       </c>
-      <c r="D33" s="44">
+      <c r="D33" s="45">
         <f>D39</f>
         <v>81350.385416666672</v>
       </c>
-      <c r="E33" s="44">
+      <c r="E33" s="45">
         <f>E39</f>
         <v>167393.88333333333</v>
       </c>
@@ -5640,8 +5641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5668,10 +5669,10 @@
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="46" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="6"/>
@@ -5685,20 +5686,20 @@
       <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="55"/>
       <c r="T4" s="6"/>
-      <c r="U4" s="59" t="s">
+      <c r="U4" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="V4" s="52"/>
-      <c r="W4" s="60" t="s">
+      <c r="V4" s="53"/>
+      <c r="W4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="X4" s="60"/>
+      <c r="X4" s="61"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -5749,10 +5750,10 @@
       <c r="T5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="46" t="s">
+      <c r="U5" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="V5" s="46" t="s">
+      <c r="V5" s="47" t="s">
         <v>54</v>
       </c>
       <c r="W5" s="36" t="s">
@@ -5805,8 +5806,8 @@
         <f>R6*60+S6</f>
         <v>6595.97</v>
       </c>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
       <c r="W6" s="36"/>
       <c r="X6" s="36"/>
     </row>
@@ -5840,11 +5841,11 @@
         <f>I7/E7</f>
         <v>0.13381537242472266</v>
       </c>
-      <c r="K7" s="57">
+      <c r="K7" s="58">
         <f>C7/$C$6*$H$6/H7</f>
         <v>0.13381537242472266</v>
       </c>
-      <c r="L7" s="57">
+      <c r="L7" s="58">
         <f t="shared" ref="L7:L12" si="3">K7/E7</f>
         <v>1.6726921553090333E-2</v>
       </c>
@@ -5869,19 +5870,19 @@
         <f>R7*60+S7</f>
         <v>986.61</v>
       </c>
-      <c r="U7" s="47">
+      <c r="U7" s="48">
         <f>$T$6/T7</f>
         <v>6.6854886936074029</v>
       </c>
-      <c r="V7" s="47">
+      <c r="V7" s="48">
         <f>U7/Q7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="W7" s="57">
+      <c r="W7" s="58">
         <f>O7/$O$6*$T$6/T7</f>
         <v>0.83568608670092537</v>
       </c>
-      <c r="X7" s="49">
+      <c r="X7" s="50">
         <f>W7/Q7</f>
         <v>0.10446076083761567</v>
       </c>
@@ -5916,11 +5917,11 @@
         <f t="shared" ref="J8:J12" si="5">I8/E8</f>
         <v>8.0647086914995211E-2</v>
       </c>
-      <c r="K8" s="57">
+      <c r="K8" s="58">
         <f t="shared" ref="K8:K11" si="6">C8/$C$6*$H$6/H8</f>
         <v>8.0647086914995211E-2</v>
       </c>
-      <c r="L8" s="57">
+      <c r="L8" s="58">
         <f t="shared" si="3"/>
         <v>5.0404429321872007E-3</v>
       </c>
@@ -5945,19 +5946,19 @@
         <f>R8*60+S8</f>
         <v>518.11900000000003</v>
       </c>
-      <c r="U8" s="47">
+      <c r="U8" s="48">
         <f>$T$6/T8</f>
         <v>12.730608219347292</v>
       </c>
-      <c r="V8" s="47">
+      <c r="V8" s="48">
         <f>U8/Q8</f>
         <v>0.79566301370920578</v>
       </c>
-      <c r="W8" s="57">
+      <c r="W8" s="58">
         <f>O8/$O$6*$T$6/T8</f>
         <v>0.79566301370920578</v>
       </c>
-      <c r="X8" s="49">
+      <c r="X8" s="50">
         <f>W8/Q8</f>
         <v>4.9728938356825361E-2</v>
       </c>
@@ -5992,11 +5993,11 @@
         <f t="shared" si="5"/>
         <v>3.5718062605752957E-2</v>
       </c>
-      <c r="K9" s="57">
+      <c r="K9" s="58">
         <f t="shared" si="6"/>
         <v>3.5718062605752957E-2</v>
       </c>
-      <c r="L9" s="57">
+      <c r="L9" s="58">
         <f t="shared" si="3"/>
         <v>1.1161894564297799E-3</v>
       </c>
@@ -6021,19 +6022,19 @@
         <f>R9*60+S9</f>
         <v>307.14999999999998</v>
       </c>
-      <c r="U9" s="47">
+      <c r="U9" s="48">
         <f>$T$6/T9</f>
         <v>21.474751749959307</v>
       </c>
-      <c r="V9" s="47">
+      <c r="V9" s="48">
         <f>U9/Q9</f>
         <v>0.67108599218622833</v>
       </c>
-      <c r="W9" s="57">
+      <c r="W9" s="58">
         <f>O9/$O$6*$T$6/T9</f>
         <v>0.67108599218622833</v>
       </c>
-      <c r="X9" s="49">
+      <c r="X9" s="50">
         <f>W9/Q9</f>
         <v>2.0971437255819635E-2</v>
       </c>
@@ -6068,11 +6069,11 @@
         <f t="shared" si="5"/>
         <v>1.3226425438596491E-2</v>
       </c>
-      <c r="K10" s="57">
+      <c r="K10" s="58">
         <f t="shared" si="6"/>
         <v>1.3226425438596491E-2</v>
       </c>
-      <c r="L10" s="57">
+      <c r="L10" s="58">
         <f t="shared" si="3"/>
         <v>2.0666289747807017E-4</v>
       </c>
@@ -6097,19 +6098,19 @@
         <f>R10*60+S10</f>
         <v>252.13</v>
       </c>
-      <c r="U10" s="47">
+      <c r="U10" s="48">
         <f>$T$6/T10</f>
         <v>26.160988379010828</v>
       </c>
-      <c r="V10" s="48">
+      <c r="V10" s="49">
         <f>U10/Q10</f>
         <v>0.40876544342204418</v>
       </c>
-      <c r="W10" s="57">
+      <c r="W10" s="58">
         <f>O10/$O$6*$T$6/T10</f>
         <v>0.40876544342204418</v>
       </c>
-      <c r="X10" s="49">
+      <c r="X10" s="50">
         <f>W10/Q10</f>
         <v>6.3869600534694404E-3</v>
       </c>
@@ -6144,11 +6145,11 @@
         <f t="shared" si="5"/>
         <v>4.1652279005524864E-3</v>
       </c>
-      <c r="K11" s="57">
+      <c r="K11" s="58">
         <f t="shared" si="6"/>
         <v>4.1652279005524864E-3</v>
       </c>
-      <c r="L11" s="57">
+      <c r="L11" s="58">
         <f t="shared" si="3"/>
         <v>3.25408429730663E-5</v>
       </c>
@@ -6174,19 +6175,19 @@
         <f>R11*60+S11</f>
         <v>216.96</v>
       </c>
-      <c r="U11" s="47">
+      <c r="U11" s="48">
         <f>$T$6/T11</f>
         <v>30.40177912979351</v>
       </c>
-      <c r="V11" s="47">
+      <c r="V11" s="48">
         <f>U11/Q11</f>
         <v>0.2375138994515118</v>
       </c>
-      <c r="W11" s="57">
+      <c r="W11" s="58">
         <f>O11/$O$6*$T$6/T11</f>
         <v>0.2375138994515118</v>
       </c>
-      <c r="X11" s="49">
+      <c r="X11" s="50">
         <f>W11/Q11</f>
         <v>1.8555773394649359E-3</v>
       </c>
@@ -6222,11 +6223,11 @@
         <f t="shared" si="5"/>
         <v>1.1840573816468477E-3</v>
       </c>
-      <c r="K12" s="57">
+      <c r="K12" s="58">
         <f>C12/$C$6*$H$6/H12</f>
         <v>1.1840573816468477E-3</v>
       </c>
-      <c r="L12" s="57">
+      <c r="L12" s="58">
         <f t="shared" si="3"/>
         <v>4.6252241470579987E-6</v>
       </c>
@@ -6252,19 +6253,19 @@
         <f>R12*60+S12</f>
         <v>296.72000000000003</v>
       </c>
-      <c r="U12" s="47">
+      <c r="U12" s="48">
         <f>$T$6/T12</f>
         <v>22.229610407117821</v>
       </c>
-      <c r="V12" s="47">
+      <c r="V12" s="48">
         <f>U12/Q12</f>
         <v>8.683441565280399E-2</v>
       </c>
-      <c r="W12" s="57">
+      <c r="W12" s="58">
         <f>O12/$O$6*$T$6/T12</f>
         <v>8.683441565280399E-2</v>
       </c>
-      <c r="X12" s="49">
+      <c r="X12" s="50">
         <f>W12/Q12</f>
         <v>3.3919693614376558E-4</v>
       </c>
@@ -6314,10 +6315,10 @@
       <c r="AB14" s="6"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="O15" s="45" t="s">
+      <c r="O15" s="46" t="s">
         <v>8</v>
       </c>
       <c r="W15" s="6"/>
@@ -6328,14 +6329,14 @@
       <c r="AB15" s="6"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="I16" s="58" t="s">
+      <c r="I16" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58" t="s">
+      <c r="J16" s="59"/>
+      <c r="K16" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="58"/>
+      <c r="L16" s="59"/>
       <c r="P16" t="s">
         <v>15</v>
       </c>
@@ -6501,11 +6502,11 @@
       <c r="G19">
         <v>18.350000000000001</v>
       </c>
-      <c r="H19" s="50">
+      <c r="H19" s="51">
         <f t="shared" si="9"/>
         <v>2478.35</v>
       </c>
-      <c r="I19" s="51">
+      <c r="I19" s="52">
         <f>$H$18/H19</f>
         <v>7.1454556458934366</v>
       </c>
@@ -6583,7 +6584,7 @@
         <f t="shared" si="9"/>
         <v>1264.05</v>
       </c>
-      <c r="I20" s="51">
+      <c r="I20" s="52">
         <f t="shared" ref="I20:I24" si="17">$H$18/H20</f>
         <v>14.009683161267354</v>
       </c>
@@ -6661,7 +6662,7 @@
         <f t="shared" si="9"/>
         <v>677.45</v>
       </c>
-      <c r="I21" s="51">
+      <c r="I21" s="52">
         <f t="shared" si="17"/>
         <v>26.140586021108565</v>
       </c>
@@ -6739,7 +6740,7 @@
         <f t="shared" si="9"/>
         <v>441</v>
       </c>
-      <c r="I22" s="51">
+      <c r="I22" s="52">
         <f t="shared" si="17"/>
         <v>40.15632653061224</v>
       </c>
@@ -6817,7 +6818,7 @@
         <f t="shared" si="9"/>
         <v>383.6</v>
       </c>
-      <c r="I23" s="51">
+      <c r="I23" s="52">
         <f t="shared" si="17"/>
         <v>46.165119916579762</v>
       </c>
@@ -6869,7 +6870,7 @@
       <c r="AA23" s="6">
         <v>46.04</v>
       </c>
-      <c r="AB23" s="41">
+      <c r="AB23" s="42">
         <f t="shared" si="13"/>
         <v>1546.04</v>
       </c>
@@ -6897,7 +6898,7 @@
         <f t="shared" ref="H24" si="21">F24*60+G24</f>
         <v>410.21</v>
       </c>
-      <c r="I24" s="51">
+      <c r="I24" s="52">
         <f t="shared" si="17"/>
         <v>43.170424904317301</v>
       </c>
@@ -6953,7 +6954,7 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="46" t="s">
         <v>9</v>
       </c>
       <c r="O27" t="s">
@@ -6962,10 +6963,10 @@
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="K28" s="58" t="s">
+      <c r="K28" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="L28" s="58"/>
+      <c r="L28" s="59"/>
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
@@ -7039,7 +7040,7 @@
         <f>F30*60+G30</f>
         <v>69233.45</v>
       </c>
-      <c r="O30" s="26" t="s">
+      <c r="O30" s="39" t="s">
         <v>64</v>
       </c>
       <c r="P30">
@@ -7183,7 +7184,7 @@
       <c r="G33">
         <v>24.53</v>
       </c>
-      <c r="H33" s="50">
+      <c r="H33" s="51">
         <f>F33*60+G33</f>
         <v>2124.5300000000002</v>
       </c>
@@ -7744,11 +7745,11 @@
       <c r="M49" s="2">
         <v>195102</v>
       </c>
-      <c r="N49" s="39">
+      <c r="N49" s="40">
         <f t="shared" ref="N49:T49" si="34">$M$49/N$48</f>
         <v>24387.75</v>
       </c>
-      <c r="O49" s="40">
+      <c r="O49" s="41">
         <f t="shared" si="34"/>
         <v>12193.875</v>
       </c>
@@ -7780,15 +7781,15 @@
       <c r="M50" s="2">
         <v>432919</v>
       </c>
-      <c r="N50" s="41">
+      <c r="N50" s="42">
         <f t="shared" ref="N50:T50" si="35">$M$50/N$48</f>
         <v>54114.875</v>
       </c>
-      <c r="O50" s="39">
+      <c r="O50" s="40">
         <f t="shared" si="35"/>
         <v>27057.4375</v>
       </c>
-      <c r="P50" s="40">
+      <c r="P50" s="41">
         <f t="shared" si="35"/>
         <v>13528.71875</v>
       </c>
@@ -7816,19 +7817,19 @@
       <c r="M51" s="2">
         <v>1017573</v>
       </c>
-      <c r="N51" s="42">
+      <c r="N51" s="43">
         <f t="shared" ref="N51:T51" si="36">$M$51/N$48</f>
         <v>127196.625</v>
       </c>
-      <c r="O51" s="41">
+      <c r="O51" s="42">
         <f t="shared" si="36"/>
         <v>63598.3125</v>
       </c>
-      <c r="P51" s="39">
+      <c r="P51" s="40">
         <f t="shared" si="36"/>
         <v>31799.15625</v>
       </c>
-      <c r="Q51" s="40">
+      <c r="Q51" s="41">
         <f t="shared" si="36"/>
         <v>15899.578125</v>
       </c>
@@ -7856,19 +7857,19 @@
         <f t="shared" ref="N52:T52" si="37">$M$52/N$48</f>
         <v>254713.75</v>
       </c>
-      <c r="O52" s="42">
+      <c r="O52" s="43">
         <f t="shared" si="37"/>
         <v>127356.875</v>
       </c>
-      <c r="P52" s="41">
+      <c r="P52" s="42">
         <f t="shared" si="37"/>
         <v>63678.4375</v>
       </c>
-      <c r="Q52" s="39">
+      <c r="Q52" s="40">
         <f t="shared" si="37"/>
         <v>31839.21875</v>
       </c>
-      <c r="R52" s="40">
+      <c r="R52" s="41">
         <f t="shared" si="37"/>
         <v>15919.609375</v>
       </c>
@@ -7896,19 +7897,19 @@
         <f t="shared" si="38"/>
         <v>250638.125</v>
       </c>
-      <c r="P53" s="42">
+      <c r="P53" s="43">
         <f t="shared" si="38"/>
         <v>125319.0625</v>
       </c>
-      <c r="Q53" s="41">
+      <c r="Q53" s="42">
         <f t="shared" si="38"/>
         <v>62659.53125</v>
       </c>
-      <c r="R53" s="39">
+      <c r="R53" s="40">
         <f t="shared" si="38"/>
         <v>31329.765625</v>
       </c>
-      <c r="S53" s="40">
+      <c r="S53" s="41">
         <f t="shared" si="38"/>
         <v>15664.8828125</v>
       </c>
@@ -7924,31 +7925,31 @@
       <c r="M54" s="15">
         <v>8101299</v>
       </c>
-      <c r="N54" s="43">
+      <c r="N54" s="44">
         <f t="shared" ref="N54:T54" si="39">$M$54/N$48</f>
         <v>1012662.375</v>
       </c>
-      <c r="O54" s="43">
+      <c r="O54" s="44">
         <f t="shared" si="39"/>
         <v>506331.1875</v>
       </c>
-      <c r="P54" s="43">
+      <c r="P54" s="44">
         <f t="shared" si="39"/>
         <v>253165.59375</v>
       </c>
-      <c r="Q54" s="42">
+      <c r="Q54" s="43">
         <f t="shared" si="39"/>
         <v>126582.796875</v>
       </c>
-      <c r="R54" s="41">
+      <c r="R54" s="42">
         <f t="shared" si="39"/>
         <v>63291.3984375</v>
       </c>
-      <c r="S54" s="39">
+      <c r="S54" s="40">
         <f t="shared" si="39"/>
         <v>31645.69921875</v>
       </c>
-      <c r="T54" s="40">
+      <c r="T54" s="41">
         <f t="shared" si="39"/>
         <v>15822.849609375</v>
       </c>
@@ -7960,31 +7961,31 @@
       <c r="M55" s="15">
         <v>15522778</v>
       </c>
-      <c r="N55" s="43">
+      <c r="N55" s="44">
         <f t="shared" ref="N55:T55" si="40">$M$55/N$48</f>
         <v>1940347.25</v>
       </c>
-      <c r="O55" s="43">
+      <c r="O55" s="44">
         <f t="shared" si="40"/>
         <v>970173.625</v>
       </c>
-      <c r="P55" s="43">
+      <c r="P55" s="44">
         <f t="shared" si="40"/>
         <v>485086.8125</v>
       </c>
-      <c r="Q55" s="43">
+      <c r="Q55" s="44">
         <f t="shared" si="40"/>
         <v>242543.40625</v>
       </c>
-      <c r="R55" s="42">
+      <c r="R55" s="43">
         <f t="shared" si="40"/>
         <v>121271.703125</v>
       </c>
-      <c r="S55" s="41">
+      <c r="S55" s="42">
         <f t="shared" si="40"/>
         <v>60635.8515625</v>
       </c>
-      <c r="T55" s="39">
+      <c r="T55" s="40">
         <f t="shared" si="40"/>
         <v>30317.92578125</v>
       </c>
@@ -8885,10 +8886,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P32"/>
+  <dimension ref="B3:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8903,7 +8904,7 @@
       <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="62" t="s">
         <v>65</v>
       </c>
       <c r="D3" t="s">
@@ -8929,14 +8930,14 @@
       <c r="B4">
         <v>200</v>
       </c>
-      <c r="C4" s="62">
+      <c r="C4" s="63">
         <v>144300</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="52">
         <f>C4/60/60</f>
         <v>40.083333333333336</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="63">
         <v>140400</v>
       </c>
       <c r="H4" s="6"/>
@@ -8945,15 +8946,15 @@
       <c r="B5">
         <v>199</v>
       </c>
-      <c r="C5" s="62">
+      <c r="C5" s="63">
         <v>143600</v>
       </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="2">
         <f>C4-C5</f>
         <v>700</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="63">
         <v>139800</v>
       </c>
       <c r="H5" s="2">
@@ -8965,15 +8966,15 @@
       <c r="B6">
         <v>198</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="63">
         <v>142900</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2">
         <f>C5-C6</f>
         <v>700</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="63">
         <v>139100</v>
       </c>
       <c r="H6" s="2">
@@ -8985,15 +8986,15 @@
       <c r="B7">
         <v>197</v>
       </c>
-      <c r="C7" s="62">
+      <c r="C7" s="63">
         <v>142200</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="2">
         <f>C6-C7</f>
         <v>700</v>
       </c>
-      <c r="F7" s="62">
+      <c r="F7" s="63">
         <v>138400</v>
       </c>
       <c r="H7" s="2">
@@ -9005,15 +9006,15 @@
       <c r="B8">
         <v>196</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="63">
         <v>141600</v>
       </c>
-      <c r="D8" s="51"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="2">
         <f>C7-C8</f>
         <v>600</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="63">
         <v>137800</v>
       </c>
       <c r="H8" s="2">
@@ -9025,15 +9026,15 @@
       <c r="B9">
         <v>195</v>
       </c>
-      <c r="C9" s="62">
+      <c r="C9" s="63">
         <v>140900</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="2">
         <f>C8-C9</f>
         <v>700</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="63">
         <v>137100</v>
       </c>
       <c r="H9" s="2">
@@ -9045,15 +9046,15 @@
       <c r="B10">
         <v>194</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C10" s="63">
         <v>140200</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="2">
         <f>C9-C10</f>
         <v>700</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="63">
         <v>136500</v>
       </c>
       <c r="H10" s="2">
@@ -9065,15 +9066,15 @@
       <c r="B11">
         <v>193</v>
       </c>
-      <c r="C11" s="62">
+      <c r="C11" s="63">
         <v>139500</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="2">
         <f>C10-C11</f>
         <v>700</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="63">
         <v>135800</v>
       </c>
       <c r="H11" s="2">
@@ -9085,9 +9086,9 @@
       <c r="B12">
         <v>192</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="51"/>
-      <c r="F12" s="62">
+      <c r="C12" s="63"/>
+      <c r="D12" s="52"/>
+      <c r="F12" s="63">
         <v>135200</v>
       </c>
       <c r="H12" s="2">
@@ -9099,9 +9100,9 @@
       <c r="B13">
         <v>191</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="51"/>
-      <c r="F13" s="62">
+      <c r="C13" s="63"/>
+      <c r="D13" s="52"/>
+      <c r="F13" s="63">
         <v>134500</v>
       </c>
       <c r="H13" s="2">
@@ -9114,46 +9115,46 @@
         <f>B13-1</f>
         <v>190</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="F14" s="62"/>
+      <c r="C14" s="63"/>
+      <c r="F14" s="63"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <f t="shared" ref="B15:B21" si="0">B14-1</f>
         <v>189</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="C15" s="63"/>
+      <c r="F15" s="63"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
         <v>188</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="C16" s="63"/>
+      <c r="F16" s="63"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <f t="shared" si="0"/>
         <v>187</v>
       </c>
-      <c r="C17" s="62"/>
+      <c r="C17" s="63"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="63"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
         <f t="shared" si="0"/>
         <v>185</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="K19" s="62">
+      <c r="C19" s="63"/>
+      <c r="K19" s="63">
         <v>104100</v>
       </c>
       <c r="O19" t="s">
@@ -9165,8 +9166,8 @@
         <f t="shared" si="0"/>
         <v>184</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="K20" s="62">
+      <c r="C20" s="63"/>
+      <c r="K20" s="63">
         <v>103500</v>
       </c>
       <c r="M20" s="2">
@@ -9177,8 +9178,8 @@
         <v>200</v>
       </c>
       <c r="P20" s="2">
-        <f>O20*AVERAGE(M20:M28)</f>
-        <v>110000</v>
+        <f>O20*AVERAGE(M20:M33)</f>
+        <v>110142.85714285713</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -9186,12 +9187,12 @@
         <f t="shared" si="0"/>
         <v>183</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="K21" s="62">
+      <c r="C21" s="63"/>
+      <c r="K21" s="63">
         <v>103000</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" ref="M21:M28" si="1">K20-K21</f>
+        <f t="shared" ref="M21:M33" si="1">K20-K21</f>
         <v>500</v>
       </c>
     </row>
@@ -9200,8 +9201,8 @@
         <f>B21-1</f>
         <v>182</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="K22" s="62">
+      <c r="C22" s="63"/>
+      <c r="K22" s="63">
         <v>102400</v>
       </c>
       <c r="M22" s="2">
@@ -9214,7 +9215,7 @@
         <f t="shared" ref="B23:B32" si="2">B22-1</f>
         <v>181</v>
       </c>
-      <c r="K23" s="62">
+      <c r="K23" s="63">
         <v>101900</v>
       </c>
       <c r="M23" s="2">
@@ -9227,7 +9228,7 @@
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="K24" s="62">
+      <c r="K24" s="63">
         <v>101300</v>
       </c>
       <c r="M24" s="2">
@@ -9240,7 +9241,7 @@
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
-      <c r="K25" s="62">
+      <c r="K25" s="63">
         <v>100800</v>
       </c>
       <c r="M25" s="2">
@@ -9253,7 +9254,7 @@
         <f t="shared" si="2"/>
         <v>178</v>
       </c>
-      <c r="K26" s="62">
+      <c r="K26" s="63">
         <v>100300</v>
       </c>
       <c r="M26" s="2">
@@ -9266,7 +9267,7 @@
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
-      <c r="K27" s="62">
+      <c r="K27" s="63">
         <v>99700</v>
       </c>
       <c r="M27" s="2">
@@ -9279,7 +9280,7 @@
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="K28" s="62">
+      <c r="K28" s="63">
         <v>99150</v>
       </c>
       <c r="M28" s="2">
@@ -9292,28 +9293,61 @@
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
-      <c r="K29" s="62"/>
+      <c r="K29" s="63">
+        <v>98600</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
-      <c r="K30" s="62"/>
+      <c r="K30" s="63">
+        <v>98060</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="1"/>
+        <v>540</v>
+      </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
-      <c r="K31" s="62"/>
+      <c r="K31" s="63">
+        <v>97500</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <f t="shared" si="2"/>
         <v>172</v>
       </c>
-      <c r="K32" s="62"/>
+      <c r="K32" s="63">
+        <v>96940</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="2">
+        <v>96390</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Weak scaling graphs, architecture graph
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="474" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="321" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HSR Cluster" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="66">
   <si>
     <t>pipe01</t>
   </si>
@@ -192,52 +192,13 @@
     <t>also</t>
   </si>
   <si>
-    <t>HSR strong scaling</t>
+    <t>HSR</t>
   </si>
   <si>
-    <t>Cores</t>
+    <t>size</t>
   </si>
   <si>
-    <t>pipe2</t>
-  </si>
-  <si>
-    <t>pipe6</t>
-  </si>
-  <si>
-    <t>pipe4</t>
-  </si>
-  <si>
-    <t>pipe5</t>
-  </si>
-  <si>
-    <t>HSR weak scaling</t>
-  </si>
-  <si>
-    <t>A8 strong scaling</t>
-  </si>
-  <si>
-    <t>Number of Cores</t>
-  </si>
-  <si>
-    <t>pipe1</t>
-  </si>
-  <si>
-    <t>A8 weak scaling</t>
-  </si>
-  <si>
-    <t>Compressor</t>
-  </si>
-  <si>
-    <t># Cores Azure</t>
-  </si>
-  <si>
-    <t>time azure</t>
-  </si>
-  <si>
-    <t>#cores hsr</t>
-  </si>
-  <si>
-    <t>time hsr</t>
+    <t>efficiency</t>
   </si>
   <si>
     <t>4--8</t>
@@ -262,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
@@ -271,8 +232,9 @@
     <numFmt numFmtId="169" formatCode="0%"/>
     <numFmt numFmtId="170" formatCode="#,##0.00"/>
     <numFmt numFmtId="171" formatCode="#,##0"/>
-    <numFmt numFmtId="172" formatCode="DD/MMM"/>
-    <numFmt numFmtId="173" formatCode="0.000E+00"/>
+    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="DD/MMM"/>
+    <numFmt numFmtId="174" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -544,7 +506,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -793,10 +755,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -825,11 +783,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -841,8 +839,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -907,7 +905,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1384,11 +1382,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="17143007"/>
-        <c:axId val="55651006"/>
+        <c:axId val="68264779"/>
+        <c:axId val="4261810"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17143007"/>
+        <c:axId val="68264779"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,14 +1403,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55651006"/>
+        <c:crossAx val="4261810"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55651006"/>
+        <c:axId val="4261810"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,7 +1434,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17143007"/>
+        <c:crossAx val="68264779"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1472,7 +1470,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1529,7 +1527,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1606,7 +1604,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1683,7 +1681,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1760,7 +1758,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1812,11 +1810,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="40665684"/>
-        <c:axId val="47776183"/>
+        <c:axId val="46034576"/>
+        <c:axId val="86418581"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40665684"/>
+        <c:axId val="46034576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,14 +1831,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47776183"/>
+        <c:crossAx val="86418581"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47776183"/>
+        <c:axId val="86418581"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,7 +1862,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40665684"/>
+        <c:crossAx val="46034576"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1900,7 +1898,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1957,7 +1955,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2049,7 +2047,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2141,7 +2139,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2230,7 +2228,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2297,11 +2295,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="30762545"/>
-        <c:axId val="64864633"/>
+        <c:axId val="9917027"/>
+        <c:axId val="80913052"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30762545"/>
+        <c:axId val="9917027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2318,14 +2316,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64864633"/>
+        <c:crossAx val="80913052"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64864633"/>
+        <c:axId val="80913052"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2349,7 +2347,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30762545"/>
+        <c:crossAx val="9917027"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2385,7 +2383,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2797,11 +2795,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="49270187"/>
-        <c:axId val="42220605"/>
+        <c:axId val="10614092"/>
+        <c:axId val="6034123"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49270187"/>
+        <c:axId val="10614092"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2818,14 +2816,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="42220605"/>
+        <c:crossAx val="6034123"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42220605"/>
+        <c:axId val="6034123"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2849,7 +2847,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49270187"/>
+        <c:crossAx val="10614092"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2885,7 +2883,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3072,11 +3070,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="18114264"/>
-        <c:axId val="90834659"/>
+        <c:axId val="4563511"/>
+        <c:axId val="52346475"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18114264"/>
+        <c:axId val="4563511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,14 +3091,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="90834659"/>
+        <c:crossAx val="52346475"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90834659"/>
+        <c:axId val="52346475"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3124,7 +3122,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18114264"/>
+        <c:crossAx val="4563511"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3155,15 +3153,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>840960</xdr:colOff>
+      <xdr:colOff>867960</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>457920</xdr:colOff>
+      <xdr:colOff>484560</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3171,8 +3169,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1513800" y="9311400"/>
-        <a:ext cx="5888880" cy="2741040"/>
+        <a:off x="1540800" y="9302400"/>
+        <a:ext cx="5888520" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3185,15 +3183,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>627120</xdr:colOff>
+      <xdr:colOff>654120</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>255600</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3201,8 +3199,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8918280" y="7826040"/>
-        <a:ext cx="3818880" cy="2739960"/>
+        <a:off x="8945280" y="7817040"/>
+        <a:ext cx="3818520" cy="2739600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3220,15 +3218,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>145800</xdr:colOff>
+      <xdr:colOff>172800</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>616320</xdr:colOff>
+      <xdr:colOff>642960</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3236,8 +3234,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5917680" y="11543400"/>
-        <a:ext cx="5222160" cy="2741400"/>
+        <a:off x="5944680" y="11534400"/>
+        <a:ext cx="5221800" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3250,15 +3248,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>132480</xdr:colOff>
+      <xdr:colOff>159480</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:colOff>300960</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3266,8 +3264,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="805320" y="9326520"/>
-        <a:ext cx="4568040" cy="2741400"/>
+        <a:off x="832320" y="9317520"/>
+        <a:ext cx="4567680" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3280,15 +3278,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>627120</xdr:colOff>
+      <xdr:colOff>654120</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>35280</xdr:colOff>
+      <xdr:colOff>61920</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3296,8 +3294,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11994120" y="9905760"/>
-        <a:ext cx="4601160" cy="2741040"/>
+        <a:off x="12021120" y="9896760"/>
+        <a:ext cx="4600800" cy="2740680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3318,7 +3316,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5415,8 +5413,8 @@
   </sheetPr>
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7004,7 +7002,7 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3"/>
       <c r="C30" s="6" t="n">
-        <f aca="false">$M$54/D30/E30</f>
+        <f aca="false">$M$54/E30</f>
         <v>4010210</v>
       </c>
       <c r="D30" s="0" t="n">
@@ -7054,7 +7052,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="6" t="n">
-        <f aca="false">$M$54/D31/E31</f>
+        <f aca="false">$M$54/E31</f>
         <v>501276.25</v>
       </c>
       <c r="D31" s="0" t="n">
@@ -7132,8 +7130,8 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="6" t="n">
-        <f aca="false">$M$54/D32/E32</f>
-        <v>125319.0625</v>
+        <f aca="false">$M$54/E32</f>
+        <v>250638.125</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>2</v>
@@ -7162,11 +7160,11 @@
       </c>
       <c r="K32" s="6" t="n">
         <f aca="false">C32/$C$30*$H$30/H32</f>
-        <v>0.49510179008673</v>
+        <v>0.990203580173459</v>
       </c>
       <c r="L32" s="6" t="n">
         <f aca="false">K32/E32</f>
-        <v>0.0309438618804206</v>
+        <v>0.0618877237608412</v>
       </c>
       <c r="O32" s="6" t="n">
         <f aca="false">$M$55/Q32</f>
@@ -7209,8 +7207,8 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="6" t="n">
-        <f aca="false">$M$54/D33/E33</f>
-        <v>31329.765625</v>
+        <f aca="false">$M$54/E33</f>
+        <v>125319.0625</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>4</v>
@@ -7239,11 +7237,11 @@
       </c>
       <c r="K33" s="6" t="n">
         <f aca="false">C33/$C$30*$H$30/H33</f>
-        <v>0.254591052197427</v>
+        <v>1.01836420878971</v>
       </c>
       <c r="L33" s="6" t="n">
         <f aca="false">K33/E33</f>
-        <v>0.0079559703811696</v>
+        <v>0.0318238815246784</v>
       </c>
       <c r="O33" s="6" t="n">
         <f aca="false">$M$55/Q33</f>
@@ -7286,8 +7284,8 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="6" t="n">
-        <f aca="false">$M$54/D34/E34</f>
-        <v>7832.44140625</v>
+        <f aca="false">$M$54/E34</f>
+        <v>62659.53125</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>8</v>
@@ -7316,11 +7314,11 @@
       </c>
       <c r="K34" s="6" t="n">
         <f aca="false">C34/$C$30*$H$30/H34</f>
-        <v>0.111161735910731</v>
+        <v>0.88929388728585</v>
       </c>
       <c r="L34" s="6" t="n">
         <f aca="false">K34/E34</f>
-        <v>0.00173690212360518</v>
+        <v>0.0138952169888414</v>
       </c>
       <c r="O34" s="6" t="n">
         <f aca="false">$M$55/Q34</f>
@@ -7363,8 +7361,8 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="6" t="n">
-        <f aca="false">$M$54/D35/E35</f>
-        <v>1958.1103515625</v>
+        <f aca="false">$M$54/E35</f>
+        <v>31329.765625</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>16</v>
@@ -7393,11 +7391,11 @@
       </c>
       <c r="K35" s="6" t="n">
         <f aca="false">C35/$C$30*$H$30/H35</f>
-        <v>0.0432842031572099</v>
+        <v>0.692547250515358</v>
       </c>
       <c r="L35" s="6" t="n">
         <f aca="false">K35/E35</f>
-        <v>0.000338157837165702</v>
+        <v>0.00541052539465124</v>
       </c>
       <c r="O35" s="6" t="n">
         <f aca="false">$M$55/Q35</f>
@@ -7441,8 +7439,8 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3"/>
       <c r="C36" s="6" t="n">
-        <f aca="false">$M$54/D36/E36</f>
-        <v>489.527587890625</v>
+        <f aca="false">$M$54/E36</f>
+        <v>15664.8828125</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>32</v>
@@ -7471,11 +7469,11 @@
       </c>
       <c r="K36" s="6" t="n">
         <f aca="false">C36/$C$30*$H$30/H36</f>
-        <v>0.0124100216985846</v>
+        <v>0.397120694354708</v>
       </c>
       <c r="L36" s="6" t="n">
         <f aca="false">K36/E36</f>
-        <v>4.84766472600962E-005</v>
+        <v>0.00155125271232308</v>
       </c>
       <c r="O36" s="6" t="n">
         <f aca="false">$M$55/Q36</f>
@@ -7519,8 +7517,8 @@
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="51"/>
       <c r="C37" s="6" t="n">
-        <f aca="false">$M$54/D37/E37</f>
-        <v>122.381896972656</v>
+        <f aca="false">$M$54/E37</f>
+        <v>7832.44140625</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>64</v>
@@ -7636,14 +7634,14 @@
       <c r="C42" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62" t="n">
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="n">
         <v>551.6</v>
       </c>
-      <c r="F42" s="62" t="n">
+      <c r="F42" s="6" t="n">
         <v>1703</v>
       </c>
-      <c r="G42" s="62" t="n">
+      <c r="G42" s="6" t="n">
         <v>2479</v>
       </c>
       <c r="H42" s="6" t="n">
@@ -7769,7 +7767,7 @@
         <f aca="false">H22</f>
         <v>441</v>
       </c>
-      <c r="E46" s="63" t="n">
+      <c r="E46" s="62" t="n">
         <f aca="false">T21</f>
         <v>594.84</v>
       </c>
@@ -7899,11 +7897,11 @@
       <c r="M50" s="6" t="n">
         <v>195102</v>
       </c>
-      <c r="N50" s="64" t="n">
+      <c r="N50" s="63" t="n">
         <f aca="false">$M$50/N$49</f>
         <v>24387.75</v>
       </c>
-      <c r="O50" s="65" t="n">
+      <c r="O50" s="64" t="n">
         <f aca="false">$M$50/O$49</f>
         <v>12193.875</v>
       </c>
@@ -7939,11 +7937,11 @@
         <f aca="false">$M$51/N$49</f>
         <v>54114.875</v>
       </c>
-      <c r="O51" s="64" t="n">
+      <c r="O51" s="63" t="n">
         <f aca="false">$M$51/O$49</f>
         <v>27057.4375</v>
       </c>
-      <c r="P51" s="65" t="n">
+      <c r="P51" s="64" t="n">
         <f aca="false">$M$51/P$49</f>
         <v>13528.71875</v>
       </c>
@@ -7963,7 +7961,7 @@
         <f aca="false">$M$51/T$49</f>
         <v>845.544921875</v>
       </c>
-      <c r="V51" s="66" t="n">
+      <c r="V51" s="65" t="n">
         <v>54114.875</v>
       </c>
       <c r="W51" s="6" t="n">
@@ -7982,7 +7980,7 @@
       <c r="M52" s="6" t="n">
         <v>1017573</v>
       </c>
-      <c r="N52" s="67" t="n">
+      <c r="N52" s="66" t="n">
         <f aca="false">$M$52/N$49</f>
         <v>127196.625</v>
       </c>
@@ -7990,11 +7988,11 @@
         <f aca="false">$M$52/O$49</f>
         <v>63598.3125</v>
       </c>
-      <c r="P52" s="64" t="n">
+      <c r="P52" s="63" t="n">
         <f aca="false">$M$52/P$49</f>
         <v>31799.15625</v>
       </c>
-      <c r="Q52" s="65" t="n">
+      <c r="Q52" s="64" t="n">
         <f aca="false">$M$52/Q$49</f>
         <v>15899.578125</v>
       </c>
@@ -8022,7 +8020,7 @@
         <f aca="false">$M$53/N$49</f>
         <v>254713.75</v>
       </c>
-      <c r="O53" s="67" t="n">
+      <c r="O53" s="66" t="n">
         <f aca="false">$M$53/O$49</f>
         <v>127356.875</v>
       </c>
@@ -8030,11 +8028,11 @@
         <f aca="false">$M$53/P$49</f>
         <v>63678.4375</v>
       </c>
-      <c r="Q53" s="64" t="n">
+      <c r="Q53" s="63" t="n">
         <f aca="false">$M$53/Q$49</f>
         <v>31839.21875</v>
       </c>
-      <c r="R53" s="65" t="n">
+      <c r="R53" s="64" t="n">
         <f aca="false">$M$53/R$49</f>
         <v>15919.609375</v>
       </c>
@@ -8062,7 +8060,7 @@
         <f aca="false">$M$54/O$49</f>
         <v>250638.125</v>
       </c>
-      <c r="P54" s="67" t="n">
+      <c r="P54" s="66" t="n">
         <f aca="false">$M$54/P$49</f>
         <v>125319.0625</v>
       </c>
@@ -8070,15 +8068,15 @@
         <f aca="false">$M$54/Q$49</f>
         <v>62659.53125</v>
       </c>
-      <c r="R54" s="64" t="n">
+      <c r="R54" s="63" t="n">
         <f aca="false">$M$54/R$49</f>
         <v>31329.765625</v>
       </c>
-      <c r="S54" s="65" t="n">
+      <c r="S54" s="64" t="n">
         <f aca="false">$M$54/S$49</f>
         <v>15664.8828125</v>
       </c>
-      <c r="T54" s="68" t="n">
+      <c r="T54" s="67" t="n">
         <f aca="false">$M$54/T$49</f>
         <v>7832.44140625</v>
       </c>
@@ -8090,19 +8088,19 @@
       <c r="M55" s="31" t="n">
         <v>8101299</v>
       </c>
-      <c r="N55" s="69" t="n">
+      <c r="N55" s="68" t="n">
         <f aca="false">$M$55/N$49</f>
         <v>1012662.375</v>
       </c>
-      <c r="O55" s="69" t="n">
+      <c r="O55" s="68" t="n">
         <f aca="false">$M$55/O$49</f>
         <v>506331.1875</v>
       </c>
-      <c r="P55" s="69" t="n">
+      <c r="P55" s="68" t="n">
         <f aca="false">$M$55/P$49</f>
         <v>253165.59375</v>
       </c>
-      <c r="Q55" s="67" t="n">
+      <c r="Q55" s="66" t="n">
         <f aca="false">$M$55/Q$49</f>
         <v>126582.796875</v>
       </c>
@@ -8110,11 +8108,11 @@
         <f aca="false">$M$55/R$49</f>
         <v>63291.3984375</v>
       </c>
-      <c r="S55" s="64" t="n">
+      <c r="S55" s="63" t="n">
         <f aca="false">$M$55/S$49</f>
         <v>31645.69921875</v>
       </c>
-      <c r="T55" s="65" t="n">
+      <c r="T55" s="64" t="n">
         <f aca="false">$M$55/T$49</f>
         <v>15822.849609375</v>
       </c>
@@ -8126,23 +8124,23 @@
       <c r="M56" s="31" t="n">
         <v>15522778</v>
       </c>
-      <c r="N56" s="69" t="n">
+      <c r="N56" s="68" t="n">
         <f aca="false">$M$56/N$49</f>
         <v>1940347.25</v>
       </c>
-      <c r="O56" s="69" t="n">
+      <c r="O56" s="68" t="n">
         <f aca="false">$M$56/O$49</f>
         <v>970173.625</v>
       </c>
-      <c r="P56" s="69" t="n">
+      <c r="P56" s="68" t="n">
         <f aca="false">$M$56/P$49</f>
         <v>485086.8125</v>
       </c>
-      <c r="Q56" s="69" t="n">
+      <c r="Q56" s="68" t="n">
         <f aca="false">$M$56/Q$49</f>
         <v>242543.40625</v>
       </c>
-      <c r="R56" s="67" t="n">
+      <c r="R56" s="66" t="n">
         <f aca="false">$M$56/R$49</f>
         <v>121271.703125</v>
       </c>
@@ -8150,7 +8148,7 @@
         <f aca="false">$M$56/S$49</f>
         <v>60635.8515625</v>
       </c>
-      <c r="T56" s="64" t="n">
+      <c r="T56" s="63" t="n">
         <f aca="false">$M$56/T$49</f>
         <v>30317.92578125</v>
       </c>
@@ -8617,472 +8615,647 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="69" width="12.9116279069767"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="69" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B3" s="70" t="n">
+        <v>37192.35</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="E3" s="70" t="n">
+        <v>79510.9416666667</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="70" t="n">
+        <v>167760.819444445</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="71" t="n">
+        <v>334873.233333333</v>
+      </c>
+      <c r="L3" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="72" t="n">
+        <v>664656.833333333</v>
+      </c>
+      <c r="O3" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="69" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="74"/>
+      <c r="D4" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="74" t="n">
+        <v>982.8</v>
+      </c>
+      <c r="F4" s="69" t="n">
+        <f aca="false">E$3*$A4/E$3*$E$4/$E4</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="69" t="n">
+        <f aca="false">F4/A4</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="74" t="n">
+        <v>2844</v>
+      </c>
+      <c r="I4" s="69" t="n">
+        <f aca="false">H$3*$A4/H$3*$H$4/$H4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="69" t="n">
+        <f aca="false">I4/A4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="72" t="n">
+        <v>4862</v>
+      </c>
+      <c r="L4" s="69" t="n">
+        <f aca="false">K$3*$A4/K$3*$K$4/$K4</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="69" t="n">
+        <f aca="false">L4/A4</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="69" t="n">
+        <v>11730</v>
+      </c>
+      <c r="O4" s="69" t="n">
+        <f aca="false">N$3*$A4/N$3*$N$4/$N4</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="69" t="n">
+        <f aca="false">O4/A4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="69" t="n">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B5" s="69" t="n">
         <v>894.62</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="E5" s="69" t="n">
         <v>1864.79</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">'HSR Cluster'!F15</f>
+      <c r="F5" s="69" t="n">
+        <f aca="false">E$3*$A5/E$3*$E$4/$E5</f>
+        <v>3.16217911936465</v>
+      </c>
+      <c r="G5" s="69" t="n">
+        <f aca="false">F5/A5</f>
+        <v>0.527029853227441</v>
+      </c>
+      <c r="H5" s="69" t="n">
         <v>4546.72</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">'HSR Cluster'!O15</f>
+      <c r="I5" s="69" t="n">
+        <f aca="false">H$3*$A5/H$3*$H$4/$H5</f>
+        <v>3.75303515501284</v>
+      </c>
+      <c r="J5" s="69" t="n">
+        <f aca="false">I5/A5</f>
+        <v>0.625505859168807</v>
+      </c>
+      <c r="K5" s="69" t="n">
         <v>7779.585</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <f aca="false">'HSR Cluster'!F24</f>
+      <c r="L5" s="69" t="n">
+        <f aca="false">K$3*$A5/K$3*$K$4/$K5</f>
+        <v>3.74981441812128</v>
+      </c>
+      <c r="M5" s="69" t="n">
+        <f aca="false">L5/A5</f>
+        <v>0.624969069686879</v>
+      </c>
+      <c r="N5" s="69" t="n">
         <v>17722.85</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="O5" s="69" t="n">
+        <f aca="false">N$3*$A5/N$3*$N$4/$N5</f>
+        <v>3.97114459581839</v>
+      </c>
+      <c r="P5" s="69" t="n">
+        <f aca="false">O5/A5</f>
+        <v>0.661857432636399</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="69" t="n">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>486.45</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B6" s="69" t="n">
         <v>743.86</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E6" s="69" t="n">
         <v>2365.75</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F6" s="69" t="n">
+        <f aca="false">E$3*$A6/E$3*$E$4/$E6</f>
+        <v>4.98514213251612</v>
+      </c>
+      <c r="G6" s="69" t="n">
+        <f aca="false">F6/A6</f>
+        <v>0.41542851104301</v>
+      </c>
+      <c r="H6" s="69" t="n">
         <v>4072.02</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="I6" s="69" t="n">
+        <f aca="false">H$3*$A6/H$3*$H$4/$H6</f>
+        <v>8.38109832466442</v>
+      </c>
+      <c r="J6" s="69" t="n">
+        <f aca="false">I6/A6</f>
+        <v>0.698424860388701</v>
+      </c>
+      <c r="K6" s="69" t="n">
         <v>5985.82</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="L6" s="69" t="n">
+        <f aca="false">K$3*$A6/K$3*$K$4/$K6</f>
+        <v>9.74703549388388</v>
+      </c>
+      <c r="M6" s="69" t="n">
+        <f aca="false">L6/A6</f>
+        <v>0.812252957823657</v>
+      </c>
+      <c r="N6" s="75" t="n">
+        <v>18709.49</v>
+      </c>
+      <c r="O6" s="69" t="n">
+        <f aca="false">N$3*$A6/N$3*$N$4/$N6</f>
+        <v>7.52345467460631</v>
+      </c>
+      <c r="P6" s="69" t="n">
+        <f aca="false">O6/A6</f>
+        <v>0.626954556217192</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="69" t="n">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>274.65</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>524.37</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="B7" s="69" t="n">
         <v>1223.82</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E7" s="69" t="n">
         <v>2008.19</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F7" s="69" t="n">
+        <f aca="false">E$3*$A7/E$3*$E$4/$E7</f>
+        <v>11.7455021686195</v>
+      </c>
+      <c r="G7" s="69" t="n">
+        <f aca="false">F7/A7</f>
+        <v>0.489395923692479</v>
+      </c>
+      <c r="H7" s="69" t="n">
         <v>4403.74</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>219.74</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>376.78</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>835.63</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>1404.86</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>2937.19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="I7" s="69" t="n">
+        <f aca="false">H$3*$A7/H$3*$H$4/$H7</f>
+        <v>15.4995526529722</v>
+      </c>
+      <c r="J7" s="69" t="n">
+        <f aca="false">I7/A7</f>
+        <v>0.645814693873844</v>
+      </c>
+      <c r="K7" s="69" t="n">
+        <v>9025.94</v>
+      </c>
+      <c r="L7" s="69" t="n">
+        <f aca="false">K$3*$A7/K$3*$K$4/$K7</f>
+        <v>12.928071757623</v>
+      </c>
+      <c r="M7" s="69" t="n">
+        <f aca="false">L7/A7</f>
+        <v>0.538669656567626</v>
+      </c>
+      <c r="N7" s="69" t="n">
+        <v>16434.67</v>
+      </c>
+      <c r="O7" s="69" t="n">
+        <f aca="false">N$3*$A7/N$3*$N$4/$N7</f>
+        <v>17.1296411792874</v>
+      </c>
+      <c r="P7" s="69" t="n">
+        <f aca="false">O7/A7</f>
+        <v>0.713735049136977</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="69" t="n">
         <v>48</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>188.05</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>336.3</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>657.32</v>
-      </c>
-      <c r="E7" s="0" t="n">
+      <c r="B8" s="69" t="n">
         <v>1096.61</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="E8" s="69" t="n">
         <v>2239.57</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">MAX(B3:F8)</f>
-        <v>17722.85</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>171.94</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>264.225</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>597.59</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>915.85</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1778.97</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>63</v>
+      <c r="F8" s="69" t="n">
+        <f aca="false">E$3*$A8/E$3*$E$4/$E8</f>
+        <v>21.0640435440732</v>
+      </c>
+      <c r="G8" s="69" t="n">
+        <f aca="false">F8/A8</f>
+        <v>0.438834240501525</v>
+      </c>
+      <c r="H8" s="69" t="n">
+        <v>4455.05</v>
+      </c>
+      <c r="I8" s="69" t="n">
+        <f aca="false">H$3*$A8/H$3*$H$4/$H8</f>
+        <v>30.6420803357987</v>
+      </c>
+      <c r="J8" s="69" t="n">
+        <f aca="false">I8/A8</f>
+        <v>0.638376673662473</v>
+      </c>
+      <c r="K8" s="69" t="n">
+        <v>7971.36</v>
+      </c>
+      <c r="L8" s="69" t="n">
+        <f aca="false">K$3*$A8/K$3*$K$4/$K8</f>
+        <v>29.2768109833203</v>
+      </c>
+      <c r="M8" s="69" t="n">
+        <f aca="false">L8/A8</f>
+        <v>0.609933562152506</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
-        <v>38361.1875</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>81350.3854166667</v>
+      <c r="A12" s="69" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>894.62</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>1864.79</v>
+      <c r="B13" s="69" t="n">
+        <v>14838.2522786458</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="76" t="n">
+        <v>29768.1361607143</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="77" t="n">
+        <v>61329.734375</v>
+      </c>
+      <c r="I13" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="78" t="n">
+        <v>125545.4125</v>
+      </c>
+      <c r="L13" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="69" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>743.86</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>2365.75</v>
+      <c r="A14" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="69" t="n">
+        <v>551.6</v>
+      </c>
+      <c r="F14" s="69" t="n">
+        <f aca="false">E$13*$A14/E$13*$E$14/$E14</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="69" t="n">
+        <f aca="false">F14/A14</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="69" t="n">
+        <v>1703</v>
+      </c>
+      <c r="I14" s="69" t="n">
+        <f aca="false">H$13*$A14/H$13*$H$14/$H14</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="69" t="n">
+        <f aca="false">I14/A14</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="69" t="n">
+        <v>2479</v>
+      </c>
+      <c r="L14" s="69" t="n">
+        <f aca="false">K$13*$A14/K$13*$K$14/$K14</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="69" t="n">
+        <f aca="false">L14/A14</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>1223.82</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>2008.19</v>
+      <c r="A15" s="69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" s="69" t="n">
+        <v>12.62</v>
+      </c>
+      <c r="F15" s="69" t="n">
+        <f aca="false">E$13*$A15/E$13*$E$14/$E15</f>
+        <v>349.667194928685</v>
+      </c>
+      <c r="G15" s="69" t="n">
+        <f aca="false">F15/A15</f>
+        <v>43.7083993660856</v>
+      </c>
+      <c r="H15" s="69" t="n">
+        <v>986.61</v>
+      </c>
+      <c r="I15" s="69" t="n">
+        <f aca="false">H$13*$A15/H$13*$H$14/$H15</f>
+        <v>13.8089011868925</v>
+      </c>
+      <c r="J15" s="69" t="n">
+        <f aca="false">I15/A15</f>
+        <v>1.72611264836156</v>
+      </c>
+      <c r="K15" s="69" t="n">
+        <v>2478.35</v>
+      </c>
+      <c r="L15" s="69" t="n">
+        <f aca="false">K$13*$A15/K$13*$K$14/$K15</f>
+        <v>8.00209817015353</v>
+      </c>
+      <c r="M15" s="69" t="n">
+        <f aca="false">L15/A15</f>
+        <v>1.00026227126919</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>1096.61</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2239.57</v>
+      <c r="A16" s="69" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="69" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="E16" s="69" t="n">
+        <v>518.119</v>
+      </c>
+      <c r="F16" s="69" t="n">
+        <f aca="false">E$13*$A16/E$13*$E$14/$E16</f>
+        <v>17.0339246389343</v>
+      </c>
+      <c r="G16" s="69" t="n">
+        <f aca="false">F16/A16</f>
+        <v>1.06462028993339</v>
+      </c>
+      <c r="H16" s="69" t="n">
+        <v>1264.05</v>
+      </c>
+      <c r="I16" s="69" t="n">
+        <f aca="false">H$13*$A16/H$13*$H$14/$H16</f>
+        <v>21.5561093311182</v>
+      </c>
+      <c r="J16" s="69" t="n">
+        <f aca="false">I16/A16</f>
+        <v>1.34725683319489</v>
+      </c>
+      <c r="K16" s="69" t="n">
+        <v>1908.35</v>
+      </c>
+      <c r="L16" s="69" t="n">
+        <f aca="false">K$13*$A16/K$13*$K$14/$K16</f>
+        <v>20.7844472974035</v>
+      </c>
+      <c r="M16" s="69" t="n">
+        <f aca="false">L16/A16</f>
+        <v>1.29902795608772</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="69" t="n">
+        <v>32</v>
+      </c>
+      <c r="B17" s="69" t="n">
+        <v>307.15</v>
+      </c>
+      <c r="E17" s="69" t="n">
+        <v>677.45</v>
+      </c>
+      <c r="F17" s="69" t="n">
+        <f aca="false">E$13*$A17/E$13*$E$14/$E17</f>
+        <v>26.0553546387187</v>
+      </c>
+      <c r="G17" s="69" t="n">
+        <f aca="false">F17/A17</f>
+        <v>0.81422983245996</v>
+      </c>
+      <c r="H17" s="69" t="n">
+        <v>990.21</v>
+      </c>
+      <c r="I17" s="69" t="n">
+        <f aca="false">H$13*$A17/H$13*$H$14/$H17</f>
+        <v>55.0347905999737</v>
+      </c>
+      <c r="J17" s="69" t="n">
+        <f aca="false">I17/A17</f>
+        <v>1.71983720624918</v>
+      </c>
+      <c r="K17" s="69" t="n">
+        <v>2124.53</v>
+      </c>
+      <c r="L17" s="69" t="n">
+        <f aca="false">K$13*$A17/K$13*$K$14/$K17</f>
+        <v>37.3390820557959</v>
+      </c>
+      <c r="M17" s="69" t="n">
+        <f aca="false">L17/A17</f>
+        <v>1.16684631424362</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="69" t="n">
+        <v>64</v>
+      </c>
+      <c r="B18" s="69" t="n">
+        <v>441</v>
+      </c>
+      <c r="E18" s="69" t="n">
+        <v>594.84</v>
+      </c>
+      <c r="F18" s="69" t="n">
+        <f aca="false">E$13*$A18/E$13*$E$14/$E18</f>
+        <v>59.3477237576491</v>
+      </c>
+      <c r="G18" s="69" t="n">
+        <f aca="false">F18/A18</f>
+        <v>0.927308183713267</v>
+      </c>
+      <c r="H18" s="69" t="n">
+        <v>1216.44</v>
+      </c>
+      <c r="I18" s="69" t="n">
+        <f aca="false">H$13*$A18/H$13*$H$14/$H18</f>
+        <v>89.5991581993358</v>
+      </c>
+      <c r="J18" s="69" t="n">
+        <f aca="false">I18/A18</f>
+        <v>1.39998684686462</v>
+      </c>
+      <c r="K18" s="69" t="n">
+        <v>2237.18</v>
+      </c>
+      <c r="L18" s="69" t="n">
+        <f aca="false">K$13*$A18/K$13*$K$14/$K18</f>
+        <v>70.9178519386013</v>
+      </c>
+      <c r="M18" s="69" t="n">
+        <f aca="false">L18/A18</f>
+        <v>1.10809143654065</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>64</v>
+      <c r="A19" s="69" t="n">
+        <v>128</v>
+      </c>
+      <c r="B19" s="69" t="n">
+        <v>499.97</v>
+      </c>
+      <c r="E19" s="69" t="n">
+        <v>781.01</v>
+      </c>
+      <c r="F19" s="69" t="n">
+        <f aca="false">E$13*$A19/E$13*$E$14/$E19</f>
+        <v>90.4019154684319</v>
+      </c>
+      <c r="G19" s="69" t="n">
+        <f aca="false">F19/A19</f>
+        <v>0.706264964597124</v>
+      </c>
+      <c r="H19" s="69" t="n">
+        <v>1246.78</v>
+      </c>
+      <c r="I19" s="69" t="n">
+        <f aca="false">H$13*$A19/H$13*$H$14/$H19</f>
+        <v>174.837581610228</v>
+      </c>
+      <c r="J19" s="69" t="n">
+        <f aca="false">I19/A19</f>
+        <v>1.36591860632991</v>
+      </c>
+      <c r="K19" s="69" t="n">
+        <v>2078.03</v>
+      </c>
+      <c r="L19" s="69" t="n">
+        <f aca="false">K$13*$A19/K$13*$K$14/$K19</f>
+        <v>152.698469223255</v>
+      </c>
+      <c r="M19" s="69" t="n">
+        <f aca="false">L19/A19</f>
+        <v>1.19295679080668</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>62</v>
+      <c r="A20" s="69" t="n">
+        <v>256</v>
+      </c>
+      <c r="B20" s="69" t="n">
+        <v>681.01</v>
+      </c>
+      <c r="E20" s="69" t="n">
+        <v>1108.038</v>
+      </c>
+      <c r="F20" s="69" t="n">
+        <f aca="false">E$13*$A20/E$13*$E$14/$E20</f>
+        <v>127.441116640404</v>
+      </c>
+      <c r="G20" s="69" t="n">
+        <f aca="false">F20/A20</f>
+        <v>0.497816861876578</v>
+      </c>
+      <c r="H20" s="69" t="n">
+        <v>1546.04</v>
+      </c>
+      <c r="I20" s="69" t="n">
+        <f aca="false">H$13*$A20/H$13*$H$14/$H20</f>
+        <v>281.990116685209</v>
+      </c>
+      <c r="J20" s="69" t="n">
+        <f aca="false">I20/A20</f>
+        <v>1.1015238933016</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>12.62</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>986.61</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>3973.31</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>2478.35</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>9184.44</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>10.47</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>518.119</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>1908.35</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>1264.05</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>4369.9</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>11.82</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>307.15</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>990.21</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>677.45</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>2124.53</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <f aca="false">MAX(B21:F24)</f>
-        <v>9184.44</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>15.96</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>252.13</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>594.84</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>441</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>1216.44</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="n">
-        <v>30506.39453125</v>
-      </c>
-      <c r="D30" s="6" t="n">
-        <v>61012.7890625</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>12.62</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>986.61</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>518.119</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>1264.05</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>677.45</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>990.21</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="C34" s="63" t="n">
-        <v>594.84</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>1216.44</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>11016.886</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>5351.41</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>5679.71</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>4472.31</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>2993.06</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>4587.58</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>1616.93</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>3487.35</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>3154.7</v>
+      <c r="A21" s="69" t="n">
+        <v>512</v>
+      </c>
+      <c r="B21" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="69" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9104,7 +9277,7 @@
   <dimension ref="B3:P33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9124,40 +9297,40 @@
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="70" t="s">
-        <v>73</v>
+      <c r="C3" s="79" t="s">
+        <v>60</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="C4" s="71" t="n">
+      <c r="C4" s="80" t="n">
         <v>144300</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">C4/60/60</f>
         <v>40.0833333333333</v>
       </c>
-      <c r="F4" s="71" t="n">
+      <c r="F4" s="80" t="n">
         <v>140400</v>
       </c>
       <c r="H4" s="3"/>
@@ -9166,14 +9339,14 @@
       <c r="B5" s="0" t="n">
         <v>199</v>
       </c>
-      <c r="C5" s="71" t="n">
+      <c r="C5" s="80" t="n">
         <v>143600</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">C4-C5</f>
         <v>700</v>
       </c>
-      <c r="F5" s="71" t="n">
+      <c r="F5" s="80" t="n">
         <v>139800</v>
       </c>
       <c r="H5" s="6" t="n">
@@ -9185,14 +9358,14 @@
       <c r="B6" s="0" t="n">
         <v>198</v>
       </c>
-      <c r="C6" s="71" t="n">
+      <c r="C6" s="80" t="n">
         <v>142900</v>
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">C5-C6</f>
         <v>700</v>
       </c>
-      <c r="F6" s="71" t="n">
+      <c r="F6" s="80" t="n">
         <v>139100</v>
       </c>
       <c r="H6" s="6" t="n">
@@ -9204,14 +9377,14 @@
       <c r="B7" s="0" t="n">
         <v>197</v>
       </c>
-      <c r="C7" s="71" t="n">
+      <c r="C7" s="80" t="n">
         <v>142200</v>
       </c>
       <c r="E7" s="6" t="n">
         <f aca="false">C6-C7</f>
         <v>700</v>
       </c>
-      <c r="F7" s="71" t="n">
+      <c r="F7" s="80" t="n">
         <v>138400</v>
       </c>
       <c r="H7" s="6" t="n">
@@ -9223,14 +9396,14 @@
       <c r="B8" s="0" t="n">
         <v>196</v>
       </c>
-      <c r="C8" s="71" t="n">
+      <c r="C8" s="80" t="n">
         <v>141600</v>
       </c>
       <c r="E8" s="6" t="n">
         <f aca="false">C7-C8</f>
         <v>600</v>
       </c>
-      <c r="F8" s="71" t="n">
+      <c r="F8" s="80" t="n">
         <v>137800</v>
       </c>
       <c r="H8" s="6" t="n">
@@ -9242,14 +9415,14 @@
       <c r="B9" s="0" t="n">
         <v>195</v>
       </c>
-      <c r="C9" s="71" t="n">
+      <c r="C9" s="80" t="n">
         <v>140900</v>
       </c>
       <c r="E9" s="6" t="n">
         <f aca="false">C8-C9</f>
         <v>700</v>
       </c>
-      <c r="F9" s="71" t="n">
+      <c r="F9" s="80" t="n">
         <v>137100</v>
       </c>
       <c r="H9" s="6" t="n">
@@ -9261,14 +9434,14 @@
       <c r="B10" s="0" t="n">
         <v>194</v>
       </c>
-      <c r="C10" s="71" t="n">
+      <c r="C10" s="80" t="n">
         <v>140200</v>
       </c>
       <c r="E10" s="6" t="n">
         <f aca="false">C9-C10</f>
         <v>700</v>
       </c>
-      <c r="F10" s="71" t="n">
+      <c r="F10" s="80" t="n">
         <v>136500</v>
       </c>
       <c r="H10" s="6" t="n">
@@ -9280,14 +9453,14 @@
       <c r="B11" s="0" t="n">
         <v>193</v>
       </c>
-      <c r="C11" s="71" t="n">
+      <c r="C11" s="80" t="n">
         <v>139500</v>
       </c>
       <c r="E11" s="6" t="n">
         <f aca="false">C10-C11</f>
         <v>700</v>
       </c>
-      <c r="F11" s="71" t="n">
+      <c r="F11" s="80" t="n">
         <v>135800</v>
       </c>
       <c r="H11" s="6" t="n">
@@ -9299,8 +9472,8 @@
       <c r="B12" s="0" t="n">
         <v>192</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="F12" s="71" t="n">
+      <c r="C12" s="80"/>
+      <c r="F12" s="80" t="n">
         <v>135200</v>
       </c>
       <c r="H12" s="6" t="n">
@@ -9312,8 +9485,8 @@
       <c r="B13" s="0" t="n">
         <v>191</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="F13" s="71" t="n">
+      <c r="C13" s="80"/>
+      <c r="F13" s="80" t="n">
         <v>134500</v>
       </c>
       <c r="H13" s="6" t="n">
@@ -9326,50 +9499,50 @@
         <f aca="false">B13-1</f>
         <v>190</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="F14" s="71"/>
+      <c r="C14" s="80"/>
+      <c r="F14" s="80"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="n">
         <f aca="false">B14-1</f>
         <v>189</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="F15" s="71"/>
+      <c r="C15" s="80"/>
+      <c r="F15" s="80"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="n">
         <f aca="false">B15-1</f>
         <v>188</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="F16" s="71"/>
+      <c r="C16" s="80"/>
+      <c r="F16" s="80"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="n">
         <f aca="false">B16-1</f>
         <v>187</v>
       </c>
-      <c r="C17" s="71"/>
+      <c r="C17" s="80"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="n">
         <f aca="false">B17-1</f>
         <v>186</v>
       </c>
-      <c r="C18" s="71"/>
+      <c r="C18" s="80"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="n">
         <f aca="false">B18-1</f>
         <v>185</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="K19" s="71" t="n">
+      <c r="C19" s="80"/>
+      <c r="K19" s="80" t="n">
         <v>104100</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9377,8 +9550,8 @@
         <f aca="false">B19-1</f>
         <v>184</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="K20" s="71" t="n">
+      <c r="C20" s="80"/>
+      <c r="K20" s="80" t="n">
         <v>103500</v>
       </c>
       <c r="M20" s="6" t="n">
@@ -9398,8 +9571,8 @@
         <f aca="false">B20-1</f>
         <v>183</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="K21" s="71" t="n">
+      <c r="C21" s="80"/>
+      <c r="K21" s="80" t="n">
         <v>103000</v>
       </c>
       <c r="M21" s="6" t="n">
@@ -9412,8 +9585,8 @@
         <f aca="false">B21-1</f>
         <v>182</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="K22" s="71" t="n">
+      <c r="C22" s="80"/>
+      <c r="K22" s="80" t="n">
         <v>102400</v>
       </c>
       <c r="M22" s="6" t="n">
@@ -9426,7 +9599,7 @@
         <f aca="false">B22-1</f>
         <v>181</v>
       </c>
-      <c r="K23" s="71" t="n">
+      <c r="K23" s="80" t="n">
         <v>101900</v>
       </c>
       <c r="M23" s="6" t="n">
@@ -9439,7 +9612,7 @@
         <f aca="false">B23-1</f>
         <v>180</v>
       </c>
-      <c r="K24" s="71" t="n">
+      <c r="K24" s="80" t="n">
         <v>101300</v>
       </c>
       <c r="M24" s="6" t="n">
@@ -9452,7 +9625,7 @@
         <f aca="false">B24-1</f>
         <v>179</v>
       </c>
-      <c r="K25" s="71" t="n">
+      <c r="K25" s="80" t="n">
         <v>100800</v>
       </c>
       <c r="M25" s="6" t="n">
@@ -9465,7 +9638,7 @@
         <f aca="false">B25-1</f>
         <v>178</v>
       </c>
-      <c r="K26" s="71" t="n">
+      <c r="K26" s="80" t="n">
         <v>100300</v>
       </c>
       <c r="M26" s="6" t="n">
@@ -9478,7 +9651,7 @@
         <f aca="false">B26-1</f>
         <v>177</v>
       </c>
-      <c r="K27" s="71" t="n">
+      <c r="K27" s="80" t="n">
         <v>99700</v>
       </c>
       <c r="M27" s="6" t="n">
@@ -9491,7 +9664,7 @@
         <f aca="false">B27-1</f>
         <v>176</v>
       </c>
-      <c r="K28" s="71" t="n">
+      <c r="K28" s="80" t="n">
         <v>99150</v>
       </c>
       <c r="M28" s="6" t="n">
@@ -9504,7 +9677,7 @@
         <f aca="false">B28-1</f>
         <v>175</v>
       </c>
-      <c r="K29" s="71" t="n">
+      <c r="K29" s="80" t="n">
         <v>98600</v>
       </c>
       <c r="M29" s="6" t="n">
@@ -9517,7 +9690,7 @@
         <f aca="false">B29-1</f>
         <v>174</v>
       </c>
-      <c r="K30" s="71" t="n">
+      <c r="K30" s="80" t="n">
         <v>98060</v>
       </c>
       <c r="M30" s="6" t="n">
@@ -9530,7 +9703,7 @@
         <f aca="false">B30-1</f>
         <v>173</v>
       </c>
-      <c r="K31" s="71" t="n">
+      <c r="K31" s="80" t="n">
         <v>97500</v>
       </c>
       <c r="M31" s="6" t="n">
@@ -9543,7 +9716,7 @@
         <f aca="false">B31-1</f>
         <v>172</v>
       </c>
-      <c r="K32" s="71" t="n">
+      <c r="K32" s="80" t="n">
         <v>96940</v>
       </c>
       <c r="M32" s="6" t="n">

</xml_diff>

<commit_message>
Added new Set up time data
</commit_message>
<xml_diff>
--- a/doc/results/ansys/resultsANSYS.xlsx
+++ b/doc/results/ansys/resultsANSYS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="104">
   <si>
     <t>pipe01</t>
   </si>
@@ -321,6 +321,18 @@
   <si>
     <t>efficiency</t>
   </si>
+  <si>
+    <t>HPC Pack, A4 nodes</t>
+  </si>
+  <si>
+    <t>Prepare Cloud Service</t>
+  </si>
+  <si>
+    <t>Create domain controller</t>
+  </si>
+  <si>
+    <t>Create nodes</t>
+  </si>
 </sst>
 </file>
 
@@ -365,16 +377,16 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -402,8 +414,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -653,16 +664,16 @@
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,7 +729,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -766,7 +777,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,7 +801,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -866,7 +877,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -882,7 +893,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1014,7 +1025,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1026,6 +1037,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1034,7 +1049,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1099,7 +1114,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1576,11 +1591,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="45548303"/>
-        <c:axId val="26006302"/>
+        <c:axId val="14930861"/>
+        <c:axId val="857383"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45548303"/>
+        <c:axId val="14930861"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,14 +1612,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26006302"/>
+        <c:crossAx val="857383"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26006302"/>
+        <c:axId val="857383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,7 +1643,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45548303"/>
+        <c:crossAx val="14930861"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1664,7 +1679,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2004,11 +2019,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="98848673"/>
-        <c:axId val="81667488"/>
+        <c:axId val="83313887"/>
+        <c:axId val="74190458"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98848673"/>
+        <c:axId val="83313887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2025,14 +2040,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="81667488"/>
+        <c:crossAx val="74190458"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81667488"/>
+        <c:axId val="74190458"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,7 +2071,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98848673"/>
+        <c:crossAx val="83313887"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2092,7 +2107,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2489,11 +2504,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88666022"/>
-        <c:axId val="81250686"/>
+        <c:axId val="76624398"/>
+        <c:axId val="11419551"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88666022"/>
+        <c:axId val="76624398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2510,14 +2525,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="81250686"/>
+        <c:crossAx val="11419551"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81250686"/>
+        <c:axId val="11419551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2541,7 +2556,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88666022"/>
+        <c:crossAx val="76624398"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2577,7 +2592,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2989,11 +3004,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51816969"/>
-        <c:axId val="99738590"/>
+        <c:axId val="81849345"/>
+        <c:axId val="25743620"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51816969"/>
+        <c:axId val="81849345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3010,14 +3025,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99738590"/>
+        <c:crossAx val="25743620"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99738590"/>
+        <c:axId val="25743620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3041,7 +3056,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51816969"/>
+        <c:crossAx val="81849345"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3077,7 +3092,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3264,11 +3279,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="49968600"/>
-        <c:axId val="75984951"/>
+        <c:axId val="48681758"/>
+        <c:axId val="73835492"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49968600"/>
+        <c:axId val="48681758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3285,14 +3300,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="75984951"/>
+        <c:crossAx val="73835492"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75984951"/>
+        <c:axId val="73835492"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3316,7 +3331,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49968600"/>
+        <c:crossAx val="48681758"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -3347,15 +3362,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>867960</xdr:colOff>
+      <xdr:colOff>894960</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>484560</xdr:colOff>
+      <xdr:colOff>511200</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3363,8 +3378,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1540800" y="9302400"/>
-        <a:ext cx="5893560" cy="2740680"/>
+        <a:off x="1567800" y="9293400"/>
+        <a:ext cx="5893200" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3376,16 +3391,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>654120</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>255600</xdr:colOff>
+      <xdr:colOff>282240</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3393,8 +3408,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8950320" y="7817040"/>
-        <a:ext cx="3818520" cy="2739600"/>
+        <a:off x="8977320" y="7808040"/>
+        <a:ext cx="3818160" cy="2739240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3412,15 +3427,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>173160</xdr:colOff>
+      <xdr:colOff>200160</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>643320</xdr:colOff>
+      <xdr:colOff>669960</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3428,8 +3443,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5945040" y="11534400"/>
-        <a:ext cx="5305680" cy="2741400"/>
+        <a:off x="5972040" y="11525400"/>
+        <a:ext cx="5305320" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3442,15 +3457,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>159840</xdr:colOff>
+      <xdr:colOff>186840</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
+      <xdr:colOff>327600</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3458,8 +3473,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="832680" y="9317520"/>
-        <a:ext cx="4567320" cy="2741400"/>
+        <a:off x="859680" y="9308520"/>
+        <a:ext cx="4566960" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3472,15 +3487,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>654120</xdr:colOff>
+      <xdr:colOff>681120</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>61920</xdr:colOff>
+      <xdr:colOff>88560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3488,8 +3503,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12105000" y="9897120"/>
-        <a:ext cx="4600800" cy="2740320"/>
+        <a:off x="12132000" y="9888120"/>
+        <a:ext cx="4600440" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3510,7 +3525,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="B59:D62 B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5607,7 +5622,7 @@
   <dimension ref="A1:AF63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="1" sqref="B59:D62 C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5639,6 +5654,10 @@
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+    </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="40" t="s">
         <v>0</v>
@@ -7045,17 +7064,23 @@
         <f aca="false">$T$6/T24</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V24" s="47" t="e">
+      <c r="V24" s="47" t="inlineStr">
         <f aca="false">U24/Q24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X24" s="48" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X24" s="48" t="inlineStr">
         <f aca="false">O24/$O$6*$T$6/T24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y24" s="49" t="e">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Y24" s="49" t="inlineStr">
         <f aca="false">X24/Q24</f>
-        <v>#DIV/0!</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="AA24" s="56" t="s">
         <v>40</v>
@@ -7721,10 +7746,14 @@
         <v>512</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="0"/>
+    </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="I39" s="0"/>
       <c r="L39" s="0" t="s">
         <v>19</v>
       </c>
@@ -7750,6 +7779,7 @@
         <v>41</v>
       </c>
       <c r="F40" s="6"/>
+      <c r="I40" s="0"/>
       <c r="M40" s="0" t="n">
         <v>1</v>
       </c>
@@ -8502,7 +8532,7 @@
   <dimension ref="B1:AA27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B59:D62 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9106,8 +9136,8 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D57" activeCellId="1" sqref="B59:D62 D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9591,7 +9621,7 @@
   <dimension ref="B3:P33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+      <selection pane="topLeft" activeCell="E54" activeCellId="1" sqref="B59:D62 E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10063,15 +10093,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5023255813953"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10463,21 +10496,560 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B21" s="92" t="n">
+        <f aca="false">D34+E34+K34</f>
+        <v>0.00106481481481481</v>
+      </c>
+      <c r="C21" s="92" t="n">
+        <f aca="false">F34+G34</f>
+        <v>0.0173611111111111</v>
+      </c>
+      <c r="D21" s="92" t="n">
+        <f aca="false">H34+I34+J34</f>
+        <v>0.0450694444444444</v>
+      </c>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B22" s="92" t="n">
+        <f aca="false">D35+E35+K35</f>
+        <v>0.00103009259259259</v>
+      </c>
+      <c r="C22" s="92" t="n">
+        <f aca="false">F35+G35</f>
+        <v>0.0141782407407407</v>
+      </c>
+      <c r="D22" s="92" t="n">
+        <f aca="false">H35+I35+J35</f>
+        <v>0.0741203703703703</v>
+      </c>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B23" s="92" t="n">
+        <f aca="false">D36+E36+K36</f>
+        <v>0.000914351851851851</v>
+      </c>
+      <c r="C23" s="92" t="n">
+        <f aca="false">F36+G36</f>
+        <v>0.0146180555555556</v>
+      </c>
+      <c r="D23" s="92" t="n">
+        <f aca="false">H36+I36+J36</f>
+        <v>0.106527777777778</v>
+      </c>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+    </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="82" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28" s="87" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="87"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="87"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="87"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="85"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="87"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="81" t="n">
+        <v>0.000185185185185185</v>
+      </c>
+      <c r="E34" s="81" t="n">
+        <v>0.000219907407407407</v>
+      </c>
+      <c r="F34" s="83" t="n">
+        <v>0.00694444444444444</v>
+      </c>
+      <c r="G34" s="83" t="n">
+        <v>0.0104166666666667</v>
+      </c>
+      <c r="H34" s="86" t="n">
+        <v>0.0381944444444444</v>
+      </c>
+      <c r="I34" s="86" t="n">
+        <v>0.00253472222222222</v>
+      </c>
+      <c r="J34" s="86" t="n">
+        <v>0.00434027777777778</v>
+      </c>
+      <c r="K34" s="88" t="n">
+        <v>0.000659722222222222</v>
+      </c>
+      <c r="L34" s="89" t="n">
+        <f aca="false">SUM(D34:K34)</f>
+        <v>0.0634953703703704</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="81" t="n">
+        <v>0.000185185185185185</v>
+      </c>
+      <c r="E35" s="81" t="n">
+        <v>0.000208333333333333</v>
+      </c>
+      <c r="F35" s="83" t="n">
+        <v>0.00584490740740741</v>
+      </c>
+      <c r="G35" s="84" t="n">
+        <v>0.00833333333333333</v>
+      </c>
+      <c r="H35" s="86" t="n">
+        <v>0.0680555555555555</v>
+      </c>
+      <c r="I35" s="86" t="n">
+        <v>0.00196759259259259</v>
+      </c>
+      <c r="J35" s="86" t="n">
+        <v>0.00409722222222222</v>
+      </c>
+      <c r="K35" s="88" t="n">
+        <v>0.000636574074074074</v>
+      </c>
+      <c r="L35" s="89" t="n">
+        <f aca="false">SUM(D35:K35)</f>
+        <v>0.0893287037037036</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="81" t="n">
+        <v>0.000185185185185185</v>
+      </c>
+      <c r="E36" s="81" t="n">
+        <v>0.000208333333333333</v>
+      </c>
+      <c r="F36" s="83" t="n">
+        <v>0.00559027777777778</v>
+      </c>
+      <c r="G36" s="83" t="n">
+        <v>0.00902777777777778</v>
+      </c>
+      <c r="H36" s="86" t="n">
+        <v>0.101388888888889</v>
+      </c>
+      <c r="I36" s="86" t="n">
+        <v>0.00144675925925926</v>
+      </c>
+      <c r="J36" s="86" t="n">
+        <v>0.00369212962962963</v>
+      </c>
+      <c r="K36" s="88" t="n">
+        <v>0.000520833333333333</v>
+      </c>
+      <c r="L36" s="89" t="n">
+        <f aca="false">SUM(D36:K36)</f>
+        <v>0.122060185185185</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="83"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="85"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="86"/>
+      <c r="L38" s="86"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="86"/>
+      <c r="L39" s="86"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="85"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="86"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="87"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="88"/>
+      <c r="L41" s="88"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J42" s="89"/>
+      <c r="K42" s="89"/>
+      <c r="L42" s="89"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>55.53</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>34.62</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <f aca="false">SUM(C49*60+D49,E49*60+F49)</f>
+        <v>510.15</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>54.59</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>38.21</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">SUM(C50*60+D50,E50*60+F50)</f>
+        <v>512.8</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>55.91</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <f aca="false">SUM(C51*60+D51,E51*60+F51)</f>
+        <v>517.71</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>20.15</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>43.94</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <f aca="false">SUM(C52*60+D52,E52*60+F52)</f>
+        <v>664.09</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>25.25</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>55.58</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <f aca="false">SUM(C53*60+D53,E53*60+F53)</f>
+        <v>800.83</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>34.75</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">SUM(C54*60+D54,E54*60+F54)</f>
+        <v>805.15</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>27.48</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>56.94</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">SUM(C55*60+D55,E55*60+F55)</f>
+        <v>804.42</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C60" s="92" t="n">
+        <f aca="false">(C52*60+D52)/(24*3600)</f>
+        <v>0.00162210648148148</v>
+      </c>
+      <c r="D60" s="92" t="n">
+        <f aca="false">(E52*60+F52)/(24*3600)</f>
+        <v>0.00606412037037037</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C61" s="92" t="n">
+        <f aca="false">(C53*60+D53)/(24*3600)</f>
+        <v>0.00168113425925926</v>
+      </c>
+      <c r="D61" s="92" t="n">
+        <f aca="false">(E53*60+F53)/(24*3600)</f>
+        <v>0.00758773148148148</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C62" s="92" t="n">
+        <f aca="false">(C54*60+D54)/(24*3600)</f>
+        <v>0.00179108796296296</v>
+      </c>
+      <c r="D62" s="92" t="n">
+        <f aca="false">(E54*60+F54)/(24*3600)</f>
+        <v>0.00752777777777778</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>